<commit_message>
[FEATURE] add Zusammenfassung Kapitel 5
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EC0892-6185-984F-8ACD-1CCA18184207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C664B00-D333-5547-A1A2-874056729918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Fertigzustellen bis</t>
   </si>
   <si>
-    <t>Dauer</t>
-  </si>
-  <si>
     <t>Projektplanung</t>
   </si>
   <si>
@@ -152,13 +149,43 @@
   </si>
   <si>
     <t>Domaenenanalyse</t>
+  </si>
+  <si>
+    <t>Kick-Off</t>
+  </si>
+  <si>
+    <t>[SEMINAR]</t>
+  </si>
+  <si>
+    <t>Zoom Call</t>
+  </si>
+  <si>
+    <t>Zusammenfassung</t>
+  </si>
+  <si>
+    <t>Everything that has already been set up but had to be done again</t>
+  </si>
+  <si>
+    <t>Everything new</t>
+  </si>
+  <si>
+    <t>Fixes something that was really wrong and breaked stuff</t>
+  </si>
+  <si>
+    <t>Everything done for the seminars</t>
+  </si>
+  <si>
+    <t>Stunden Seminar</t>
+  </si>
+  <si>
+    <t>Stunden Projekt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +197,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -325,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -364,6 +398,10 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I26" sqref="A1:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,14 +730,15 @@
     <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="19"/>
-    <col min="10" max="10" width="10.83203125" style="20"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="19"/>
+    <col min="11" max="11" width="10.83203125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,13 +746,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -722,34 +761,37 @@
         <v>4</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="14"/>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L1" s="14"/>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2">
         <v>44292</v>
@@ -757,28 +799,31 @@
       <c r="G2" s="2">
         <v>44298</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>6</v>
       </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2">
         <v>44295</v>
@@ -786,28 +831,31 @@
       <c r="G3" s="2">
         <v>44298</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="M3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2">
         <v>44296</v>
@@ -815,28 +863,31 @@
       <c r="G4" s="2">
         <v>44298</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2">
         <v>44296</v>
@@ -844,48 +895,55 @@
       <c r="G5" s="2">
         <v>44298</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N5" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2">
         <v>44298</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="13"/>
+      <c r="I6" s="13">
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="2">
         <v>44298</v>
@@ -893,25 +951,25 @@
       <c r="G7" s="2">
         <v>44317</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>10</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2">
         <v>44298</v>
@@ -919,26 +977,26 @@
       <c r="G8" s="2">
         <v>44338</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>1.5</v>
       </c>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2">
         <v>44298</v>
@@ -946,35 +1004,36 @@
       <c r="G9" s="2">
         <v>44317</v>
       </c>
-      <c r="H9" s="15">
-        <f>ROUNDUP(((SUM(J9-I9)*24*60/60)/0.25),0)*0.25</f>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15">
+        <f>ROUNDUP(((SUM(K9-J9)*24*60/60)/0.25),0)*0.25</f>
         <v>1</v>
       </c>
-      <c r="I9" s="21">
+      <c r="J9" s="21">
         <v>0.68402777777777779</v>
       </c>
-      <c r="J9" s="22">
+      <c r="K9" s="22">
         <v>0.72222222222222221</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="15"/>
-      <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L9" s="16"/>
+      <c r="M9" s="15"/>
+      <c r="P9" s="15"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2">
         <v>44298</v>
@@ -982,72 +1041,247 @@
       <c r="G10" s="2">
         <v>44317</v>
       </c>
-      <c r="H10" s="15">
-        <f>ROUNDUP(((SUM(J10-I10)*24*60/60)/0.25),0)*0.25</f>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
+        <f>ROUNDUP(((SUM(K10-J10)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="I10" s="21">
+      <c r="J10" s="21">
         <v>0.72916666666666663</v>
       </c>
-      <c r="J10" s="22">
+      <c r="K10" s="22">
         <v>0.73958333333333337</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="15"/>
-      <c r="O10" s="15"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L10" s="16"/>
+      <c r="M10" s="15"/>
+      <c r="P10" s="15"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G11" s="2">
+        <v>44299</v>
+      </c>
+      <c r="H11" s="15">
+        <f>ROUNDUP(((SUM(K11-J11)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K11" s="22">
+        <v>0.47361111111111115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G12" s="2">
+        <v>44299</v>
+      </c>
+      <c r="H12" s="15">
+        <f>ROUNDUP(((SUM(K12-J12)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="22">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I13" s="15">
+        <f t="shared" ref="H11:I25" si="0">ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I17" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I19" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I20" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
       <c r="F23" s="2"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26">
+      <c r="I23" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="24">
+        <f>SUM(I:I)+SUM(H:H)</f>
+        <v>18.5</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="24">
         <f>SUM(H:H)</f>
+        <v>3.75</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="24">
+        <f>SUM(I:I)</f>
         <v>14.75</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C6 C7:C25" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
-      <formula1>$M$2:$M$4</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C3:C10" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+      <formula1>$N$2:$N$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2 C11:C25" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+      <formula1>$N$2:$N$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1066,19 +1300,19 @@
   <sheetData>
     <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1099,7 +1333,7 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <f>SUM(E5:E7)</f>
@@ -1161,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8">
         <f>SUM(E8:E10)</f>
@@ -1223,7 +1457,7 @@
         <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G11">
         <f>SUM(E11:E13)</f>
@@ -1285,7 +1519,7 @@
         <v>37</v>
       </c>
       <c r="F14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14">
         <f>SUM(E14:E15)</f>
@@ -1329,7 +1563,7 @@
         <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16">
         <f>SUM(E16:E17)</f>

</xml_diff>

<commit_message>
[TASK] Systemanforderungen & Abhängigkeiten identifizieren
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C664B00-D333-5547-A1A2-874056729918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13454A0A-2744-BD4A-82FE-EB065A789697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Stunden Projekt</t>
+  </si>
+  <si>
+    <t>Zitate gepflegt</t>
+  </si>
+  <si>
+    <t>Weitere Nutzeranforderungen</t>
   </si>
 </sst>
 </file>
@@ -720,7 +726,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I26" sqref="A1:I26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -924,6 +930,9 @@
       <c r="F6" s="2">
         <v>44298</v>
       </c>
+      <c r="G6" s="2">
+        <v>44298</v>
+      </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13">
         <v>0.25</v>
@@ -1125,132 +1134,142 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
       <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G13" s="2">
+        <v>44317</v>
+      </c>
       <c r="I13" s="15">
         <f t="shared" ref="H11:I25" si="0">ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="J13" s="21">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="K13" s="22">
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G14" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H14" s="15"/>
       <c r="I14" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J14" s="21">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0.7270833333333333</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
       <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G15" s="2">
+        <v>44317</v>
+      </c>
       <c r="I15" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.75</v>
+      </c>
+      <c r="J15" s="21">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="K15" s="22">
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
       <c r="F16" s="2"/>
-      <c r="I16" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I16" s="15"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
       <c r="F17" s="2"/>
-      <c r="I17" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I17" s="15"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
       <c r="F18" s="2"/>
-      <c r="I18" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I18" s="15"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
       <c r="F19" s="2"/>
-      <c r="I19" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I19" s="15"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
       <c r="F20" s="2"/>
-      <c r="I20" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
       <c r="F21" s="2"/>
-      <c r="I21" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I21" s="15"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
       <c r="F22" s="2"/>
-      <c r="I22" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>12</v>
-      </c>
       <c r="F23" s="2"/>
-      <c r="I23" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I23" s="15"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I24" s="15"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I25" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="I25" s="15"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
@@ -1258,7 +1277,7 @@
       </c>
       <c r="C26" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>18.5</v>
+        <v>20.5</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>46</v>
@@ -1272,7 +1291,7 @@
       </c>
       <c r="G26" s="24">
         <f>SUM(I:I)</f>
-        <v>14.75</v>
+        <v>16.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[TASK] Anpassungen der Nutzeranforderungen
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13454A0A-2744-BD4A-82FE-EB065A789697}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824A2057-12B6-2B40-8C16-D35086F7CFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Weitere Nutzeranforderungen</t>
+  </si>
+  <si>
+    <t>Domainen Experten rekrutieren</t>
   </si>
 </sst>
 </file>
@@ -726,7 +729,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1159,7 @@
         <v>44317</v>
       </c>
       <c r="I13" s="15">
-        <f t="shared" ref="H11:I25" si="0">ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I13:I16" si="0">ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J13" s="21">
@@ -1234,50 +1237,101 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="F16" s="2"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F17" s="2"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="2">
+        <v>44299</v>
+      </c>
+      <c r="G16" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I16" s="15">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="J16" s="21">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="K16" s="22">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44300</v>
+      </c>
+      <c r="G17" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F18" s="2"/>
       <c r="I18" s="15"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F19" s="2"/>
       <c r="I19" s="15"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F20" s="2"/>
       <c r="I20" s="15"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F21" s="2"/>
       <c r="I21" s="15"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F22" s="2"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F23" s="2"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I24" s="15"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I25" s="15"/>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>20.5</v>
+        <v>22</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>46</v>
@@ -1291,15 +1345,15 @@
       </c>
       <c r="G26" s="24">
         <f>SUM(I:I)</f>
-        <v>16.75</v>
+        <v>18.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C3:C10" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C3:C10 C16:C17" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$2:$N$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2 C11:C25" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2 C11:C15 C18:C25" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$2:$N$5</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Add new Software Architecture
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824A2057-12B6-2B40-8C16-D35086F7CFEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44140267-C9C8-294D-8EE4-3AB79ADE121F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="17600" yWindow="760" windowWidth="51200" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -188,6 +188,21 @@
   </si>
   <si>
     <t>Domainen Experten rekrutieren</t>
+  </si>
+  <si>
+    <t>Architekturstile Recherche</t>
+  </si>
+  <si>
+    <t>Uber Architektur recherchieren</t>
+  </si>
+  <si>
+    <t>Architekturstile vergleichen</t>
+  </si>
+  <si>
+    <t>Architektur modellieren &amp; planen</t>
+  </si>
+  <si>
+    <t>Moegliche Technologien</t>
   </si>
 </sst>
 </file>
@@ -368,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -411,6 +426,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,35 +809,33 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="F2" s="2">
-        <v>44292</v>
+        <v>44293</v>
       </c>
       <c r="G2" s="2">
-        <v>44298</v>
-      </c>
+        <v>44317</v>
+      </c>
+      <c r="H2" s="14"/>
       <c r="I2">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>44</v>
-      </c>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -826,28 +845,28 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F3" s="2">
-        <v>44295</v>
+        <v>44292</v>
       </c>
       <c r="G3" s="2">
         <v>44298</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -858,28 +877,28 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="G4" s="2">
         <v>44298</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -896,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2">
         <v>44296</v>
@@ -907,11 +926,11 @@
       <c r="I5">
         <v>1</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>39</v>
+      <c r="N5" t="s">
+        <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -922,130 +941,125 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2">
-        <v>44298</v>
+        <v>44296</v>
       </c>
       <c r="G6" s="2">
         <v>44298</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13">
-        <v>0.25</v>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2">
         <v>44298</v>
       </c>
       <c r="G7" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
+        <v>44298</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13">
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="2">
         <v>44298</v>
       </c>
       <c r="G8" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I8">
-        <v>1.5</v>
-      </c>
-      <c r="L8" s="15"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="2">
         <v>44298</v>
       </c>
       <c r="G9" s="2">
-        <v>44317</v>
-      </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15">
-        <f>ROUNDUP(((SUM(K9-J9)*24*60/60)/0.25),0)*0.25</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="21">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="K9" s="22">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="L9" s="16"/>
-      <c r="M9" s="15"/>
-      <c r="P9" s="15"/>
+        <v>44338</v>
+      </c>
+      <c r="I9">
+        <v>1.5</v>
+      </c>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2">
         <v>44298</v>
@@ -1056,13 +1070,13 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15">
         <f>ROUNDUP(((SUM(K10-J10)*24*60/60)/0.25),0)*0.25</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J10" s="21">
-        <v>0.72916666666666663</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="K10" s="22">
-        <v>0.73958333333333337</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="L10" s="16"/>
       <c r="M10" s="15"/>
@@ -1070,37 +1084,40 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F11" s="2">
-        <v>44299</v>
+        <v>44298</v>
       </c>
       <c r="G11" s="2">
-        <v>44299</v>
-      </c>
-      <c r="H11" s="15">
+        <v>44317</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
         <f>ROUNDUP(((SUM(K11-J11)*24*60/60)/0.25),0)*0.25</f>
-        <v>1.5</v>
-      </c>
-      <c r="I11" s="15"/>
+        <v>0.5</v>
+      </c>
       <c r="J11" s="21">
-        <v>0.41666666666666669</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="K11" s="22">
-        <v>0.47361111111111115</v>
-      </c>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="L11" s="16"/>
+      <c r="M11" s="15"/>
+      <c r="P11" s="15"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1116,7 +1133,7 @@
         <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="2">
         <v>44299</v>
@@ -1126,47 +1143,48 @@
       </c>
       <c r="H12" s="15">
         <f>ROUNDUP(((SUM(K12-J12)*24*60/60)/0.25),0)*0.25</f>
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="I12" s="15"/>
       <c r="J12" s="21">
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="K12" s="22">
-        <v>0.59375</v>
+        <v>0.47361111111111115</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2">
         <v>44299</v>
       </c>
       <c r="G13" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I13" s="15">
-        <f t="shared" ref="I13:I16" si="0">ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
-        <v>0.25</v>
-      </c>
+        <v>44299</v>
+      </c>
+      <c r="H13" s="15">
+        <f>ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="I13" s="15"/>
       <c r="J13" s="21">
-        <v>0.59722222222222221</v>
+        <v>0.5</v>
       </c>
       <c r="K13" s="22">
-        <v>0.60416666666666663</v>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -1183,7 +1201,7 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="2">
         <v>44299</v>
@@ -1191,16 +1209,15 @@
       <c r="G14" s="2">
         <v>44317</v>
       </c>
-      <c r="H14" s="15"/>
       <c r="I14" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="I14:I23" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.25</v>
       </c>
       <c r="J14" s="21">
-        <v>0.69097222222222221</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="K14" s="22">
-        <v>0.7270833333333333</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1217,7 +1234,7 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2">
         <v>44299</v>
@@ -1225,51 +1242,52 @@
       <c r="G15" s="2">
         <v>44317</v>
       </c>
+      <c r="H15" s="15"/>
       <c r="I15" s="15">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J15" s="21">
-        <v>0.75347222222222221</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="K15" s="22">
-        <v>0.77777777777777779</v>
+        <v>0.7270833333333333</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F16" s="2">
         <v>44299</v>
       </c>
       <c r="G16" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I16" s="15">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="J16" s="21">
-        <v>0.79513888888888884</v>
+        <v>0.75347222222222221</v>
       </c>
       <c r="K16" s="22">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1283,78 +1301,278 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F17" s="2">
-        <v>44300</v>
+        <v>44299</v>
       </c>
       <c r="G17" s="2">
         <v>44338</v>
       </c>
       <c r="I17" s="15">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F18" s="2"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F19" s="2"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F21" s="2"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F22" s="2"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F23" s="2"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="21">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="K17" s="22">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44300</v>
+      </c>
+      <c r="G18" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44302</v>
+      </c>
+      <c r="G19" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I19" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J19" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K19" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="2">
+        <v>44302</v>
+      </c>
+      <c r="G20" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2">
+        <v>44302</v>
+      </c>
+      <c r="G21" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I21" s="15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="K21" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="2">
+        <v>44305</v>
+      </c>
+      <c r="G22" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J22" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K22" s="22">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F23" s="2">
+        <v>44305</v>
+      </c>
+      <c r="G23" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I23" s="15">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J23" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K23" s="22">
+        <v>0.6020833333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F24" s="2"/>
       <c r="I24" s="15"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F25" s="2"/>
       <c r="I25" s="15"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F26" s="2"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F27" s="2"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F28" s="2"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F29" s="2"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F30" s="2"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I32" s="15"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>22</v>
-      </c>
-      <c r="D26" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E34" s="24">
         <f>SUM(H:H)</f>
         <v>3.75</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F34" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>18.25</v>
+        <v>31.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C3:C10 C16:C17" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
-      <formula1>$N$2:$N$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+      <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2 C11:C15 C18:C25" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
-      <formula1>$N$2:$N$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+      <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[TASK] Add moderation für user story mapping
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5032CE4-6B3A-6F47-9894-2AA2D7683D76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2E7291-1908-0A48-836F-524D9E5DCC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30660" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Themenfeldanalyse</t>
+  </si>
+  <si>
+    <t>Moderation und Miro board vorbereiten</t>
   </si>
 </sst>
 </file>
@@ -759,7 +762,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,7 +1050,7 @@
         <v>44298</v>
       </c>
       <c r="G9" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I9">
         <v>1.5</v>
@@ -1219,7 +1222,7 @@
         <v>44317</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" ref="I14:I24" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I14:I27" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J14" s="21">
@@ -1316,7 +1319,7 @@
         <v>44299</v>
       </c>
       <c r="G17" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I17" s="15">
         <f t="shared" si="0"/>
@@ -1349,7 +1352,7 @@
         <v>44300</v>
       </c>
       <c r="G18" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I18" s="15">
         <v>0.75</v>
@@ -1375,7 +1378,7 @@
         <v>44302</v>
       </c>
       <c r="G19" s="2">
-        <v>44338</v>
+        <v>44317</v>
       </c>
       <c r="I19" s="15">
         <f t="shared" si="0"/>
@@ -1534,7 +1537,7 @@
         <v>44306</v>
       </c>
       <c r="G24" s="2">
-        <v>44306</v>
+        <v>44317</v>
       </c>
       <c r="H24" s="15">
         <f>ROUNDUP(((SUM(K24-J24)*24*60/60)/0.25),0)*0.25</f>
@@ -1550,7 +1553,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
@@ -1559,7 +1562,7 @@
         <v>39</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
         <v>58</v>
@@ -1568,7 +1571,7 @@
         <v>44306</v>
       </c>
       <c r="G25" s="2">
-        <v>44306</v>
+        <v>44317</v>
       </c>
       <c r="H25" s="15">
         <f>ROUNDUP(((SUM(K25-J25)*24*60/60)/0.25),0)*0.25</f>
@@ -1583,12 +1586,70 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F26" s="2"/>
-      <c r="I26" s="15"/>
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="2">
+        <v>44309</v>
+      </c>
+      <c r="G26" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I26" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J26" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K26" s="22">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="2"/>
-      <c r="I27" s="15"/>
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" s="2">
+        <v>44309</v>
+      </c>
+      <c r="G27" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I27" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J27" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K27" s="22">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F28" s="2"/>
@@ -1618,7 +1679,7 @@
       </c>
       <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>40.25</v>
+        <v>45.25</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>46</v>
@@ -1632,15 +1693,15 @@
       </c>
       <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>31.25</v>
+        <v>36.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C27" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C28:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add user stories by volunteers
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2E7291-1908-0A48-836F-524D9E5DCC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A94A33-75EB-F24E-A820-5E7E64E40460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -215,6 +215,18 @@
   </si>
   <si>
     <t>Moderation und Miro board vorbereiten</t>
+  </si>
+  <si>
+    <t>User Stories mit Freiwilligen</t>
+  </si>
+  <si>
+    <t>User Stories erweitern</t>
+  </si>
+  <si>
+    <t>Wochensumme</t>
+  </si>
+  <si>
+    <t>Mit Arbeit bei IW Medien</t>
   </si>
 </sst>
 </file>
@@ -259,7 +271,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -391,11 +403,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -444,6 +467,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,6 +809,8 @@
     <col min="9" max="9" width="18.1640625" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="19"/>
     <col min="11" max="11" width="10.83203125" style="20"/>
+    <col min="12" max="12" width="16.1640625" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -814,7 +847,12 @@
       <c r="K1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="14"/>
+      <c r="L1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="N1" t="s">
         <v>10</v>
       </c>
@@ -945,7 +983,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -970,6 +1008,14 @@
       <c r="I6">
         <v>1</v>
       </c>
+      <c r="L6" s="27">
+        <f>SUM(H2:I6)</f>
+        <v>17</v>
+      </c>
+      <c r="M6">
+        <f>SUM(L6+16)</f>
+        <v>33</v>
+      </c>
       <c r="N6" s="23" t="s">
         <v>39</v>
       </c>
@@ -977,7 +1023,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1222,7 +1268,7 @@
         <v>44317</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" ref="I14:I27" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I14:I29" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J14" s="21">
@@ -1299,7 +1345,7 @@
         <v>0.77777777777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1332,7 +1378,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1357,8 +1403,16 @@
       <c r="I18" s="15">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="27">
+        <f>SUM(H7:I18)</f>
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <f>SUM(L18+16)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1391,7 +1445,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1417,7 +1471,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1446,11 +1500,12 @@
       <c r="J21" s="21">
         <v>0.75</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="28">
         <v>0.79166666666666663</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="29"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1484,7 +1539,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1517,7 +1572,7 @@
         <v>0.6020833333333333</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>12</v>
       </c>
@@ -1551,7 +1606,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>13</v>
       </c>
@@ -1585,7 +1640,7 @@
         <v>0.63541666666666663</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10</v>
       </c>
@@ -1618,7 +1673,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10</v>
       </c>
@@ -1651,23 +1706,89 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="2"/>
-      <c r="I28" s="15"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="2"/>
-      <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="2">
+        <v>44311</v>
+      </c>
+      <c r="G28" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I28" s="15">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="J28" s="21">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="K28" s="22">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="L28" s="27">
+        <f>SUM(H19:I28)</f>
+        <v>20</v>
+      </c>
+      <c r="M28">
+        <f>SUM(L28+16)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="2">
+        <v>44312</v>
+      </c>
+      <c r="G29" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I29" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J29" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K29" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F30" s="2"/>
       <c r="I30" s="15"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F31" s="2"/>
       <c r="I31" s="15"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
@@ -1679,7 +1800,7 @@
       </c>
       <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>45.25</v>
+        <v>52</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>46</v>
@@ -1693,15 +1814,15 @@
       </c>
       <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>36.25</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C27" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C29" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C28:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C30:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add extended user stories
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A94A33-75EB-F24E-A820-5E7E64E40460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A744A3E-EFEC-A144-93EF-B395E9CA87EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28920" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,13 +1771,13 @@
       </c>
       <c r="I29" s="15">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="J29" s="21">
         <v>0.375</v>
       </c>
       <c r="K29" s="22">
-        <v>0.54166666666666663</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -1800,7 +1800,7 @@
       </c>
       <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>52</v>
+        <v>52.5</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>46</v>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>43</v>
+        <v>43.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Add dependencies between user requirements
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A744A3E-EFEC-A144-93EF-B395E9CA87EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BFCF0A-FC89-E448-91A8-517E33F62795}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Erste Schaetzung und Recherche</t>
   </si>
   <si>
-    <t>User Story Mapping</t>
-  </si>
-  <si>
     <t>User Stories (mapping)</t>
   </si>
   <si>
@@ -227,6 +224,9 @@
   </si>
   <si>
     <t>Mit Arbeit bei IW Medien</t>
+  </si>
+  <si>
+    <t>Beziehungen herstellen zwischen den Anforderungen</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -836,22 +836,22 @@
         <v>4</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="J1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="18" t="s">
-        <v>34</v>
-      </c>
       <c r="L1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="30" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>63</v>
       </c>
       <c r="N1" t="s">
         <v>10</v>
@@ -862,16 +862,16 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" s="2">
         <v>44293</v>
@@ -916,7 +916,7 @@
         <v>11</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -980,7 +980,7 @@
         <v>6</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>33</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -1055,16 +1055,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" s="2">
         <v>44298</v>
@@ -1081,16 +1081,16 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2">
         <v>44298</v>
@@ -1108,16 +1108,16 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2">
         <v>44298</v>
@@ -1154,7 +1154,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="2">
         <v>44298</v>
@@ -1182,16 +1182,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>40</v>
       </c>
       <c r="F12" s="2">
         <v>44299</v>
@@ -1216,16 +1216,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="2">
         <v>44299</v>
@@ -1250,16 +1250,16 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2">
         <v>44299</v>
@@ -1268,7 +1268,7 @@
         <v>44317</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" ref="I14:I29" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I14:I30" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J14" s="21">
@@ -1283,16 +1283,16 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="2">
         <v>44299</v>
@@ -1317,16 +1317,16 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="2">
         <v>44299</v>
@@ -1350,16 +1350,16 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="2">
         <v>44299</v>
@@ -1383,16 +1383,16 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="2">
         <v>44300</v>
@@ -1417,16 +1417,16 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="2">
         <v>44302</v>
@@ -1450,16 +1450,16 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
         <v>51</v>
-      </c>
-      <c r="E20" t="s">
-        <v>52</v>
       </c>
       <c r="F20" s="2">
         <v>44302</v>
@@ -1476,16 +1476,16 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21" s="2">
         <v>44302</v>
@@ -1510,16 +1510,16 @@
         <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="2">
         <v>44305</v>
@@ -1544,16 +1544,16 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F23" s="2">
         <v>44305</v>
@@ -1577,16 +1577,16 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" t="s">
         <v>56</v>
-      </c>
-      <c r="E24" t="s">
-        <v>57</v>
       </c>
       <c r="F24" s="2">
         <v>44306</v>
@@ -1611,16 +1611,16 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F25" s="2">
         <v>44306</v>
@@ -1645,16 +1645,16 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F26" s="2">
         <v>44309</v>
@@ -1678,16 +1678,16 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="2">
         <v>44309</v>
@@ -1711,16 +1711,16 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" s="2">
         <v>44311</v>
@@ -1752,16 +1752,16 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29" s="2">
         <v>44312</v>
@@ -1781,8 +1781,37 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F30" s="2"/>
-      <c r="I30" s="15"/>
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" s="2">
+        <v>44312</v>
+      </c>
+      <c r="G30" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I30" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="J30" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K30" s="22">
+        <v>0.72916666666666663</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F31" s="2"/>
@@ -1800,29 +1829,29 @@
       </c>
       <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>52.5</v>
+        <v>55</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="24">
         <f>SUM(H:H)</f>
         <v>9</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>43.5</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C29" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C30" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C30:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C31:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Update dependencies between system and user requirements
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BFCF0A-FC89-E448-91A8-517E33F62795}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246373DF-D389-6A46-AA2F-C0862F28AA24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>Beziehungen herstellen zwischen den Anforderungen</t>
+  </si>
+  <si>
+    <t>UML Diagramm anfertigen</t>
+  </si>
+  <si>
+    <t>Erfassen und Dokumentieren im Issue</t>
   </si>
 </sst>
 </file>
@@ -793,7 +799,7 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1274,7 @@
         <v>44317</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" ref="I14:I30" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I14:I31" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J14" s="21">
@@ -1791,10 +1797,10 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F30" s="2">
         <v>44312</v>
@@ -1814,8 +1820,37 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F31" s="2"/>
-      <c r="I31" s="15"/>
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="2">
+        <v>44312</v>
+      </c>
+      <c r="G31" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="J31" s="21">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="K31" s="22">
+        <v>0.77083333333333337</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="I32" s="15"/>
@@ -1829,7 +1864,7 @@
       </c>
       <c r="C34" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>55</v>
+        <v>56.25</v>
       </c>
       <c r="D34" s="14" t="s">
         <v>45</v>
@@ -1843,15 +1878,15 @@
       </c>
       <c r="G34" s="24">
         <f>SUM(I:I)</f>
-        <v>46</v>
+        <v>47.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C30" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C31" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C31:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C32:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Update user stories
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246373DF-D389-6A46-AA2F-C0862F28AA24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A082448-4FD5-364B-B473-E49846F6E85A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -233,6 +233,15 @@
   </si>
   <si>
     <t>Erfassen und Dokumentieren im Issue</t>
+  </si>
+  <si>
+    <t>Vorstellung</t>
+  </si>
+  <si>
+    <t>Notizen von der Vorstellung festhalten</t>
+  </si>
+  <si>
+    <t>Änderungen übernehmen und weitere Organisation</t>
   </si>
 </sst>
 </file>
@@ -796,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P34"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1274,7 +1283,7 @@
         <v>44317</v>
       </c>
       <c r="I14" s="15">
-        <f t="shared" ref="I14:I31" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I14:I34" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J14" s="21">
@@ -1853,40 +1862,165 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
+      <c r="A32">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="2">
+        <v>44313</v>
+      </c>
+      <c r="G32" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H32" s="15">
+        <f>ROUNDUP(((SUM(K32-J32)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="J32" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K32" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="2">
+        <v>44313</v>
+      </c>
+      <c r="G33" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H33" s="15">
+        <f>ROUNDUP(((SUM(K33-J33)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K33" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44313</v>
+      </c>
+      <c r="G34" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K34" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="15"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="22"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="15"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="22"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="15"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="22"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="15"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="22"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="24">
+      <c r="C40" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>56.25</v>
-      </c>
-      <c r="D34" s="14" t="s">
+        <v>63.25</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="24">
+      <c r="E40" s="24">
         <f>SUM(H:H)</f>
-        <v>9</v>
-      </c>
-      <c r="F34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G40" s="24">
         <f>SUM(I:I)</f>
-        <v>47.25</v>
+        <v>49.25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C31" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C31 C34" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C32:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C35:C39 C32:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add compared system-architecture
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A082448-4FD5-364B-B473-E49846F6E85A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D931866B-E34B-BE4D-A617-6D2CAECA97CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -241,7 +241,22 @@
     <t>Notizen von der Vorstellung festhalten</t>
   </si>
   <si>
-    <t>Änderungen übernehmen und weitere Organisation</t>
+    <t>Aenderungen uebernehmen und weitere Organisation</t>
+  </si>
+  <si>
+    <t>Abhaengigkeiten aktualisieren und Architekturstile recherchieren</t>
+  </si>
+  <si>
+    <t>Konzeptuelles Design</t>
+  </si>
+  <si>
+    <t>Systemarchitektur</t>
+  </si>
+  <si>
+    <t>Architekturstile sammeln</t>
+  </si>
+  <si>
+    <t>Architekturstile gegenueberstellen</t>
   </si>
 </sst>
 </file>
@@ -805,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,73 +1054,53 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="2">
-        <v>44298</v>
-      </c>
-      <c r="G7" s="2">
-        <v>44298</v>
-      </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13">
-        <v>0.25</v>
-      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="L7" s="7"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="2">
         <v>44298</v>
       </c>
       <c r="G8" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I8">
-        <v>0.5</v>
+        <v>44298</v>
+      </c>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13">
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2">
         <v>44298</v>
@@ -1114,25 +1109,24 @@
         <v>44317</v>
       </c>
       <c r="I9">
-        <v>1.5</v>
-      </c>
-      <c r="L9" s="15"/>
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F10" s="2">
         <v>44298</v>
@@ -1140,36 +1134,26 @@
       <c r="G10" s="2">
         <v>44317</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15">
-        <f>ROUNDUP(((SUM(K10-J10)*24*60/60)/0.25),0)*0.25</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="21">
-        <v>0.68402777777777779</v>
-      </c>
-      <c r="K10" s="22">
-        <v>0.72222222222222221</v>
-      </c>
-      <c r="L10" s="16"/>
-      <c r="M10" s="15"/>
-      <c r="P10" s="15"/>
+      <c r="I10">
+        <v>1.5</v>
+      </c>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" s="2">
         <v>44298</v>
@@ -1180,13 +1164,13 @@
       <c r="H11" s="15"/>
       <c r="I11" s="15">
         <f>ROUNDUP(((SUM(K11-J11)*24*60/60)/0.25),0)*0.25</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J11" s="21">
-        <v>0.72916666666666663</v>
+        <v>0.68402777777777779</v>
       </c>
       <c r="K11" s="22">
-        <v>0.73958333333333337</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="15"/>
@@ -1194,37 +1178,40 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F12" s="2">
-        <v>44299</v>
+        <v>44298</v>
       </c>
       <c r="G12" s="2">
-        <v>44299</v>
-      </c>
-      <c r="H12" s="15">
+        <v>44317</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
         <f>ROUNDUP(((SUM(K12-J12)*24*60/60)/0.25),0)*0.25</f>
-        <v>1.5</v>
-      </c>
-      <c r="I12" s="15"/>
+        <v>0.5</v>
+      </c>
       <c r="J12" s="21">
-        <v>0.41666666666666669</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="K12" s="22">
-        <v>0.47361111111111115</v>
-      </c>
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="L12" s="16"/>
+      <c r="M12" s="15"/>
+      <c r="P12" s="15"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1240,7 +1227,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2">
         <v>44299</v>
@@ -1250,47 +1237,48 @@
       </c>
       <c r="H13" s="15">
         <f>ROUNDUP(((SUM(K13-J13)*24*60/60)/0.25),0)*0.25</f>
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="21">
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="K13" s="22">
-        <v>0.59375</v>
+        <v>0.47361111111111115</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F14" s="2">
         <v>44299</v>
       </c>
       <c r="G14" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I14" s="15">
-        <f t="shared" ref="I14:I34" si="0">ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
-        <v>0.25</v>
-      </c>
+        <v>44299</v>
+      </c>
+      <c r="H14" s="15">
+        <f>ROUNDUP(((SUM(K14-J14)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="I14" s="15"/>
       <c r="J14" s="21">
-        <v>0.59722222222222221</v>
+        <v>0.5</v>
       </c>
       <c r="K14" s="22">
-        <v>0.60416666666666663</v>
+        <v>0.59375</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1307,7 +1295,7 @@
         <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="2">
         <v>44299</v>
@@ -1315,16 +1303,15 @@
       <c r="G15" s="2">
         <v>44317</v>
       </c>
-      <c r="H15" s="15"/>
       <c r="I15" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="I15:I42" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.25</v>
       </c>
       <c r="J15" s="21">
-        <v>0.69097222222222221</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="K15" s="22">
-        <v>0.7270833333333333</v>
+        <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1341,7 +1328,7 @@
         <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F16" s="2">
         <v>44299</v>
@@ -1349,20 +1336,21 @@
       <c r="G16" s="2">
         <v>44317</v>
       </c>
+      <c r="H16" s="15"/>
       <c r="I16" s="15">
         <f t="shared" si="0"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J16" s="21">
-        <v>0.75347222222222221</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="K16" s="22">
-        <v>0.77777777777777779</v>
+        <v>0.7270833333333333</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -1371,10 +1359,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F17" s="2">
         <v>44299</v>
@@ -1387,13 +1375,13 @@
         <v>0.75</v>
       </c>
       <c r="J17" s="21">
-        <v>0.79513888888888884</v>
+        <v>0.75347222222222221</v>
       </c>
       <c r="K17" s="22">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.77777777777777779</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1407,27 +1395,26 @@
         <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="F18" s="2">
-        <v>44300</v>
+        <v>44299</v>
       </c>
       <c r="G18" s="2">
         <v>44317</v>
       </c>
       <c r="I18" s="15">
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="L18" s="27">
-        <f>SUM(H7:I18)</f>
-        <v>11</v>
-      </c>
-      <c r="M18">
-        <f>SUM(L18+16)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="21">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="K18" s="22">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1441,54 +1428,35 @@
         <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F19" s="2">
-        <v>44302</v>
+        <v>44300</v>
       </c>
       <c r="G19" s="2">
         <v>44317</v>
       </c>
       <c r="I19" s="15">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J19" s="21">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="2">
-        <v>44302</v>
-      </c>
-      <c r="G20" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0.5</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="L19" s="27">
+        <f>SUM(H8:I19)</f>
+        <v>11</v>
+      </c>
+      <c r="M19">
+        <f>SUM(L19+16)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="I20" s="15"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
@@ -1497,10 +1465,10 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F21" s="2">
         <v>44302</v>
@@ -1510,15 +1478,14 @@
       </c>
       <c r="I21" s="15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="21">
-        <v>0.75</v>
-      </c>
-      <c r="K21" s="28">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="L21" s="29"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K21" s="22">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1534,24 +1501,16 @@
         <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F22" s="2">
-        <v>44305</v>
+        <v>44302</v>
       </c>
       <c r="G22" s="2">
         <v>44317</v>
       </c>
-      <c r="H22" s="14"/>
       <c r="I22" s="15">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J22" s="21">
-        <v>0.375</v>
-      </c>
-      <c r="K22" s="22">
-        <v>0.45833333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -1568,160 +1527,162 @@
         <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" s="2">
-        <v>44305</v>
+        <v>44302</v>
       </c>
       <c r="G23" s="2">
         <v>44317</v>
       </c>
       <c r="I23" s="15">
         <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J23" s="21">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="K23" s="22">
-        <v>0.6020833333333333</v>
-      </c>
+        <v>0.75</v>
+      </c>
+      <c r="K23" s="28">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="L23" s="29"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F24" s="2">
-        <v>44306</v>
+        <v>44305</v>
       </c>
       <c r="G24" s="2">
         <v>44317</v>
       </c>
-      <c r="H24" s="15">
-        <f>ROUNDUP(((SUM(K24-J24)*24*60/60)/0.25),0)*0.25</f>
-        <v>4</v>
-      </c>
-      <c r="I24" s="15"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J24" s="21">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="K24" s="22">
-        <v>0.58333333333333337</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F25" s="2">
-        <v>44306</v>
+        <v>44305</v>
       </c>
       <c r="G25" s="2">
         <v>44317</v>
       </c>
-      <c r="H25" s="15">
-        <f>ROUNDUP(((SUM(K25-J25)*24*60/60)/0.25),0)*0.25</f>
-        <v>1.25</v>
-      </c>
-      <c r="I25" s="15"/>
+      <c r="I25" s="15">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="J25" s="21">
-        <v>0.58333333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="K25" s="22">
-        <v>0.63541666666666663</v>
+        <v>0.6020833333333333</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
         <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="F26" s="2">
-        <v>44309</v>
+        <v>44306</v>
       </c>
       <c r="G26" s="2">
         <v>44317</v>
       </c>
-      <c r="I26" s="15">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
+      <c r="H26" s="15">
+        <f>ROUNDUP(((SUM(K26-J26)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="I26" s="15"/>
       <c r="J26" s="21">
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="K26" s="22">
-        <v>0.5</v>
+        <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2">
-        <v>44309</v>
+        <v>44306</v>
       </c>
       <c r="G27" s="2">
         <v>44317</v>
       </c>
-      <c r="I27" s="15">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+      <c r="H27" s="15">
+        <f>ROUNDUP(((SUM(K27-J27)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="I27" s="15"/>
       <c r="J27" s="21">
-        <v>0.66666666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="K27" s="22">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>0.63541666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1729,40 +1690,32 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="F28" s="2">
-        <v>44311</v>
+        <v>44309</v>
       </c>
       <c r="G28" s="2">
         <v>44317</v>
       </c>
       <c r="I28" s="15">
         <f t="shared" si="0"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="J28" s="21">
-        <v>0.69097222222222221</v>
+        <v>0.375</v>
       </c>
       <c r="K28" s="22">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="L28" s="27">
-        <f>SUM(H19:I28)</f>
-        <v>20</v>
-      </c>
-      <c r="M28">
-        <f>SUM(L28+16)</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -1770,34 +1723,34 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
         <v>29</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F29" s="2">
-        <v>44312</v>
+        <v>44309</v>
       </c>
       <c r="G29" s="2">
         <v>44317</v>
       </c>
       <c r="I29" s="15">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>2</v>
       </c>
       <c r="J29" s="21">
-        <v>0.375</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K29" s="22">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
         <v>36</v>
@@ -1806,130 +1759,113 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F30" s="2">
-        <v>44312</v>
+        <v>44311</v>
       </c>
       <c r="G30" s="2">
         <v>44317</v>
       </c>
       <c r="I30" s="15">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="J30" s="21">
-        <v>0.625</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="K30" s="22">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="2">
-        <v>44312</v>
-      </c>
-      <c r="G31" s="2">
-        <v>44317</v>
-      </c>
-      <c r="I31" s="15">
-        <f t="shared" si="0"/>
-        <v>1.25</v>
-      </c>
-      <c r="J31" s="21">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="K31" s="22">
-        <v>0.77083333333333337</v>
-      </c>
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="L30" s="27">
+        <f>SUM(H21:I30)</f>
+        <v>20</v>
+      </c>
+      <c r="M30">
+        <f>SUM(L30+16)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" t="s">
-        <v>38</v>
-      </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F32" s="2">
-        <v>44313</v>
+        <v>44312</v>
       </c>
       <c r="G32" s="2">
         <v>44317</v>
       </c>
-      <c r="H32" s="15">
-        <f>ROUNDUP(((SUM(K32-J32)*24*60/60)/0.25),0)*0.25</f>
-        <v>4</v>
+      <c r="I32" s="15">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
       <c r="J32" s="21">
         <v>0.375</v>
       </c>
       <c r="K32" s="22">
-        <v>0.54166666666666663</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" t="s">
         <v>12</v>
       </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F33" s="2">
-        <v>44313</v>
+        <v>44312</v>
       </c>
       <c r="G33" s="2">
         <v>44317</v>
       </c>
-      <c r="H33" s="15">
-        <f>ROUNDUP(((SUM(K33-J33)*24*60/60)/0.25),0)*0.25</f>
-        <v>1</v>
+      <c r="I33" s="15">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="J33" s="21">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
       <c r="K33" s="22">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
         <v>36</v>
@@ -1938,89 +1874,377 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44312</v>
+      </c>
+      <c r="G34" s="2">
+        <v>44317</v>
+      </c>
+      <c r="I34" s="15">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="J34" s="21">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="K34" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="2">
+        <v>44313</v>
+      </c>
+      <c r="G35" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H35" s="15">
+        <f>ROUNDUP(((SUM(K35-J35)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="J35" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K35" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F36" s="2">
+        <v>44313</v>
+      </c>
+      <c r="G36" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H36" s="15">
+        <f>ROUNDUP(((SUM(K36-J36)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J36" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K36" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
         <v>29</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E37" t="s">
         <v>68</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F37" s="2">
         <v>44313</v>
       </c>
-      <c r="G34" s="2">
-        <v>44317</v>
-      </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15">
+      <c r="G37" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J34" s="21">
+      <c r="J37" s="21">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K37" s="22">
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="15"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="22"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="15"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="22"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="15"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="22"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" t="s">
+        <v>69</v>
+      </c>
+      <c r="F38" s="2">
+        <v>44317</v>
+      </c>
+      <c r="G38" s="2">
+        <v>44317</v>
+      </c>
       <c r="H38" s="15"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="22"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+      <c r="I38" s="15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J38" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K38" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="E39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="2">
+        <v>44318</v>
+      </c>
+      <c r="G39" s="2">
+        <v>44317</v>
+      </c>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J39" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K39" s="22">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="L39" s="27">
+        <f>SUM(H32:I39)</f>
+        <v>23.25</v>
+      </c>
+      <c r="M39">
+        <f>SUM(L39+16)</f>
+        <v>39.25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="22"/>
+      <c r="L40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>9</v>
       </c>
-      <c r="C40" s="24">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" t="s">
+        <v>72</v>
+      </c>
+      <c r="F41" s="2">
+        <v>44319</v>
+      </c>
+      <c r="G41" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J41" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K41" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="2">
+        <v>44319</v>
+      </c>
+      <c r="G42" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="J42" s="21">
+        <v>0.5625</v>
+      </c>
+      <c r="K42" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="22"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="22"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="22"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="22"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="22"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>63.25</v>
-      </c>
-      <c r="D40" s="14" t="s">
+        <v>76.75</v>
+      </c>
+      <c r="D52" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="24">
+      <c r="E52" s="24">
         <f>SUM(H:H)</f>
         <v>14</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F52" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G52" s="24">
         <f>SUM(I:I)</f>
-        <v>49.25</v>
+        <v>62.75</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C11 C17:C19 C26:C31 C34" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C12:C16 C20:C25 C35:C39 C32:C33" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Add system architecture
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D931866B-E34B-BE4D-A617-6D2CAECA97CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD726BB-892B-F74E-8E27-0881FCD7AF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29780" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -257,6 +257,12 @@
   </si>
   <si>
     <t>Architekturstile gegenueberstellen</t>
+  </si>
+  <si>
+    <t>Systemarchitektur Anforderungen sammeln</t>
+  </si>
+  <si>
+    <t>Systemarchitektur modellieren</t>
   </si>
 </sst>
 </file>
@@ -822,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,7 +1310,7 @@
         <v>44317</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" ref="I15:I42" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I15:I44" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J15" s="21">
@@ -2150,24 +2156,74 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
+        <v>74</v>
+      </c>
+      <c r="F43" s="2">
+        <v>44320</v>
+      </c>
+      <c r="G43" s="2">
+        <v>44338</v>
+      </c>
       <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="22"/>
+      <c r="I43" s="15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J43" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K43" s="22">
+        <v>0.54166666666666663</v>
+      </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="2">
+        <v>44320</v>
+      </c>
+      <c r="G44" s="2">
+        <v>44338</v>
+      </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
+      <c r="I44" s="15">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="J44" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K44" s="22">
+        <v>0.78125</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
       <c r="H45" s="15"/>
       <c r="I45" s="15"/>
       <c r="J45" s="21"/>
@@ -2222,7 +2278,7 @@
       </c>
       <c r="C52" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>76.75</v>
+        <v>85.5</v>
       </c>
       <c r="D52" s="14" t="s">
         <v>45</v>
@@ -2236,7 +2292,7 @@
       </c>
       <c r="G52" s="24">
         <f>SUM(I:I)</f>
-        <v>62.75</v>
+        <v>71.5</v>
       </c>
     </row>
   </sheetData>
@@ -2244,7 +2300,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C44 C46:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Add system diagram
Enhancement
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD726BB-892B-F74E-8E27-0881FCD7AF9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7A84EA-FBCC-684A-827A-096DD4858CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29780" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="78">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>Systemarchitektur modellieren</t>
+  </si>
+  <si>
+    <t>Modellierung erweitern</t>
+  </si>
+  <si>
+    <t>Modellierung verfeinern</t>
   </si>
 </sst>
 </file>
@@ -828,8 +834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1316,7 @@
         <v>44317</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" ref="I15:I44" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I15:I47" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J15" s="21">
@@ -2224,26 +2230,106 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" s="2">
+        <v>44322</v>
+      </c>
+      <c r="G45" s="2">
+        <v>44338</v>
+      </c>
       <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="22"/>
+      <c r="I45" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J45" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K45" s="22">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="A46">
+        <v>9</v>
+      </c>
+      <c r="B46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>71</v>
+      </c>
+      <c r="E46" t="s">
+        <v>76</v>
+      </c>
+      <c r="F46" s="2">
+        <v>44323</v>
+      </c>
+      <c r="G46" s="2">
+        <v>44338</v>
+      </c>
       <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="22"/>
+      <c r="I46" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J46" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K46" s="22">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="A47">
+        <v>9</v>
+      </c>
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="2">
+        <v>44323</v>
+      </c>
+      <c r="G47" s="2">
+        <v>44338</v>
+      </c>
       <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="22"/>
+      <c r="I47" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J47" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K47" s="22">
+        <v>0.83333333333333337</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F48" s="2"/>
@@ -2254,8 +2340,12 @@
       <c r="K48" s="22"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="F49" s="2">
+        <v>44326</v>
+      </c>
+      <c r="G49" s="2">
+        <v>44338</v>
+      </c>
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="21"/>
@@ -2278,7 +2368,7 @@
       </c>
       <c r="C52" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>85.5</v>
+        <v>94.5</v>
       </c>
       <c r="D52" s="14" t="s">
         <v>45</v>
@@ -2292,7 +2382,7 @@
       </c>
       <c r="G52" s="24">
         <f>SUM(I:I)</f>
-        <v>71.5</v>
+        <v>80.5</v>
       </c>
     </row>
   </sheetData>
@@ -2300,7 +2390,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C44 C46:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Add system architecture documentation
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7A84EA-FBCC-684A-827A-096DD4858CE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69016CB9-946E-F44C-A039-08C6BA2D6801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="-51200" yWindow="-5600" windowWidth="29780" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="79">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Modellierung verfeinern</t>
+  </si>
+  <si>
+    <t>Modellierung dokumentieren</t>
   </si>
 </sst>
 </file>
@@ -832,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P52"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1316,7 +1319,7 @@
         <v>44317</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" ref="I15:I47" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I15:I48" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J15" s="21">
@@ -2331,58 +2334,100 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+    <row r="48" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="2">
+        <v>44325</v>
+      </c>
+      <c r="G48" s="2">
+        <v>44338</v>
+      </c>
       <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="22"/>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F49" s="2">
-        <v>44326</v>
-      </c>
-      <c r="G49" s="2">
-        <v>44338</v>
-      </c>
+      <c r="I48" s="15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J48" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K48" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="L48" s="27">
+        <f>SUM(H41:I48)</f>
+        <v>29.25</v>
+      </c>
+      <c r="M48">
+        <f>SUM(L48+16)</f>
+        <v>45.25</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
       <c r="H49" s="15"/>
       <c r="I49" s="15"/>
       <c r="J49" s="21"/>
       <c r="K49" s="22"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="F50" s="2">
+        <v>44326</v>
+      </c>
+      <c r="G50" s="2">
+        <v>44338</v>
+      </c>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
       <c r="J50" s="21"/>
       <c r="K50" s="22"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="15"/>
       <c r="I51" s="15"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="22"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="24">
+      <c r="C53" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>94.5</v>
-      </c>
-      <c r="D52" s="14" t="s">
+        <v>100.5</v>
+      </c>
+      <c r="D53" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E52" s="24">
+      <c r="E53" s="24">
         <f>SUM(H:H)</f>
         <v>14</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F53" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="24">
+      <c r="G53" s="24">
         <f>SUM(I:I)</f>
-        <v>80.5</v>
+        <v>86.5</v>
       </c>
     </row>
   </sheetData>
@@ -2390,7 +2435,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C51" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C52" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add expose for seminar
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D2564D-9A34-354D-8684-AF55045EF1E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB7C84-94EB-BB45-87B4-11FAE0AC08CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-5600" windowWidth="29780" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="83">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>Modellierung dokumentieren</t>
+  </si>
+  <si>
+    <t>Schreibwerkstatt</t>
+  </si>
+  <si>
+    <t>Abschlussvorträge und Fragen stellen</t>
+  </si>
+  <si>
+    <t>Expose überarbeiten</t>
+  </si>
+  <si>
+    <t>Peer Reviewed Expose</t>
   </si>
 </sst>
 </file>
@@ -463,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -521,6 +533,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -835,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1319,7 +1332,7 @@
         <v>44317</v>
       </c>
       <c r="I15" s="15">
-        <f t="shared" ref="I15:I49" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I15:I51" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J15" s="21">
@@ -2334,7 +2347,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>9</v>
       </c>
@@ -2367,16 +2380,8 @@
       <c r="K48" s="22">
         <v>0.75</v>
       </c>
-      <c r="L48" s="27">
-        <f>SUM(H41:I48)</f>
-        <v>29.25</v>
-      </c>
-      <c r="M48">
-        <f>SUM(L48+16)</f>
-        <v>45.25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9</v>
       </c>
@@ -2409,8 +2414,16 @@
       <c r="K49" s="22">
         <v>0.82291666666666663</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" s="31">
+        <f>SUM(H41:I49)</f>
+        <v>30</v>
+      </c>
+      <c r="M49">
+        <f>SUM(L49+16)</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="15"/>
@@ -2418,7 +2431,19 @@
       <c r="J50" s="21"/>
       <c r="K50" s="22"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>71</v>
+      </c>
       <c r="F51" s="2">
         <v>44326</v>
       </c>
@@ -2426,40 +2451,149 @@
         <v>44338</v>
       </c>
       <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
+      <c r="I51" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="J51" s="21"/>
       <c r="K51" s="22"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="15"/>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>15</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" t="s">
+        <v>80</v>
+      </c>
+      <c r="F52" s="2">
+        <v>44327</v>
+      </c>
+      <c r="G52" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H52" s="15">
+        <f>ROUNDUP(((SUM(K52-J52)*24*60/60)/0.25),0)*0.25</f>
+        <v>4.75</v>
+      </c>
       <c r="I52" s="15"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="22"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J52" s="21">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="K52" s="22">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>82</v>
+      </c>
+      <c r="E53" t="s">
+        <v>81</v>
+      </c>
+      <c r="F53" s="2">
+        <v>44327</v>
+      </c>
+      <c r="G53" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H53" s="15">
+        <f>ROUNDUP(((SUM(K53-J53)*24*60/60)/0.25),0)*0.25</f>
+        <v>4.75</v>
+      </c>
       <c r="I53" s="15"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="1" t="s">
+      <c r="J53" s="21">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K53" s="22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s">
+        <v>81</v>
+      </c>
+      <c r="F54" s="2">
+        <v>44329</v>
+      </c>
+      <c r="G54" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H54" s="15">
+        <f>ROUNDUP(((SUM(K54-J54)*24*60/60)/0.25),0)*0.25</f>
+        <v>6</v>
+      </c>
+      <c r="I54" s="15"/>
+      <c r="J54" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K54" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="24">
+      <c r="C60" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>101.25</v>
-      </c>
-      <c r="D54" s="14" t="s">
+        <v>116.75</v>
+      </c>
+      <c r="D60" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E54" s="24">
+      <c r="E60" s="24">
         <f>SUM(H:H)</f>
-        <v>14</v>
-      </c>
-      <c r="F54" s="14" t="s">
+        <v>29.5</v>
+      </c>
+      <c r="F60" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G54" s="24">
+      <c r="G60" s="24">
         <f>SUM(I:I)</f>
         <v>87.25</v>
       </c>
@@ -2469,7 +2603,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C53" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C59" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[WIP][FEATURE] Add content map
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C33886B-8C4E-4742-8C21-463BF9A16777}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AAC7B2-7456-3F47-9959-1721EB1FFD6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="1020" yWindow="960" windowWidth="30460" windowHeight="17860" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -284,6 +284,33 @@
   </si>
   <si>
     <t>Peer Reviewed Expose</t>
+  </si>
+  <si>
+    <t>Expose der anderen kommentieren</t>
+  </si>
+  <si>
+    <t>Umfrage</t>
+  </si>
+  <si>
+    <t>Umfrage erstellt und versendet</t>
+  </si>
+  <si>
+    <t>Umfrage auswerten</t>
+  </si>
+  <si>
+    <t>Content Map</t>
+  </si>
+  <si>
+    <t>Content Map beginnen</t>
+  </si>
+  <si>
+    <t>Content Map iterieren</t>
+  </si>
+  <si>
+    <t>Peer reviewed Exposé</t>
+  </si>
+  <si>
+    <t>Exposé vorstellen</t>
   </si>
 </sst>
 </file>
@@ -848,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="K63" sqref="K63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2561,49 +2588,287 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>15</v>
+      </c>
+      <c r="B55" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>82</v>
+      </c>
+      <c r="E55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" s="2">
+        <v>44331</v>
+      </c>
+      <c r="G55" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H55" s="15">
+        <f>ROUNDUP(((SUM(K55-J55)*24*60/60)/0.25),0)*0.25</f>
+        <v>3</v>
+      </c>
       <c r="I55" s="15"/>
+      <c r="J55" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K55" s="22">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I56" s="15"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="2">
+        <v>44331</v>
+      </c>
+      <c r="G56" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I56" s="15">
+        <f t="shared" ref="I56:I62" si="1">ROUNDUP(((SUM(K56-J56)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.75</v>
+      </c>
+      <c r="J56" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K56" s="22">
+        <v>0.57291666666666663</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" t="s">
+        <v>86</v>
+      </c>
+      <c r="F57" s="2">
+        <v>44332</v>
+      </c>
+      <c r="G57" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I57" s="15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J57" s="21">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K57" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="L57" s="31">
+        <f>SUM(H49:I57)</f>
+        <v>23</v>
+      </c>
+      <c r="M57">
+        <f>SUM(L57+16)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="G58" s="2"/>
       <c r="I58" s="15"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="22"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="I59" s="15"/>
+      <c r="A59">
+        <v>18</v>
+      </c>
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>88</v>
+      </c>
+      <c r="F59" s="2">
+        <v>44333</v>
+      </c>
+      <c r="G59" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I59" s="15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J59" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K59" s="22">
+        <v>0.54166666666666663</v>
+      </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B60" s="1" t="s">
+      <c r="A60">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" s="2">
+        <v>44333</v>
+      </c>
+      <c r="G60" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I60" s="15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J60" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K60" s="22">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" s="2">
+        <v>44334</v>
+      </c>
+      <c r="G61" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H61" s="15">
+        <f>ROUNDUP(((SUM(K61-J61)*24*60/60)/0.25),0)*0.25</f>
+        <v>3</v>
+      </c>
+      <c r="I61" s="15"/>
+      <c r="J61" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K61" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>18</v>
+      </c>
+      <c r="B62" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>87</v>
+      </c>
+      <c r="E62" t="s">
+        <v>89</v>
+      </c>
+      <c r="F62" s="2">
+        <v>44334</v>
+      </c>
+      <c r="G62" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I62" s="15">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J62" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K62" s="22">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="24">
+      <c r="C65" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>116.75</v>
-      </c>
-      <c r="D60" s="14" t="s">
+        <v>136.5</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E60" s="24">
+      <c r="E65" s="24">
         <f>SUM(H:H)</f>
-        <v>29.5</v>
-      </c>
-      <c r="F60" s="14" t="s">
+        <v>35.5</v>
+      </c>
+      <c r="F65" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G60" s="24">
+      <c r="G65" s="24">
         <f>SUM(I:I)</f>
-        <v>87.25</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C59" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C64" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add interview results
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AAC7B2-7456-3F47-9959-1721EB1FFD6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F86D878-5735-7F4C-A29C-418A6AEB2EBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="960" windowWidth="30460" windowHeight="17860" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="93">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Exposé vorstellen</t>
+  </si>
+  <si>
+    <t>Exposé reviewen</t>
   </si>
 </sst>
 </file>
@@ -875,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P65"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2838,29 +2841,117 @@
       <c r="I63" s="15"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>90</v>
+      </c>
+      <c r="E64" t="s">
+        <v>92</v>
+      </c>
+      <c r="F64" s="2">
+        <v>44334</v>
+      </c>
+      <c r="G64" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H64" s="15">
+        <f>ROUNDUP(((SUM(K64-J64)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
       <c r="I64" s="15"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B65" s="1" t="s">
+      <c r="J64" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K64" s="22">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" t="s">
+        <v>86</v>
+      </c>
+      <c r="F65" s="2">
+        <v>44332</v>
+      </c>
+      <c r="G65" s="2">
+        <v>44338</v>
+      </c>
+      <c r="I65" s="15">
+        <f t="shared" ref="I65" si="2">ROUNDUP(((SUM(K65-J65)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J65" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K65" s="22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="24">
+      <c r="C70" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>136.5</v>
-      </c>
-      <c r="D65" s="14" t="s">
+        <v>139.5</v>
+      </c>
+      <c r="D70" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E65" s="24">
+      <c r="E70" s="24">
         <f>SUM(H:H)</f>
-        <v>35.5</v>
-      </c>
-      <c r="F65" s="14" t="s">
+        <v>36.5</v>
+      </c>
+      <c r="F70" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G65" s="24">
+      <c r="G70" s="24">
         <f>SUM(I:I)</f>
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2868,7 +2959,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C64" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C62 C64:C69" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Update Content Map
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41151CF-C09A-CC46-B82A-B7C65A6660C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D216F0D-D385-A541-84D0-C57B03DFB103}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="93">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -880,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2897,7 +2897,7 @@
         <v>44338</v>
       </c>
       <c r="I65" s="15">
-        <f t="shared" ref="I65:I66" si="2">ROUNDUP(((SUM(K65-J65)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I65:I67" si="2">ROUNDUP(((SUM(K65-J65)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
       <c r="J65" s="21">
@@ -2942,10 +2942,38 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
+      <c r="A67">
+        <v>18</v>
+      </c>
+      <c r="B67" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" t="s">
+        <v>89</v>
+      </c>
+      <c r="F67" s="2">
+        <v>44337</v>
+      </c>
+      <c r="G67" s="2">
+        <v>44338</v>
+      </c>
       <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
+      <c r="I67" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J67" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K67" s="22">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F68" s="2"/>
@@ -2965,7 +2993,7 @@
       </c>
       <c r="C70" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>140.25</v>
+        <v>141.25</v>
       </c>
       <c r="D70" s="14" t="s">
         <v>45</v>
@@ -2979,7 +3007,7 @@
       </c>
       <c r="G70" s="24">
         <f>SUM(I:I)</f>
-        <v>103.75</v>
+        <v>104.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Add Navigation Model and Wireframe first iteration
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0824A65A-4B17-844C-A3D5-685B8A80B1A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440D431B-AF5D-774A-BA2A-38DF34F8EC64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="31760" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="100">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -323,6 +323,18 @@
   </si>
   <si>
     <t>Folien erstellen und Vortrag üben</t>
+  </si>
+  <si>
+    <t>Navigation Map</t>
+  </si>
+  <si>
+    <t>Rudimentäre Navigationswege zeichnen</t>
+  </si>
+  <si>
+    <t>Wireframes</t>
+  </si>
+  <si>
+    <t>Navigationswege auf Wireframes darstellen</t>
   </si>
 </sst>
 </file>
@@ -887,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P77"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I76" sqref="A1:I76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2847,23 +2859,54 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>90</v>
+      </c>
+      <c r="E63" t="s">
+        <v>92</v>
+      </c>
+      <c r="F63" s="2">
+        <v>44337</v>
+      </c>
+      <c r="G63" s="2">
+        <v>44338</v>
+      </c>
+      <c r="H63" s="15">
+        <f>ROUNDUP(((SUM(K63-J63)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
       <c r="I63" s="15"/>
+      <c r="J63" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K63" s="22">
+        <v>0.41666666666666669</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B64" t="s">
         <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E64" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F64" s="2">
         <v>44337</v>
@@ -2871,21 +2914,20 @@
       <c r="G64" s="2">
         <v>44338</v>
       </c>
-      <c r="H64" s="15">
-        <f>ROUNDUP(((SUM(K64-J64)*24*60/60)/0.25),0)*0.25</f>
-        <v>1</v>
-      </c>
-      <c r="I64" s="15"/>
+      <c r="I64" s="15">
+        <f t="shared" ref="I64:I67" si="2">ROUNDUP(((SUM(K64-J64)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
       <c r="J64" s="21">
-        <v>0.375</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="K64" s="22">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
@@ -2894,10 +2936,10 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E65" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="F65" s="2">
         <v>44337</v>
@@ -2905,20 +2947,21 @@
       <c r="G65" s="2">
         <v>44338</v>
       </c>
+      <c r="H65" s="15"/>
       <c r="I65" s="15">
-        <f t="shared" ref="I65:I68" si="2">ROUNDUP(((SUM(K65-J65)*24*60/60)/0.25),0)*0.25</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>0.75</v>
       </c>
       <c r="J65" s="21">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="K65" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.57291666666666663</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B66" t="s">
         <v>70</v>
@@ -2927,10 +2970,10 @@
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="E66" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F66" s="2">
         <v>44337</v>
@@ -2941,16 +2984,16 @@
       <c r="H66" s="15"/>
       <c r="I66" s="15">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J66" s="21">
-        <v>0.54166666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="K66" s="22">
-        <v>0.57291666666666663</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>18</v>
       </c>
@@ -2967,7 +3010,7 @@
         <v>89</v>
       </c>
       <c r="F67" s="2">
-        <v>44337</v>
+        <v>44338</v>
       </c>
       <c r="G67" s="2">
         <v>44338</v>
@@ -2975,70 +3018,78 @@
       <c r="H67" s="15"/>
       <c r="I67" s="15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J67" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K67" s="22">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K67" s="22">
+      <c r="L67" s="31">
+        <f>SUM(H59:I67)</f>
+        <v>22.75</v>
+      </c>
+      <c r="M67">
+        <f>SUM(L67+16)</f>
+        <v>38.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>17</v>
+      </c>
+      <c r="B69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" t="s">
+        <v>94</v>
+      </c>
+      <c r="E69" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="2">
+        <v>44341</v>
+      </c>
+      <c r="G69" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H69" s="15">
+        <f>ROUNDUP(((SUM(K69-J69)*24*60/60)/0.25),0)*0.25</f>
+        <v>6</v>
+      </c>
+      <c r="I69" s="15"/>
+      <c r="J69" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K69" s="22">
         <v>0.625</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>18</v>
-      </c>
-      <c r="B68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" t="s">
-        <v>87</v>
-      </c>
-      <c r="E68" t="s">
-        <v>89</v>
-      </c>
-      <c r="F68" s="2">
-        <v>44338</v>
-      </c>
-      <c r="G68" s="2">
-        <v>44338</v>
-      </c>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="J68" s="21">
-        <v>0.375</v>
-      </c>
-      <c r="K68" s="22">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B70" t="s">
         <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E70" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F70" s="2">
         <v>44341</v>
@@ -3046,75 +3097,97 @@
       <c r="G70" s="2">
         <v>44359</v>
       </c>
-      <c r="H70" s="15">
-        <f>ROUNDUP(((SUM(K70-J70)*24*60/60)/0.25),0)*0.25</f>
-        <v>6</v>
-      </c>
-      <c r="I70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15">
+        <f t="shared" ref="I70:I71" si="3">ROUNDUP(((SUM(K70-J70)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.25</v>
+      </c>
       <c r="J70" s="21">
-        <v>0.375</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K70" s="22">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
+        <v>0.71875</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>98</v>
+      </c>
+      <c r="E71" t="s">
+        <v>99</v>
+      </c>
+      <c r="F71" s="2">
+        <v>44341</v>
+      </c>
+      <c r="G71" s="2">
+        <v>44359</v>
+      </c>
       <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I71" s="15">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
+      <c r="J71" s="21">
+        <v>0.71875</v>
+      </c>
+      <c r="K71" s="22">
+        <v>0.77083333333333337</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="15"/>
       <c r="I72" s="15"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="15"/>
       <c r="I75" s="15"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="15"/>
-      <c r="I76" s="15"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="1" t="s">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B76" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C77" s="24">
+      <c r="C76" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>152.25</v>
-      </c>
-      <c r="D77" s="14" t="s">
+        <v>154.75</v>
+      </c>
+      <c r="D76" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E77" s="24">
+      <c r="E76" s="24">
         <f>SUM(H:H)</f>
         <v>42.5</v>
       </c>
-      <c r="F77" s="14" t="s">
+      <c r="F76" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G77" s="24">
+      <c r="G76" s="24">
         <f>SUM(I:I)</f>
-        <v>109.75</v>
+        <v>112.25</v>
       </c>
     </row>
   </sheetData>
@@ -3122,7 +3195,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C62 C64:C76" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C75" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[SEMINAR][FEATURE] Add vorlagen and tipps and tricks to latex
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84D62FB-E9AC-2D45-B526-C3EA0C907131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE4CA91-4D58-A741-B03A-F7B9E8D94F73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="111">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -362,6 +362,12 @@
   </si>
   <si>
     <t>Farbschema, Schriftart, Moodboard</t>
+  </si>
+  <si>
+    <t>LaTex Workshop</t>
+  </si>
+  <si>
+    <t>How to LaTex</t>
   </si>
 </sst>
 </file>
@@ -926,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="K83" sqref="K83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3494,7 +3500,7 @@
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="15">
-        <f t="shared" ref="I82" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I82:I83" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
         <v>5.25</v>
       </c>
       <c r="J82" s="21">
@@ -3505,30 +3511,64 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="15"/>
+      <c r="A83">
+        <v>17</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" t="s">
+        <v>109</v>
+      </c>
+      <c r="E83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83" s="2">
+        <v>44355</v>
+      </c>
+      <c r="G83" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H83" s="15">
+        <f>ROUNDUP(((SUM(K83-J83)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.75</v>
+      </c>
       <c r="I83" s="15"/>
+      <c r="J83" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K83" s="22">
+        <v>0.53125</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B84" s="1" t="s">
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="24">
+      <c r="C85" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>184.25</v>
-      </c>
-      <c r="D84" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D85" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E84" s="24">
+      <c r="E85" s="24">
         <f>SUM(H:H)</f>
-        <v>46.75</v>
-      </c>
-      <c r="F84" s="14" t="s">
+        <v>49.5</v>
+      </c>
+      <c r="F85" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G84" s="24">
+      <c r="G85" s="24">
         <f>SUM(I:I)</f>
         <v>137.5</v>
       </c>
@@ -3538,7 +3578,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C83" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C84" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add and update recipe moodboard and typography
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE4CA91-4D58-A741-B03A-F7B9E8D94F73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003984AF-E58C-414C-AE17-EC0E6B70FD14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="111">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -932,10 +932,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="K83" sqref="K83"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="15">
-        <f t="shared" ref="I82:I83" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I82:I84" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
         <v>5.25</v>
       </c>
       <c r="J82" s="21">
@@ -3545,32 +3545,66 @@
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
+      <c r="A84">
+        <v>22</v>
+      </c>
+      <c r="B84" t="s">
+        <v>93</v>
+      </c>
+      <c r="C84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" t="s">
+        <v>107</v>
+      </c>
+      <c r="E84" t="s">
+        <v>108</v>
+      </c>
+      <c r="F84" s="2">
+        <v>44355</v>
+      </c>
+      <c r="G84" s="2">
+        <v>44359</v>
+      </c>
       <c r="H84" s="15"/>
-      <c r="I84" s="15"/>
+      <c r="I84" s="15">
+        <f t="shared" si="5"/>
+        <v>6.5</v>
+      </c>
+      <c r="J84" s="21">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K84" s="22">
+        <v>0.82291666666666663</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B85" s="1" t="s">
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B86" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="24">
+      <c r="C86" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>187</v>
-      </c>
-      <c r="D85" s="14" t="s">
+        <v>193.5</v>
+      </c>
+      <c r="D86" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E85" s="24">
+      <c r="E86" s="24">
         <f>SUM(H:H)</f>
         <v>49.5</v>
       </c>
-      <c r="F85" s="14" t="s">
+      <c r="F86" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G85" s="24">
+      <c r="G86" s="24">
         <f>SUM(I:I)</f>
-        <v>137.5</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3578,7 +3612,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C84" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C85" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add interview results for typography
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003984AF-E58C-414C-AE17-EC0E6B70FD14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7072AA8-8D2F-9C4F-80B8-0425C2D02DCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17060" yWindow="460" windowWidth="34140" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="113">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Schreibwerkstatt</t>
   </si>
   <si>
-    <t>Abschlussvorträge und Fragen stellen</t>
-  </si>
-  <si>
     <t>Expose überarbeiten</t>
   </si>
   <si>
@@ -307,15 +304,6 @@
     <t>Content Map iterieren</t>
   </si>
   <si>
-    <t>Peer reviewed Exposé</t>
-  </si>
-  <si>
-    <t>Exposé vorstellen</t>
-  </si>
-  <si>
-    <t>Exposé reviewen</t>
-  </si>
-  <si>
     <t>Interface Design</t>
   </si>
   <si>
@@ -328,9 +316,6 @@
     <t>Navigation Map</t>
   </si>
   <si>
-    <t>Rudimentäre Navigationswege zeichnen</t>
-  </si>
-  <si>
     <t>Wireframes</t>
   </si>
   <si>
@@ -343,9 +328,6 @@
     <t>Verbesserungen</t>
   </si>
   <si>
-    <t>Vorträge hören und selber halten</t>
-  </si>
-  <si>
     <t>Domaenenmodell überarbeiten</t>
   </si>
   <si>
@@ -368,13 +350,37 @@
   </si>
   <si>
     <t>How to LaTex</t>
+  </si>
+  <si>
+    <t>Typografie</t>
+  </si>
+  <si>
+    <t>Typografie Umfrage auswertung</t>
+  </si>
+  <si>
+    <t>Abschlussvortraege und Fragen stellen</t>
+  </si>
+  <si>
+    <t>Peer reviewed Expose</t>
+  </si>
+  <si>
+    <t>Expose vorstellen</t>
+  </si>
+  <si>
+    <t>Expose reviewen</t>
+  </si>
+  <si>
+    <t>Rudimentaere Navigationswege zeichnen</t>
+  </si>
+  <si>
+    <t>Vortraege hoeren und selber halten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -393,6 +399,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -559,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -618,6 +631,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -932,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2556,7 +2570,7 @@
         <v>79</v>
       </c>
       <c r="E52" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="F52" s="2">
         <v>44327</v>
@@ -2587,10 +2601,10 @@
         <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F53" s="2">
         <v>44327</v>
@@ -2621,10 +2635,10 @@
         <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F54" s="2">
         <v>44329</v>
@@ -2655,10 +2669,10 @@
         <v>38</v>
       </c>
       <c r="D55" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" t="s">
         <v>82</v>
-      </c>
-      <c r="E55" t="s">
-        <v>83</v>
       </c>
       <c r="F55" s="2">
         <v>44331</v>
@@ -2689,10 +2703,10 @@
         <v>12</v>
       </c>
       <c r="D56" t="s">
+        <v>83</v>
+      </c>
+      <c r="E56" t="s">
         <v>84</v>
-      </c>
-      <c r="E56" t="s">
-        <v>85</v>
       </c>
       <c r="F56" s="2">
         <v>44331</v>
@@ -2722,10 +2736,10 @@
         <v>6</v>
       </c>
       <c r="D57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="2">
         <v>44332</v>
@@ -2769,10 +2783,10 @@
         <v>12</v>
       </c>
       <c r="D59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" t="s">
         <v>87</v>
-      </c>
-      <c r="E59" t="s">
-        <v>88</v>
       </c>
       <c r="F59" s="2">
         <v>44333</v>
@@ -2802,10 +2816,10 @@
         <v>6</v>
       </c>
       <c r="D60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F60" s="2">
         <v>44333</v>
@@ -2835,10 +2849,10 @@
         <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E61" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="F61" s="2">
         <v>44334</v>
@@ -2869,10 +2883,10 @@
         <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F62" s="2">
         <v>44334</v>
@@ -2902,10 +2916,10 @@
         <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F63" s="2">
         <v>44337</v>
@@ -2936,10 +2950,10 @@
         <v>6</v>
       </c>
       <c r="D64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F64" s="2">
         <v>44337</v>
@@ -3003,10 +3017,10 @@
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F66" s="2">
         <v>44337</v>
@@ -3037,10 +3051,10 @@
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E67" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F67" s="2">
         <v>44338</v>
@@ -3079,16 +3093,16 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E69" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F69" s="2">
         <v>44341</v>
@@ -3113,16 +3127,16 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
         <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E70" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="F70" s="2">
         <v>44341</v>
@@ -3147,16 +3161,16 @@
         <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
         <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E71" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F71" s="2">
         <v>44341</v>
@@ -3181,16 +3195,16 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C72" t="s">
         <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E72" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F72" s="2">
         <v>44344</v>
@@ -3229,16 +3243,16 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
         <v>12</v>
       </c>
       <c r="D74" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E74" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F74" s="2">
         <v>44347</v>
@@ -3263,16 +3277,16 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C75" t="s">
         <v>38</v>
       </c>
       <c r="D75" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E75" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F75" s="2">
         <v>44347</v>
@@ -3297,16 +3311,16 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+      <c r="D76" t="s">
         <v>93</v>
       </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" t="s">
-        <v>98</v>
-      </c>
       <c r="E76" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F76" s="2">
         <v>44347</v>
@@ -3331,16 +3345,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
         <v>38</v>
       </c>
       <c r="D77" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E77" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F77" s="2">
         <v>44348</v>
@@ -3365,16 +3379,16 @@
         <v>23</v>
       </c>
       <c r="B78" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E78" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="F78" s="2">
         <v>44348</v>
@@ -3399,16 +3413,16 @@
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
       </c>
       <c r="D79" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E79" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F79" s="2">
         <v>44350</v>
@@ -3442,21 +3456,21 @@
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E81" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="F81" s="2">
         <v>44354</v>
@@ -3476,21 +3490,21 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C82" t="s">
         <v>12</v>
       </c>
       <c r="D82" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E82" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F82" s="2">
         <v>44354</v>
@@ -3500,7 +3514,7 @@
       </c>
       <c r="H82" s="15"/>
       <c r="I82" s="15">
-        <f t="shared" ref="I82:I84" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I82:I86" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
         <v>5.25</v>
       </c>
       <c r="J82" s="21">
@@ -3510,21 +3524,21 @@
         <v>0.76736111111111116</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C83" t="s">
         <v>38</v>
       </c>
       <c r="D83" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E83" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F83" s="2">
         <v>44355</v>
@@ -3544,21 +3558,21 @@
         <v>0.53125</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C84" t="s">
         <v>12</v>
       </c>
       <c r="D84" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E84" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F84" s="2">
         <v>44355</v>
@@ -3578,33 +3592,121 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="32">
+        <v>22</v>
+      </c>
+      <c r="B85" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F85" s="2">
+        <v>44358</v>
+      </c>
+      <c r="G85" s="2">
+        <v>44359</v>
+      </c>
       <c r="H85" s="15"/>
-      <c r="I85" s="15"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B86" s="1" t="s">
+      <c r="I85" s="15">
+        <f t="shared" si="5"/>
+        <v>5.75</v>
+      </c>
+      <c r="J85" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K85" s="22">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="32">
+        <v>22</v>
+      </c>
+      <c r="B86" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E86" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="F86" s="2">
+        <v>44359</v>
+      </c>
+      <c r="G86" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J86" s="21">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K86" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="L86" s="31">
+        <f>SUM(H81:I86)</f>
+        <v>25.5</v>
+      </c>
+      <c r="M86">
+        <f>SUM(L86+16)</f>
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C86" s="24">
+      <c r="C90" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>193.5</v>
-      </c>
-      <c r="D86" s="14" t="s">
+        <v>201.25</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E86" s="24">
+      <c r="E90" s="24">
         <f>SUM(H:H)</f>
         <v>49.5</v>
       </c>
-      <c r="F86" s="14" t="s">
+      <c r="F90" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G86" s="24">
+      <c r="G90" s="24">
         <f>SUM(I:I)</f>
-        <v>144</v>
+        <v>151.75</v>
       </c>
     </row>
   </sheetData>
@@ -3612,7 +3714,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C85" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C89" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add new recipe template
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAAB03A-1AA6-3149-93F0-A8FFFF97A02C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178E4E1-450C-4C46-91F5-D6948A577335}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="120">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -386,6 +386,15 @@
   </si>
   <si>
     <t>Typography und Color Scheme</t>
+  </si>
+  <si>
+    <t>Neue Umfrage</t>
+  </si>
+  <si>
+    <t>Design iterationen</t>
+  </si>
+  <si>
+    <t>Umfrage auswertung &amp; Design iterationen</t>
   </si>
 </sst>
 </file>
@@ -958,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3778,7 +3787,7 @@
       </c>
       <c r="H90" s="15"/>
       <c r="I90" s="15">
-        <f t="shared" ref="I90:I91" si="7">ROUNDUP(((SUM(K90-J90)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I90:I92" si="7">ROUNDUP(((SUM(K90-J90)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
       <c r="J90" s="21">
@@ -3823,38 +3832,182 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
+      <c r="A92" s="32">
+        <v>22</v>
+      </c>
+      <c r="B92" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E92" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F92" s="2">
+        <v>44365</v>
+      </c>
+      <c r="G92" s="2">
+        <v>44359</v>
+      </c>
       <c r="H92" s="15"/>
-      <c r="I92" s="15"/>
+      <c r="I92" s="15">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="J92" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K92" s="22">
+        <v>0.58333333333333337</v>
+      </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
+      <c r="A93" s="32">
+        <v>22</v>
+      </c>
+      <c r="B93" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C93" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E93" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="F93" s="2">
+        <v>44365</v>
+      </c>
+      <c r="G93" s="2">
+        <v>44359</v>
+      </c>
       <c r="H93" s="15"/>
-      <c r="I93" s="15"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B94" s="1" t="s">
+      <c r="I93" s="15">
+        <f t="shared" ref="I93" si="8">ROUNDUP(((SUM(K93-J93)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J93" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K93" s="22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="32">
+        <v>22</v>
+      </c>
+      <c r="B94" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F94" s="2">
+        <v>44366</v>
+      </c>
+      <c r="G94" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15">
+        <f t="shared" ref="I94" si="9">ROUNDUP(((SUM(K94-J94)*24*60/60)/0.25),0)*0.25</f>
+        <v>3</v>
+      </c>
+      <c r="J94" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K94" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="L94" s="31">
+        <f>SUM(H89:I94)</f>
+        <v>17.5</v>
+      </c>
+      <c r="M94">
+        <f>SUM(L94+16)</f>
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="32">
+        <v>22</v>
+      </c>
+      <c r="B96" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F96" s="2">
+        <v>44368</v>
+      </c>
+      <c r="G96" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15">
+        <f t="shared" ref="I96" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
         <v>9</v>
       </c>
-      <c r="C94" s="24">
+      <c r="J96" s="21">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K96" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B98" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C98" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>210.25</v>
-      </c>
-      <c r="D94" s="14" t="s">
+        <v>229.25</v>
+      </c>
+      <c r="D98" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E94" s="24">
+      <c r="E98" s="24">
         <f>SUM(H:H)</f>
         <v>51</v>
       </c>
-      <c r="F94" s="14" t="s">
+      <c r="F98" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G94" s="24">
+      <c r="G98" s="24">
         <f>SUM(I:I)</f>
-        <v>159.25</v>
+        <v>178.25</v>
       </c>
     </row>
   </sheetData>
@@ -3862,7 +4015,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C93" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C97" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add algorithm structure for recommendation and similar recipes
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178E4E1-450C-4C46-91F5-D6948A577335}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D964BAC8-9C3E-A24F-94CC-7281F3B905A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="122">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Schreibwerkstatt</t>
   </si>
   <si>
-    <t>Expose überarbeiten</t>
-  </si>
-  <si>
     <t>Peer Reviewed Expose</t>
   </si>
   <si>
@@ -310,9 +307,6 @@
     <t>Kurzvortrag</t>
   </si>
   <si>
-    <t>Folien erstellen und Vortrag üben</t>
-  </si>
-  <si>
     <t>Navigation Map</t>
   </si>
   <si>
@@ -322,15 +316,9 @@
     <t>Navigationswege auf Wireframes darstellen</t>
   </si>
   <si>
-    <t>Vortrag üben</t>
-  </si>
-  <si>
     <t>Verbesserungen</t>
   </si>
   <si>
-    <t>Domaenenmodell überarbeiten</t>
-  </si>
-  <si>
     <t>Iteration eins</t>
   </si>
   <si>
@@ -376,9 +364,6 @@
     <t>Vortraege hoeren und selber halten</t>
   </si>
   <si>
-    <t>Abschlussvortrag hören und Open Space</t>
-  </si>
-  <si>
     <t>Guidelines vergleichen</t>
   </si>
   <si>
@@ -395,6 +380,27 @@
   </si>
   <si>
     <t>Umfrage auswertung &amp; Design iterationen</t>
+  </si>
+  <si>
+    <t>Pseudo Code</t>
+  </si>
+  <si>
+    <t>Expose ueberarbeiten</t>
+  </si>
+  <si>
+    <t>Folien erstellen und Vortrag ueben</t>
+  </si>
+  <si>
+    <t>Vortrag ueben</t>
+  </si>
+  <si>
+    <t>Domaenenmodell ueberarbeiten</t>
+  </si>
+  <si>
+    <t>Algorithmus fuer Empfehlungen und Aehnliche Rezepte</t>
+  </si>
+  <si>
+    <t>Abschlussvortrag hoeren und Open Space</t>
   </si>
 </sst>
 </file>
@@ -967,19 +973,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="J97" sqref="J97"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="44.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
@@ -998,10 +1004,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>23</v>
@@ -1042,10 +1048,10 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
         <v>50</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>54</v>
@@ -1072,10 +1078,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -1104,10 +1110,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>24</v>
@@ -1136,10 +1142,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
         <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -1168,10 +1174,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
         <v>7</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
@@ -1201,6 +1207,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="13"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="L7" s="7"/>
@@ -1214,10 +1221,10 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -1241,10 +1248,10 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
       <c r="E9" t="s">
         <v>30</v>
@@ -1267,10 +1274,10 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
         <v>29</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
@@ -1294,10 +1301,10 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -1331,10 +1338,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
         <v>7</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E12" t="s">
         <v>34</v>
@@ -1368,10 +1375,10 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -1402,10 +1409,10 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
       </c>
       <c r="E14" t="s">
         <v>40</v>
@@ -1436,10 +1443,10 @@
         <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" t="s">
         <v>35</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E15" t="s">
         <v>47</v>
@@ -1469,10 +1476,10 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
         <v>35</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>48</v>
@@ -1503,10 +1510,10 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" t="s">
         <v>35</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -1536,10 +1543,10 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
         <v>29</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E18" t="s">
         <v>31</v>
@@ -1569,10 +1576,10 @@
         <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" t="s">
         <v>29</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
@@ -1596,6 +1603,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="13"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="I20" s="15"/>
@@ -1609,10 +1617,10 @@
         <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
         <v>29</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>31</v>
@@ -1642,10 +1650,10 @@
         <v>36</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" t="s">
         <v>50</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E22" t="s">
         <v>51</v>
@@ -1668,10 +1676,10 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" t="s">
         <v>50</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E23" t="s">
         <v>52</v>
@@ -1702,10 +1710,10 @@
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
         <v>50</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E24" t="s">
         <v>54</v>
@@ -1736,10 +1744,10 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
         <v>50</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E25" t="s">
         <v>53</v>
@@ -1769,10 +1777,10 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>55</v>
       </c>
       <c r="E26" t="s">
         <v>56</v>
@@ -1803,10 +1811,10 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>57</v>
       </c>
       <c r="E27" t="s">
         <v>57</v>
@@ -1837,10 +1845,10 @@
         <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" t="s">
         <v>29</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E28" t="s">
         <v>49</v>
@@ -1870,10 +1878,10 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
         <v>29</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E29" t="s">
         <v>58</v>
@@ -1903,10 +1911,10 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>29</v>
       </c>
       <c r="E30" t="s">
         <v>59</v>
@@ -1937,6 +1945,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="13"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="I31" s="15"/>
@@ -1952,10 +1961,10 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>29</v>
       </c>
       <c r="E32" t="s">
         <v>60</v>
@@ -1985,10 +1994,10 @@
         <v>36</v>
       </c>
       <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>63</v>
       </c>
       <c r="E33" t="s">
         <v>64</v>
@@ -2018,10 +2027,10 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D34" t="s">
-        <v>35</v>
       </c>
       <c r="E34" t="s">
         <v>65</v>
@@ -2051,10 +2060,10 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D35" t="s">
-        <v>57</v>
       </c>
       <c r="E35" t="s">
         <v>66</v>
@@ -2084,10 +2093,10 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>38</v>
-      </c>
-      <c r="D36" t="s">
-        <v>57</v>
       </c>
       <c r="E36" t="s">
         <v>67</v>
@@ -2117,10 +2126,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D37" t="s">
-        <v>29</v>
       </c>
       <c r="E37" t="s">
         <v>68</v>
@@ -2151,10 +2160,10 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
         <v>35</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>69</v>
@@ -2185,10 +2194,10 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
         <v>35</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E39" t="s">
         <v>52</v>
@@ -2220,6 +2229,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D40" s="13"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="15"/>
@@ -2236,10 +2246,10 @@
         <v>70</v>
       </c>
       <c r="C41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D41" t="s">
-        <v>71</v>
       </c>
       <c r="E41" t="s">
         <v>72</v>
@@ -2270,10 +2280,10 @@
         <v>70</v>
       </c>
       <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="D42" t="s">
-        <v>71</v>
       </c>
       <c r="E42" t="s">
         <v>73</v>
@@ -2304,10 +2314,10 @@
         <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
         <v>71</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E43" t="s">
         <v>74</v>
@@ -2338,10 +2348,10 @@
         <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
         <v>71</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E44" t="s">
         <v>75</v>
@@ -2372,10 +2382,10 @@
         <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" t="s">
         <v>71</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E45" t="s">
         <v>75</v>
@@ -2406,10 +2416,10 @@
         <v>70</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" t="s">
         <v>71</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E46" t="s">
         <v>76</v>
@@ -2440,10 +2450,10 @@
         <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
         <v>71</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E47" t="s">
         <v>77</v>
@@ -2474,10 +2484,10 @@
         <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" t="s">
         <v>71</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E48" t="s">
         <v>78</v>
@@ -2508,10 +2518,10 @@
         <v>70</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" t="s">
         <v>71</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E49" t="s">
         <v>78</v>
@@ -2543,6 +2553,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D50" s="13"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="15"/>
@@ -2558,10 +2569,10 @@
         <v>70</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
-      </c>
-      <c r="D51" t="s">
         <v>71</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="F51" s="2">
         <v>44326</v>
@@ -2585,13 +2596,13 @@
         <v>70</v>
       </c>
       <c r="C52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D52" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D52" t="s">
-        <v>79</v>
-      </c>
       <c r="E52" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F52" s="2">
         <v>44327</v>
@@ -2619,13 +2630,13 @@
         <v>70</v>
       </c>
       <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D53" t="s">
-        <v>81</v>
-      </c>
       <c r="E53" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F53" s="2">
         <v>44327</v>
@@ -2653,13 +2664,13 @@
         <v>70</v>
       </c>
       <c r="C54" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D54" t="s">
-        <v>81</v>
-      </c>
       <c r="E54" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="F54" s="2">
         <v>44329</v>
@@ -2687,13 +2698,13 @@
         <v>70</v>
       </c>
       <c r="C55" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>81</v>
-      </c>
-      <c r="E55" t="s">
-        <v>82</v>
       </c>
       <c r="F55" s="2">
         <v>44331</v>
@@ -2721,13 +2732,13 @@
         <v>70</v>
       </c>
       <c r="C56" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>83</v>
-      </c>
-      <c r="E56" t="s">
-        <v>84</v>
       </c>
       <c r="F56" s="2">
         <v>44331</v>
@@ -2754,13 +2765,13 @@
         <v>70</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F57" s="2">
         <v>44332</v>
@@ -2788,6 +2799,7 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D58" s="13"/>
       <c r="G58" s="2"/>
       <c r="I58" s="15"/>
       <c r="J58" s="21"/>
@@ -2801,13 +2813,13 @@
         <v>70</v>
       </c>
       <c r="C59" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>86</v>
-      </c>
-      <c r="E59" t="s">
-        <v>87</v>
       </c>
       <c r="F59" s="2">
         <v>44333</v>
@@ -2834,13 +2846,13 @@
         <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F60" s="2">
         <v>44333</v>
@@ -2867,13 +2879,13 @@
         <v>70</v>
       </c>
       <c r="C61" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D61" t="s">
-        <v>108</v>
-      </c>
       <c r="E61" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F61" s="2">
         <v>44334</v>
@@ -2901,13 +2913,13 @@
         <v>70</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F62" s="2">
         <v>44334</v>
@@ -2934,13 +2946,13 @@
         <v>70</v>
       </c>
       <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D63" t="s">
-        <v>108</v>
-      </c>
       <c r="E63" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F63" s="2">
         <v>44337</v>
@@ -2968,13 +2980,13 @@
         <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F64" s="2">
         <v>44337</v>
@@ -3001,10 +3013,10 @@
         <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" t="s">
         <v>71</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E65" t="s">
         <v>77</v>
@@ -3035,13 +3047,13 @@
         <v>70</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F66" s="2">
         <v>44337</v>
@@ -3069,13 +3081,13 @@
         <v>70</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F67" s="2">
         <v>44338</v>
@@ -3104,6 +3116,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D68" s="13"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="15"/>
@@ -3114,16 +3127,16 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
         <v>89</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D69" t="s">
-        <v>90</v>
-      </c>
       <c r="E69" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="F69" s="2">
         <v>44341</v>
@@ -3148,16 +3161,16 @@
         <v>19</v>
       </c>
       <c r="B70" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C70" t="s">
+        <v>90</v>
+      </c>
+      <c r="D70" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D70" t="s">
-        <v>92</v>
-      </c>
       <c r="E70" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F70" s="2">
         <v>44341</v>
@@ -3182,16 +3195,16 @@
         <v>19</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71" t="s">
+        <v>91</v>
+      </c>
+      <c r="D71" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D71" t="s">
-        <v>93</v>
-      </c>
       <c r="E71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F71" s="2">
         <v>44341</v>
@@ -3216,16 +3229,16 @@
         <v>19</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C72" t="s">
+        <v>91</v>
+      </c>
+      <c r="D72" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D72" t="s">
-        <v>93</v>
-      </c>
       <c r="E72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F72" s="2">
         <v>44344</v>
@@ -3254,6 +3267,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D73" s="13"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="15"/>
@@ -3264,16 +3278,16 @@
         <v>19</v>
       </c>
       <c r="B74" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74" t="s">
+        <v>91</v>
+      </c>
+      <c r="D74" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D74" t="s">
-        <v>93</v>
-      </c>
       <c r="E74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F74" s="2">
         <v>44347</v>
@@ -3298,16 +3312,16 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
         <v>89</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D75" t="s">
-        <v>90</v>
-      </c>
       <c r="E75" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="F75" s="2">
         <v>44347</v>
@@ -3332,16 +3346,16 @@
         <v>19</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
         <v>93</v>
-      </c>
-      <c r="E76" t="s">
-        <v>96</v>
       </c>
       <c r="F76" s="2">
         <v>44347</v>
@@ -3366,16 +3380,16 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" t="s">
         <v>89</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D77" t="s">
-        <v>90</v>
-      </c>
       <c r="E77" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F77" s="2">
         <v>44348</v>
@@ -3400,16 +3414,16 @@
         <v>23</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
-      </c>
-      <c r="D78" t="s">
-        <v>97</v>
+        <v>119</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F78" s="2">
         <v>44348</v>
@@ -3434,16 +3448,16 @@
         <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" t="s">
-        <v>97</v>
+        <v>119</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E79" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F79" s="2">
         <v>44350</v>
@@ -3472,6 +3486,7 @@
       </c>
     </row>
     <row r="80" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D80" s="13"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="15"/>
@@ -3482,16 +3497,16 @@
         <v>23</v>
       </c>
       <c r="B81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" t="s">
-        <v>97</v>
+        <v>119</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E81" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F81" s="2">
         <v>44354</v>
@@ -3516,16 +3531,16 @@
         <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C82" t="s">
+        <v>97</v>
+      </c>
+      <c r="D82" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D82" t="s">
-        <v>101</v>
-      </c>
       <c r="E82" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F82" s="2">
         <v>44354</v>
@@ -3550,16 +3565,16 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C83" t="s">
+        <v>99</v>
+      </c>
+      <c r="D83" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D83" t="s">
-        <v>103</v>
-      </c>
       <c r="E83" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F83" s="2">
         <v>44355</v>
@@ -3584,16 +3599,16 @@
         <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C84" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D84" t="s">
-        <v>101</v>
-      </c>
       <c r="E84" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F84" s="2">
         <v>44355</v>
@@ -3618,16 +3633,16 @@
         <v>22</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C85" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C85" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D85" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="32" t="s">
         <v>101</v>
-      </c>
-      <c r="E85" s="32" t="s">
-        <v>105</v>
       </c>
       <c r="F85" s="2">
         <v>44358</v>
@@ -3652,16 +3667,16 @@
         <v>22</v>
       </c>
       <c r="B86" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C86" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D86" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E86" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F86" s="2">
         <v>44359</v>
@@ -3690,6 +3705,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D87" s="13"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="15"/>
@@ -3700,16 +3716,16 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C88" t="s">
+        <v>121</v>
+      </c>
+      <c r="D88" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D88" t="s">
-        <v>113</v>
-      </c>
       <c r="E88" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="F88" s="2">
         <v>44362</v>
@@ -3734,16 +3750,16 @@
         <v>22</v>
       </c>
       <c r="B89" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C89" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F89" s="2">
         <v>44362</v>
@@ -3768,16 +3784,16 @@
         <v>22</v>
       </c>
       <c r="B90" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C90" t="s">
-        <v>6</v>
-      </c>
-      <c r="D90" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C90" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F90" s="2">
         <v>44362</v>
@@ -3802,16 +3818,16 @@
         <v>22</v>
       </c>
       <c r="B91" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C91" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C91" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F91" s="2">
         <v>44362</v>
@@ -3836,16 +3852,16 @@
         <v>22</v>
       </c>
       <c r="B92" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C92" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C92" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F92" s="2">
         <v>44365</v>
@@ -3870,16 +3886,16 @@
         <v>22</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C93" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C93" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F93" s="2">
         <v>44365</v>
@@ -3904,16 +3920,16 @@
         <v>22</v>
       </c>
       <c r="B94" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C94" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C94" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D94" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F94" s="2">
         <v>44366</v>
@@ -3942,6 +3958,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D95" s="13"/>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="15"/>
@@ -3952,16 +3969,16 @@
         <v>22</v>
       </c>
       <c r="B96" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="C96" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="32" t="s">
-        <v>101</v>
+        <v>88</v>
+      </c>
+      <c r="C96" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D96" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F96" s="2">
         <v>44368</v>
@@ -3971,7 +3988,7 @@
       </c>
       <c r="H96" s="15"/>
       <c r="I96" s="15">
-        <f t="shared" ref="I96" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I96:I98" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
         <v>9</v>
       </c>
       <c r="J96" s="21">
@@ -3981,41 +3998,111 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="15"/>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>17</v>
+      </c>
+      <c r="B97" t="s">
+        <v>88</v>
+      </c>
+      <c r="C97" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E97" t="s">
+        <v>121</v>
+      </c>
+      <c r="F97" s="2">
+        <v>44369</v>
+      </c>
+      <c r="G97" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H97" s="15">
+        <f>ROUNDUP(((SUM(K97-J97)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
       <c r="I97" s="15"/>
-    </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B98" s="1" t="s">
+      <c r="J97" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K97" s="22">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="32">
+        <v>21</v>
+      </c>
+      <c r="B98" t="s">
+        <v>88</v>
+      </c>
+      <c r="C98" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D98" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F98" s="2">
+        <v>44369</v>
+      </c>
+      <c r="G98" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="J98" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K98" s="22">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="21"/>
+      <c r="K99" s="22"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="24">
+      <c r="C100" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>229.25</v>
-      </c>
-      <c r="D98" s="14" t="s">
+        <v>235.75</v>
+      </c>
+      <c r="D100" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E98" s="24">
+      <c r="E100" s="24">
         <f>SUM(H:H)</f>
-        <v>51</v>
-      </c>
-      <c r="F98" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F100" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G98" s="24">
+      <c r="G100" s="24">
         <f>SUM(I:I)</f>
-        <v>178.25</v>
+        <v>180.75</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C4:C12 C18:C21 C28:C34 C37:C40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="C2:C3 C13:C17 C22:C27 C35:C36 C41:C97" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D99" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add pseudo code
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D964BAC8-9C3E-A24F-94CC-7281F3B905A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61379E0-2E79-B54E-9485-E90D982BA404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="125">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -401,6 +401,15 @@
   </si>
   <si>
     <t>Abschlussvortrag hoeren und Open Space</t>
+  </si>
+  <si>
+    <t>Erklaerung der Struktur</t>
+  </si>
+  <si>
+    <t>Pseudocode fuer Aehnliche Rezepte</t>
+  </si>
+  <si>
+    <t>Pseudocode fuer Empfohlene Rezepte</t>
   </si>
 </sst>
 </file>
@@ -973,10 +982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3988,7 +3997,7 @@
       </c>
       <c r="H96" s="15"/>
       <c r="I96" s="15">
-        <f t="shared" ref="I96:I98" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I96:I100" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
         <v>9</v>
       </c>
       <c r="J96" s="21">
@@ -4067,34 +4076,144 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
+      <c r="A99" s="32">
+        <v>21</v>
+      </c>
+      <c r="B99" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D99" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="F99" s="2">
+        <v>44369</v>
+      </c>
+      <c r="G99" s="2">
+        <v>44359</v>
+      </c>
       <c r="H99" s="15"/>
-      <c r="I99" s="15"/>
-      <c r="J99" s="21"/>
-      <c r="K99" s="22"/>
+      <c r="I99" s="15">
+        <f t="shared" si="10"/>
+        <v>0.5</v>
+      </c>
+      <c r="J99" s="21">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="K99" s="22">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B100" s="1" t="s">
+      <c r="A100" s="32">
+        <v>22</v>
+      </c>
+      <c r="B100" t="s">
+        <v>88</v>
+      </c>
+      <c r="C100" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F100" s="2">
+        <v>44372</v>
+      </c>
+      <c r="G100" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15">
+        <f>ROUNDUP(((SUM(K100-J100)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J100" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K100" s="22">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101" s="32">
+        <v>23</v>
+      </c>
+      <c r="B101" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D101" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="F101" s="2">
+        <v>44372</v>
+      </c>
+      <c r="G101" s="2">
+        <v>44359</v>
+      </c>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15">
+        <f>ROUNDUP(((SUM(K101-J101)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J101" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K101" s="22">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J102" s="21"/>
+      <c r="K102" s="22"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
+      <c r="J103" s="21"/>
+      <c r="K103" s="22"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C100" s="24">
+      <c r="C105" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>235.75</v>
-      </c>
-      <c r="D100" s="14" t="s">
+        <v>240.25</v>
+      </c>
+      <c r="D105" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E100" s="24">
+      <c r="E105" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F100" s="14" t="s">
+      <c r="F105" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G100" s="24">
+      <c r="G105" s="24">
         <f>SUM(I:I)</f>
-        <v>180.75</v>
+        <v>185.25</v>
       </c>
     </row>
   </sheetData>
@@ -4102,7 +4221,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D99" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D103:D104 D41:D101" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add MockUps Icons Grid and Layouts
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64A70CC-7DE1-364E-B268-49A9D5223E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359F2F4E-F1F6-4B40-9516-04DD814D74A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="127">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -410,6 +410,12 @@
   </si>
   <si>
     <t>Pseudocode fuer Empfohlene Rezepte</t>
+  </si>
+  <si>
+    <t>MockUps Icons Grid und Layouts</t>
+  </si>
+  <si>
+    <t>MockUps</t>
   </si>
 </sst>
 </file>
@@ -984,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="J103" sqref="J103"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3997,7 +4003,7 @@
       </c>
       <c r="H96" s="15"/>
       <c r="I96" s="15">
-        <f t="shared" ref="I96:I100" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I96:I99" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
         <v>9</v>
       </c>
       <c r="J96" s="21">
@@ -4212,12 +4218,38 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
+      <c r="A103" s="32">
+        <v>22</v>
+      </c>
+      <c r="B103" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C103" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D103" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="F103" s="2">
+        <v>44373</v>
+      </c>
+      <c r="G103" s="2">
+        <v>44359</v>
+      </c>
       <c r="H103" s="15"/>
-      <c r="I103" s="15"/>
-      <c r="J103" s="21"/>
-      <c r="K103" s="22"/>
+      <c r="I103" s="15">
+        <f>ROUNDUP(((SUM(K103-J103)*24*60/60)/0.25),0)*0.25</f>
+        <v>8</v>
+      </c>
+      <c r="J103" s="21">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K103" s="22">
+        <v>0.79166666666666663</v>
+      </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F104" s="2"/>
@@ -4229,7 +4261,7 @@
       </c>
       <c r="C105" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>241.25</v>
+        <v>249.25</v>
       </c>
       <c r="D105" s="14" t="s">
         <v>45</v>
@@ -4243,7 +4275,7 @@
       </c>
       <c r="G105" s="24">
         <f>SUM(I:I)</f>
-        <v>186.25</v>
+        <v>194.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FEATURE] Add filter option list
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359F2F4E-F1F6-4B40-9516-04DD814D74A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4118FC9-CF7B-F04B-84A5-D7BB5B961E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="130">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>MockUps</t>
+  </si>
+  <si>
+    <t>Alle Filter Optionen Sammeln</t>
+  </si>
+  <si>
+    <t>MockUps Icons bauen</t>
+  </si>
+  <si>
+    <t>MockUps Rezept Teaser</t>
   </si>
 </sst>
 </file>
@@ -988,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P105"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4256,26 +4265,135 @@
       <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B105" s="1" t="s">
+      <c r="A105" s="32">
+        <v>22</v>
+      </c>
+      <c r="B105" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C105" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="F105" s="2">
+        <v>44375</v>
+      </c>
+      <c r="G105" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I105" s="15">
+        <f>ROUNDUP(((SUM(K105-J105)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="J105" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K105" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A106" s="32">
+        <v>22</v>
+      </c>
+      <c r="B106" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C106" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D106" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="F106" s="2">
+        <v>44376</v>
+      </c>
+      <c r="G106" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I106" s="15">
+        <f>ROUNDUP(((SUM(K106-J106)*24*60/60)/0.25),0)*0.25</f>
+        <v>6</v>
+      </c>
+      <c r="J106" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="K106" s="22">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>18</v>
+      </c>
+      <c r="B107" t="s">
+        <v>70</v>
+      </c>
+      <c r="C107" t="s">
+        <v>85</v>
+      </c>
+      <c r="D107" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" t="s">
+        <v>127</v>
+      </c>
+      <c r="F107" s="2">
+        <v>44376</v>
+      </c>
+      <c r="G107" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I107" s="15">
+        <f>ROUNDUP(((SUM(K107-J107)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="J107" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K107" s="22">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D108" s="13"/>
+      <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D109" s="13"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="24">
+      <c r="C110" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>249.25</v>
-      </c>
-      <c r="D105" s="14" t="s">
+        <v>260.5</v>
+      </c>
+      <c r="D110" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E105" s="24">
+      <c r="E110" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F105" s="14" t="s">
+      <c r="F110" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G105" s="24">
+      <c r="G110" s="24">
         <f>SUM(I:I)</f>
-        <v>194.25</v>
+        <v>205.5</v>
       </c>
     </row>
   </sheetData>
@@ -4283,7 +4401,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D104" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D109" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add new filter types and Update domainmodel
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4118FC9-CF7B-F04B-84A5-D7BB5B961E4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64650A9B-5247-5046-B0B7-47AB3EE6057E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="134">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -425,6 +425,18 @@
   </si>
   <si>
     <t>MockUps Rezept Teaser</t>
+  </si>
+  <si>
+    <t>Filterarten bestimmen und konzipieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget: </t>
+  </si>
+  <si>
+    <t>Kredits erreicht:</t>
+  </si>
+  <si>
+    <t>Kredits erfordert:</t>
   </si>
 </sst>
 </file>
@@ -623,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -683,6 +695,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -997,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P110"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="M108" sqref="M108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4022,7 +4037,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>17</v>
       </c>
@@ -4056,7 +4071,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="32">
         <v>21</v>
       </c>
@@ -4090,7 +4105,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="32">
         <v>21</v>
       </c>
@@ -4124,7 +4139,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="32">
         <v>22</v>
       </c>
@@ -4158,7 +4173,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="32">
         <v>23</v>
       </c>
@@ -4192,7 +4207,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="32">
         <v>22</v>
       </c>
@@ -4226,7 +4241,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A103" s="32">
         <v>22</v>
       </c>
@@ -4259,12 +4274,20 @@
       <c r="K103" s="22">
         <v>0.79166666666666663</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L103" s="31">
+        <f>SUM(H96:I103)</f>
+        <v>29</v>
+      </c>
+      <c r="M103" s="15">
+        <f>SUM(L103+19.5)</f>
+        <v>48.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="32">
         <v>22</v>
       </c>
@@ -4297,7 +4320,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="32">
         <v>22</v>
       </c>
@@ -4330,7 +4353,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>18</v>
       </c>
@@ -4363,37 +4386,118 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D108" s="13"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>18</v>
+      </c>
+      <c r="B108" t="s">
+        <v>70</v>
+      </c>
+      <c r="C108" t="s">
+        <v>85</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" t="s">
+        <v>130</v>
+      </c>
+      <c r="F108" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G108" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I108" s="15">
+        <f>ROUNDUP(((SUM(K108-J108)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J108" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="K108" s="22">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D109" s="13"/>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="1" t="s">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D110" s="13"/>
+      <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D111" s="13"/>
+      <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D112" s="13"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D113" s="13"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B114" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C110" s="24">
+      <c r="C114" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>260.5</v>
-      </c>
-      <c r="D110" s="14" t="s">
+        <v>262.5</v>
+      </c>
+      <c r="D114" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E110" s="24">
+      <c r="E114" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F110" s="14" t="s">
+      <c r="F114" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G110" s="24">
+      <c r="G114" s="24">
         <f>SUM(I:I)</f>
-        <v>205.5</v>
+        <v>207.5</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D115" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E115" s="33">
+        <f>135-E114</f>
+        <v>80</v>
+      </c>
+      <c r="F115" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G115" s="33">
+        <f>315-G114</f>
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B116" t="s">
+        <v>132</v>
+      </c>
+      <c r="C116">
+        <f>ROUNDUP(C114/30, 0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B117" t="s">
+        <v>133</v>
+      </c>
+      <c r="C117">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4401,7 +4505,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D109" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Update Wireframes and Filters
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64650A9B-5247-5046-B0B7-47AB3EE6057E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C1909D-258D-9A4F-90BF-A33EBF2BA71B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="135">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Kredits erfordert:</t>
+  </si>
+  <si>
+    <t>MockUps Rezept Filter</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="M108" sqref="M108"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="M109" sqref="M109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4410,24 +4413,80 @@
       </c>
       <c r="I108" s="15">
         <f>ROUNDUP(((SUM(K108-J108)*24*60/60)/0.25),0)*0.25</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J108" s="21">
         <v>0.625</v>
       </c>
       <c r="K108" s="22">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>23</v>
+      </c>
+      <c r="B109" t="s">
+        <v>88</v>
+      </c>
+      <c r="C109" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" t="s">
+        <v>96</v>
+      </c>
+      <c r="F109" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G109" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I109" s="15">
+        <f>ROUNDUP(((SUM(K109-J109)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="J109" s="21">
         <v>0.70833333333333337</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D109" s="13"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
+      <c r="K109" s="22">
+        <v>0.71875</v>
+      </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D110" s="13"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
+      <c r="A110" s="32">
+        <v>22</v>
+      </c>
+      <c r="B110" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D110" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F110" s="2">
+        <v>44379</v>
+      </c>
+      <c r="G110" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I110" s="15">
+        <f>ROUNDUP(((SUM(K110-J110)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.75</v>
+      </c>
+      <c r="J110" s="21">
+        <v>0.71875</v>
+      </c>
+      <c r="K110" s="22">
+        <v>0.79166666666666663</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D111" s="13"/>
@@ -4450,7 +4509,7 @@
       </c>
       <c r="C114" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>262.5</v>
+        <v>263.5</v>
       </c>
       <c r="D114" s="14" t="s">
         <v>45</v>
@@ -4464,7 +4523,7 @@
       </c>
       <c r="G114" s="24">
         <f>SUM(I:I)</f>
-        <v>207.5</v>
+        <v>208.5</v>
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.2">
@@ -4480,7 +4539,7 @@
       </c>
       <c r="G115" s="33">
         <f>315-G114</f>
-        <v>107.5</v>
+        <v>106.5</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[TASK] Update filter mockups and concept
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C1909D-258D-9A4F-90BF-A33EBF2BA71B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8B9B86-3A18-9A43-BB33-EF99AC6E88F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="135">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -1017,8 +1017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="M109" sqref="M109"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4313,7 +4313,7 @@
         <v>44359</v>
       </c>
       <c r="I105" s="15">
-        <f>ROUNDUP(((SUM(K105-J105)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I105:I110" si="11">ROUNDUP(((SUM(K105-J105)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
       </c>
       <c r="J105" s="21">
@@ -4346,7 +4346,7 @@
         <v>44359</v>
       </c>
       <c r="I106" s="15">
-        <f>ROUNDUP(((SUM(K106-J106)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="J106" s="21">
@@ -4379,7 +4379,7 @@
         <v>44359</v>
       </c>
       <c r="I107" s="15">
-        <f>ROUNDUP(((SUM(K107-J107)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" si="11"/>
         <v>1.25</v>
       </c>
       <c r="J107" s="21">
@@ -4412,7 +4412,7 @@
         <v>44359</v>
       </c>
       <c r="I108" s="15">
-        <f>ROUNDUP(((SUM(K108-J108)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="J108" s="21">
@@ -4445,7 +4445,7 @@
         <v>44359</v>
       </c>
       <c r="I109" s="15">
-        <f>ROUNDUP(((SUM(K109-J109)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
       <c r="J109" s="21">
@@ -4478,7 +4478,7 @@
         <v>44359</v>
       </c>
       <c r="I110" s="15">
-        <f>ROUNDUP(((SUM(K110-J110)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" si="11"/>
         <v>1.75</v>
       </c>
       <c r="J110" s="21">
@@ -4489,14 +4489,70 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D111" s="13"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
+      <c r="A111" s="32">
+        <v>22</v>
+      </c>
+      <c r="B111" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C111" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="F111" s="2">
+        <v>44380</v>
+      </c>
+      <c r="G111" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I111" s="15">
+        <f t="shared" ref="I111:I112" si="12">ROUNDUP(((SUM(K111-J111)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J111" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K111" s="22">
+        <v>0.66666666666666663</v>
+      </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D112" s="13"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
+      <c r="A112">
+        <v>18</v>
+      </c>
+      <c r="B112" t="s">
+        <v>70</v>
+      </c>
+      <c r="C112" t="s">
+        <v>85</v>
+      </c>
+      <c r="D112" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" t="s">
+        <v>130</v>
+      </c>
+      <c r="F112" s="2">
+        <v>44380</v>
+      </c>
+      <c r="G112" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I112" s="15">
+        <f t="shared" si="12"/>
+        <v>1.25</v>
+      </c>
+      <c r="J112" s="21">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K112" s="22">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D113" s="13"/>
@@ -4509,7 +4565,7 @@
       </c>
       <c r="C114" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>263.5</v>
+        <v>266.75</v>
       </c>
       <c r="D114" s="14" t="s">
         <v>45</v>
@@ -4523,7 +4579,7 @@
       </c>
       <c r="G114" s="24">
         <f>SUM(I:I)</f>
-        <v>208.5</v>
+        <v>211.75</v>
       </c>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.2">
@@ -4539,7 +4595,7 @@
       </c>
       <c r="G115" s="33">
         <f>315-G114</f>
-        <v>106.5</v>
+        <v>103.25</v>
       </c>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add new filter to mock ups and clean up in said progress
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8B9B86-3A18-9A43-BB33-EF99AC6E88F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A62975-AEFA-A04F-B040-190D22A8F97C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="135">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -638,7 +638,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -701,6 +701,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1015,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P117"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4554,73 +4558,111 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D113" s="13"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B114" s="1" t="s">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A114" s="32">
+        <v>18</v>
+      </c>
+      <c r="B114" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C114" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="D114" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="F114" s="35">
+        <v>44382</v>
+      </c>
+      <c r="G114" s="35">
+        <v>44359</v>
+      </c>
+      <c r="I114" s="15">
+        <f t="shared" ref="I114" si="13">ROUNDUP(((SUM(K114-J114)*24*60/60)/0.25),0)*0.25</f>
+        <v>3.5</v>
+      </c>
+      <c r="J114" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K114" s="22">
+        <v>0.68402777777777779</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D115" s="13"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B116" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C114" s="24">
+      <c r="C116" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>266.75</v>
-      </c>
-      <c r="D114" s="14" t="s">
+        <v>270.25</v>
+      </c>
+      <c r="D116" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E114" s="24">
+      <c r="E116" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F114" s="14" t="s">
+      <c r="F116" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G114" s="24">
+      <c r="G116" s="24">
         <f>SUM(I:I)</f>
-        <v>211.75</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D115" s="13" t="s">
+        <v>215.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D117" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E115" s="33">
-        <f>135-E114</f>
+      <c r="E117" s="33">
+        <f>135-E116</f>
         <v>80</v>
       </c>
-      <c r="F115" s="13" t="s">
+      <c r="F117" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G115" s="33">
-        <f>315-G114</f>
-        <v>103.25</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B116" t="s">
+      <c r="G117" s="33">
+        <f>315-G116</f>
+        <v>99.75</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B118" t="s">
         <v>132</v>
       </c>
-      <c r="C116">
-        <f>ROUNDUP(C114/30, 0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B117" t="s">
+      <c r="C118">
+        <f>ROUNDUP(C116/30, 0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B119" t="s">
         <v>133</v>
       </c>
-      <c r="C117">
+      <c r="C119">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add new recipe mock ups
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A62975-AEFA-A04F-B040-190D22A8F97C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B04E1-D040-7949-8F0B-A4B329F1E7AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="138">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -440,6 +440,15 @@
   </si>
   <si>
     <t>MockUps Rezept Filter</t>
+  </si>
+  <si>
+    <t>Sommerpause: Urlaub und Denkblokade</t>
+  </si>
+  <si>
+    <t>Neues Rezept Mock Up refinement</t>
+  </si>
+  <si>
+    <t>Neues Rezept Mock Up finished</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P119"/>
+  <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4525,7 +4534,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>18</v>
       </c>
@@ -4557,8 +4566,16 @@
       <c r="K112" s="22">
         <v>0.70833333333333337</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L112" s="31">
+        <f>SUM(H105:I112)</f>
+        <v>17.5</v>
+      </c>
+      <c r="M112" s="15">
+        <f>SUM(L112+19.5)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D113" s="13"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -4602,67 +4619,171 @@
       <c r="G115" s="2"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
+        <v>135</v>
+      </c>
+      <c r="D116" s="13"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D117" s="13"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A118" s="32">
+        <v>22</v>
+      </c>
+      <c r="B118" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C118" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D118" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F118" s="2">
+        <v>44438</v>
+      </c>
+      <c r="G118" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I118" s="15">
+        <f t="shared" ref="I118" si="14">ROUNDUP(((SUM(K118-J118)*24*60/60)/0.25),0)*0.25</f>
+        <v>6</v>
+      </c>
+      <c r="J118" s="21">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K118" s="22">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A119" s="32">
+        <v>22</v>
+      </c>
+      <c r="B119" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C119" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D119" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="F119" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G119" s="2">
+        <v>44359</v>
+      </c>
+      <c r="I119" s="15">
+        <f t="shared" ref="I119" si="15">ROUNDUP(((SUM(K119-J119)*24*60/60)/0.25),0)*0.25</f>
+        <v>5.25</v>
+      </c>
+      <c r="J119" s="21">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K119" s="22">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D120" s="13"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D121" s="13"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D122" s="13"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D123" s="13"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D124" s="13"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B125" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C116" s="24">
+      <c r="C125" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>270.25</v>
-      </c>
-      <c r="D116" s="14" t="s">
+        <v>281.5</v>
+      </c>
+      <c r="D125" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E116" s="24">
+      <c r="E125" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F116" s="14" t="s">
+      <c r="F125" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G116" s="24">
+      <c r="G125" s="24">
         <f>SUM(I:I)</f>
-        <v>215.25</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D117" s="13" t="s">
+        <v>226.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D126" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E117" s="33">
-        <f>135-E116</f>
+      <c r="E126" s="33">
+        <f>135-E125</f>
         <v>80</v>
       </c>
-      <c r="F117" s="13" t="s">
+      <c r="F126" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G117" s="33">
-        <f>315-G116</f>
-        <v>99.75</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B118" t="s">
+      <c r="G126" s="33">
+        <f>315-G125</f>
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B127" t="s">
         <v>132</v>
       </c>
-      <c r="C118">
-        <f>ROUNDUP(C116/30, 0)</f>
+      <c r="C127">
+        <f>ROUNDUP(C125/30, 0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B119" t="s">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B128" t="s">
         <v>133</v>
       </c>
-      <c r="C119">
+      <c r="C128">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D124" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add my cookbook first iteration low fidelity prototype
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87B04E1-D040-7949-8F0B-A4B329F1E7AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E5989-FEBF-A94A-A150-4C278DD1F7A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="140">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>Neues Rezept Mock Up finished</t>
+  </si>
+  <si>
+    <t>Neue Abgabe Termine</t>
+  </si>
+  <si>
+    <t>Mein Kochbuch Mock Up first iteration</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1037,7 @@
   <dimension ref="A1:P128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A111" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+      <selection activeCell="I128" sqref="A1:I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4624,7 +4630,9 @@
       </c>
       <c r="D116" s="13"/>
       <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
+      <c r="G116" s="2" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D117" s="13"/>
@@ -4651,7 +4659,7 @@
         <v>44438</v>
       </c>
       <c r="G118" s="2">
-        <v>44359</v>
+        <v>44479</v>
       </c>
       <c r="I118" s="15">
         <f t="shared" ref="I118" si="14">ROUNDUP(((SUM(K118-J118)*24*60/60)/0.25),0)*0.25</f>
@@ -4684,7 +4692,7 @@
         <v>44445</v>
       </c>
       <c r="G119" s="2">
-        <v>44359</v>
+        <v>44481</v>
       </c>
       <c r="I119" s="15">
         <f t="shared" ref="I119" si="15">ROUNDUP(((SUM(K119-J119)*24*60/60)/0.25),0)*0.25</f>
@@ -4698,9 +4706,37 @@
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D120" s="13"/>
-      <c r="F120" s="2"/>
-      <c r="G120" s="2"/>
+      <c r="A120" s="32">
+        <v>22</v>
+      </c>
+      <c r="B120" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C120" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D120" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="F120" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G120" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I120" s="15">
+        <f t="shared" ref="I120" si="16">ROUNDUP(((SUM(K120-J120)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="J120" s="21">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K120" s="22">
+        <v>0.60416666666666663</v>
+      </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D121" s="13"/>
@@ -4728,7 +4764,7 @@
       </c>
       <c r="C125" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>281.5</v>
+        <v>282.75</v>
       </c>
       <c r="D125" s="14" t="s">
         <v>45</v>
@@ -4742,7 +4778,7 @@
       </c>
       <c r="G125" s="24">
         <f>SUM(I:I)</f>
-        <v>226.5</v>
+        <v>227.75</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -4758,7 +4794,7 @@
       </c>
       <c r="G126" s="33">
         <f>315-G125</f>
-        <v>88.5</v>
+        <v>87.25</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[WIP][FEATURE] Add recipe view first iteration
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49E5989-FEBF-A94A-A150-4C278DD1F7A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB36D3F-F463-4145-868E-0B7D4A2D6DF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="141">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -455,6 +455,9 @@
   </si>
   <si>
     <t>Mein Kochbuch Mock Up first iteration</t>
+  </si>
+  <si>
+    <t>Rezeptansicht Mock Up first iteration</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I128" sqref="A1:I128"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I128" sqref="I128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4728,7 +4731,7 @@
         <v>44481</v>
       </c>
       <c r="I120" s="15">
-        <f t="shared" ref="I120" si="16">ROUNDUP(((SUM(K120-J120)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I120:I121" si="16">ROUNDUP(((SUM(K120-J120)*24*60/60)/0.25),0)*0.25</f>
         <v>1.25</v>
       </c>
       <c r="J120" s="21">
@@ -4739,9 +4742,37 @@
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D121" s="13"/>
-      <c r="F121" s="2"/>
-      <c r="G121" s="2"/>
+      <c r="A121" s="32">
+        <v>22</v>
+      </c>
+      <c r="B121" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C121" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D121" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F121" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G121" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I121" s="15">
+        <f t="shared" si="16"/>
+        <v>2.5</v>
+      </c>
+      <c r="J121" s="21">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="K121" s="22">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D122" s="13"/>
@@ -4764,7 +4795,7 @@
       </c>
       <c r="C125" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>282.75</v>
+        <v>285.25</v>
       </c>
       <c r="D125" s="14" t="s">
         <v>45</v>
@@ -4778,7 +4809,7 @@
       </c>
       <c r="G125" s="24">
         <f>SUM(I:I)</f>
-        <v>227.75</v>
+        <v>230.25</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -4794,7 +4825,7 @@
       </c>
       <c r="G126" s="33">
         <f>315-G125</f>
-        <v>87.25</v>
+        <v>84.75</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[TASK] Enhance menus and spacing
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB36D3F-F463-4145-868E-0B7D4A2D6DF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36BEB8-F8E1-BE4C-A2CA-17351678E55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="142">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>Rezeptansicht Mock Up first iteration</t>
+  </si>
+  <si>
+    <t>Rezeptansicht Mock Up refinement</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I128" sqref="I128"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="L121" sqref="L121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4775,9 +4778,37 @@
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D122" s="13"/>
-      <c r="F122" s="2"/>
-      <c r="G122" s="2"/>
+      <c r="A122" s="32">
+        <v>22</v>
+      </c>
+      <c r="B122" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C122" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D122" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F122" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G122" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I122" s="15">
+        <f t="shared" ref="I122" si="17">ROUNDUP(((SUM(K122-J122)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="J122" s="21">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="K122" s="22">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D123" s="13"/>
@@ -4795,7 +4826,7 @@
       </c>
       <c r="C125" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>285.25</v>
+        <v>285.75</v>
       </c>
       <c r="D125" s="14" t="s">
         <v>45</v>
@@ -4809,7 +4840,7 @@
       </c>
       <c r="G125" s="24">
         <f>SUM(I:I)</f>
-        <v>230.25</v>
+        <v>230.75</v>
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
@@ -4825,7 +4856,7 @@
       </c>
       <c r="G126" s="33">
         <f>315-G125</f>
-        <v>84.75</v>
+        <v>84.25</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add recipe view to prototype
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E36BEB8-F8E1-BE4C-A2CA-17351678E55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22854DF3-442F-9849-A700-8B19DE96F523}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="143">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>Rezeptansicht Mock Up refinement</t>
+  </si>
+  <si>
+    <t>Rezeptansicht Mock Up finished</t>
   </si>
 </sst>
 </file>
@@ -1040,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P128"/>
+  <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="L121" sqref="L121"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4811,9 +4814,37 @@
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D123" s="13"/>
-      <c r="F123" s="2"/>
-      <c r="G123" s="2"/>
+      <c r="A123" s="32">
+        <v>22</v>
+      </c>
+      <c r="B123" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C123" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="F123" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G123" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I123" s="15">
+        <f t="shared" ref="I123" si="18">ROUNDUP(((SUM(K123-J123)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="J123" s="21">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="K123" s="22">
+        <v>0.44791666666666669</v>
+      </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D124" s="13"/>
@@ -4821,58 +4852,83 @@
       <c r="G124" s="2"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B125" s="1" t="s">
+      <c r="D125" s="13"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D126" s="13"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D127" s="13"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D128" s="13"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D129" s="13"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B130" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C125" s="24">
+      <c r="C130" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>285.75</v>
-      </c>
-      <c r="D125" s="14" t="s">
+        <v>287.25</v>
+      </c>
+      <c r="D130" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E125" s="24">
+      <c r="E130" s="24">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F125" s="14" t="s">
+      <c r="F130" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G125" s="24">
+      <c r="G130" s="24">
         <f>SUM(I:I)</f>
-        <v>230.75</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D126" s="13" t="s">
+        <v>232.25</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D131" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E126" s="33">
-        <f>135-E125</f>
+      <c r="E131" s="33">
+        <f>135-E130</f>
         <v>80</v>
       </c>
-      <c r="F126" s="13" t="s">
+      <c r="F131" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G126" s="33">
-        <f>315-G125</f>
-        <v>84.25</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B127" t="s">
+      <c r="G131" s="33">
+        <f>315-G130</f>
+        <v>82.75</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B132" t="s">
         <v>132</v>
       </c>
-      <c r="C127">
-        <f>ROUNDUP(C125/30, 0)</f>
+      <c r="C132">
+        <f>ROUNDUP(C130/30, 0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B128" t="s">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B133" t="s">
         <v>133</v>
       </c>
-      <c r="C128">
+      <c r="C133">
         <v>15</v>
       </c>
     </row>
@@ -4881,7 +4937,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D124" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D129" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add different profile views and minor enhancements
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22854DF3-442F-9849-A700-8B19DE96F523}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B74E1-4545-304B-BE8F-9E82DC4548D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="144">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>Rezeptansicht Mock Up finished</t>
+  </si>
+  <si>
+    <t>Profil ansichten und refinements</t>
   </si>
 </sst>
 </file>
@@ -1045,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F126" sqref="F126"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4847,9 +4850,37 @@
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D124" s="13"/>
-      <c r="F124" s="2"/>
-      <c r="G124" s="2"/>
+      <c r="A124" s="32">
+        <v>22</v>
+      </c>
+      <c r="B124" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C124" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D124" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="F124" s="2">
+        <v>44445</v>
+      </c>
+      <c r="G124" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I124" s="15">
+        <f t="shared" ref="I124" si="19">ROUNDUP(((SUM(K124-J124)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.75</v>
+      </c>
+      <c r="J124" s="21">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="K124" s="22">
+        <v>0.55555555555555558</v>
+      </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D125" s="13"/>
@@ -4882,7 +4913,7 @@
       </c>
       <c r="C130" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>287.25</v>
+        <v>290</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>45</v>
@@ -4896,7 +4927,7 @@
       </c>
       <c r="G130" s="24">
         <f>SUM(I:I)</f>
-        <v>232.25</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.2">
@@ -4912,7 +4943,7 @@
       </c>
       <c r="G131" s="33">
         <f>315-G130</f>
-        <v>82.75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add recipe edit screen
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{763B74E1-4545-304B-BE8F-9E82DC4548D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19929582-5184-F446-8770-FD0125B9D14B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="145">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>Profil ansichten und refinements</t>
+  </si>
+  <si>
+    <t>Rezept bearbeiten Screen anfertigen</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4872,7 +4875,7 @@
         <v>44481</v>
       </c>
       <c r="I124" s="15">
-        <f t="shared" ref="I124" si="19">ROUNDUP(((SUM(K124-J124)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I124:I126" si="19">ROUNDUP(((SUM(K124-J124)*24*60/60)/0.25),0)*0.25</f>
         <v>2.75</v>
       </c>
       <c r="J124" s="21">
@@ -4888,9 +4891,37 @@
       <c r="G125" s="2"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D126" s="13"/>
-      <c r="F126" s="2"/>
-      <c r="G126" s="2"/>
+      <c r="A126" s="32">
+        <v>22</v>
+      </c>
+      <c r="B126" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C126" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D126" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="F126" s="2">
+        <v>44459</v>
+      </c>
+      <c r="G126" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I126" s="15">
+        <f t="shared" si="19"/>
+        <v>1.5</v>
+      </c>
+      <c r="J126" s="21">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K126" s="22">
+        <v>0.64583333333333337</v>
+      </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D127" s="13"/>
@@ -4913,7 +4944,7 @@
       </c>
       <c r="C130" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>290</v>
+        <v>291.5</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>45</v>
@@ -4927,7 +4958,7 @@
       </c>
       <c r="G130" s="24">
         <f>SUM(I:I)</f>
-        <v>235</v>
+        <v>236.5</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.2">
@@ -4943,7 +4974,7 @@
       </c>
       <c r="G131" s="33">
         <f>315-G130</f>
-        <v>80</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add friend list screen and minor enhancements
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19929582-5184-F446-8770-FD0125B9D14B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE7152C-4C5F-7242-989F-265FDD8445B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="146">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>Rezept bearbeiten Screen anfertigen</t>
+  </si>
+  <si>
+    <t>Freundeliste und kleine Anpassungen</t>
   </si>
 </sst>
 </file>
@@ -1051,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I129" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4924,9 +4927,37 @@
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D127" s="13"/>
-      <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
+      <c r="A127" s="32">
+        <v>22</v>
+      </c>
+      <c r="B127" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C127" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="D127" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="F127" s="2">
+        <v>44459</v>
+      </c>
+      <c r="G127" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I127" s="15">
+        <f t="shared" ref="I127" si="20">ROUNDUP(((SUM(K127-J127)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="J127" s="21">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="K127" s="22">
+        <v>0.66666666666666663</v>
+      </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D128" s="13"/>
@@ -4944,7 +4975,7 @@
       </c>
       <c r="C130" s="24">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>291.5</v>
+        <v>292</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>45</v>
@@ -4958,7 +4989,7 @@
       </c>
       <c r="G130" s="24">
         <f>SUM(I:I)</f>
-        <v>236.5</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="2:7" x14ac:dyDescent="0.2">
@@ -4974,7 +5005,7 @@
       </c>
       <c r="G131" s="33">
         <f>315-G130</f>
-        <v>78.5</v>
+        <v>78</v>
       </c>
     </row>
     <row r="132" spans="2:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[TASK] Refine todo list
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE7152C-4C5F-7242-989F-265FDD8445B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F6FFF-8029-8841-97AC-9C16413D34F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="147">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>Freundeliste und kleine Anpassungen</t>
+  </si>
+  <si>
+    <t>TODO refinement</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -613,53 +616,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="double">
@@ -671,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -693,43 +650,16 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -738,6 +668,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1054,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I129" sqref="I129"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I133" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1069,13 +1007,12 @@
     <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="15.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.1640625" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="19"/>
-    <col min="11" max="11" width="10.83203125" style="20"/>
+    <col min="10" max="11" width="10.83203125" style="28"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
     <col min="13" max="13" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1103,16 +1040,16 @@
       <c r="I1" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="27" t="s">
         <v>33</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="20" t="s">
         <v>62</v>
       </c>
       <c r="N1" t="s">
@@ -1145,8 +1082,8 @@
       <c r="I2">
         <v>6</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="26"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
       <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -1270,7 +1207,7 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="L6" s="27">
+      <c r="L6" s="25">
         <f>SUM(H2:I6)</f>
         <v>17</v>
       </c>
@@ -1278,7 +1215,7 @@
         <f>SUM(L6+16)</f>
         <v>33</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="17" t="s">
         <v>38</v>
       </c>
       <c r="O6" t="s">
@@ -1290,7 +1227,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="L7" s="7"/>
-      <c r="N7" s="23"/>
+      <c r="N7" s="17"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1399,10 +1336,10 @@
         <f>ROUNDUP(((SUM(K11-J11)*24*60/60)/0.25),0)*0.25</f>
         <v>1</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="19">
         <v>0.68402777777777779</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="19">
         <v>0.72222222222222221</v>
       </c>
       <c r="L11" s="16"/>
@@ -1436,10 +1373,10 @@
         <f>ROUNDUP(((SUM(K12-J12)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>0.73958333333333337</v>
       </c>
       <c r="L12" s="16"/>
@@ -1473,10 +1410,10 @@
         <v>1.5</v>
       </c>
       <c r="I13" s="15"/>
-      <c r="J13" s="21">
+      <c r="J13" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="19">
         <v>0.47361111111111115</v>
       </c>
     </row>
@@ -1507,10 +1444,10 @@
         <v>2.25</v>
       </c>
       <c r="I14" s="15"/>
-      <c r="J14" s="21">
+      <c r="J14" s="19">
         <v>0.5</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="19">
         <v>0.59375</v>
       </c>
     </row>
@@ -1540,10 +1477,10 @@
         <f t="shared" ref="I15:I51" si="0">ROUNDUP(((SUM(K15-J15)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
-      <c r="J15" s="21">
+      <c r="J15" s="19">
         <v>0.59722222222222221</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="19">
         <v>0.60416666666666663</v>
       </c>
     </row>
@@ -1574,10 +1511,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="19">
         <v>0.69097222222222221</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="19">
         <v>0.7270833333333333</v>
       </c>
     </row>
@@ -1607,10 +1544,10 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J17" s="21">
+      <c r="J17" s="19">
         <v>0.75347222222222221</v>
       </c>
-      <c r="K17" s="22">
+      <c r="K17" s="19">
         <v>0.77777777777777779</v>
       </c>
     </row>
@@ -1640,10 +1577,10 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="19">
         <v>0.79513888888888884</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="19">
         <v>0.82291666666666663</v>
       </c>
     </row>
@@ -1672,7 +1609,7 @@
       <c r="I19" s="15">
         <v>0.75</v>
       </c>
-      <c r="L19" s="27">
+      <c r="L19" s="25">
         <f>SUM(H8:I19)</f>
         <v>11</v>
       </c>
@@ -1714,10 +1651,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J21" s="21">
+      <c r="J21" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K21" s="22">
+      <c r="K21" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -1773,13 +1710,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="19">
         <v>0.75</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="19">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L23" s="29"/>
+      <c r="L23" s="7"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1808,10 +1745,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="19">
         <v>0.375</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="19">
         <v>0.45833333333333331</v>
       </c>
     </row>
@@ -1841,10 +1778,10 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="J25" s="21">
+      <c r="J25" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="19">
         <v>0.6020833333333333</v>
       </c>
     </row>
@@ -1875,10 +1812,10 @@
         <v>4</v>
       </c>
       <c r="I26" s="15"/>
-      <c r="J26" s="21">
+      <c r="J26" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="19">
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -1909,10 +1846,10 @@
         <v>1.25</v>
       </c>
       <c r="I27" s="15"/>
-      <c r="J27" s="21">
+      <c r="J27" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K27" s="22">
+      <c r="K27" s="19">
         <v>0.63541666666666663</v>
       </c>
     </row>
@@ -1942,10 +1879,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="19">
         <v>0.375</v>
       </c>
-      <c r="K28" s="22">
+      <c r="K28" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -1975,10 +1912,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J29" s="21">
+      <c r="J29" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K29" s="22">
+      <c r="K29" s="19">
         <v>0.75</v>
       </c>
     </row>
@@ -2008,13 +1945,13 @@
         <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
-      <c r="J30" s="21">
+      <c r="J30" s="19">
         <v>0.69097222222222221</v>
       </c>
-      <c r="K30" s="22">
+      <c r="K30" s="19">
         <v>0.80208333333333337</v>
       </c>
-      <c r="L30" s="27">
+      <c r="L30" s="25">
         <f>SUM(H21:I30)</f>
         <v>20</v>
       </c>
@@ -2028,8 +1965,8 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="I31" s="15"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
       <c r="L31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -2058,10 +1995,10 @@
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
-      <c r="J32" s="21">
+      <c r="J32" s="19">
         <v>0.375</v>
       </c>
-      <c r="K32" s="22">
+      <c r="K32" s="19">
         <v>0.5625</v>
       </c>
     </row>
@@ -2091,10 +2028,10 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="J33" s="21">
+      <c r="J33" s="19">
         <v>0.625</v>
       </c>
-      <c r="K33" s="22">
+      <c r="K33" s="19">
         <v>0.72916666666666663</v>
       </c>
     </row>
@@ -2124,10 +2061,10 @@
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="J34" s="21">
+      <c r="J34" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="19">
         <v>0.77083333333333337</v>
       </c>
     </row>
@@ -2157,10 +2094,10 @@
         <f>ROUNDUP(((SUM(K35-J35)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
       </c>
-      <c r="J35" s="21">
+      <c r="J35" s="19">
         <v>0.375</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -2190,10 +2127,10 @@
         <f>ROUNDUP(((SUM(K36-J36)*24*60/60)/0.25),0)*0.25</f>
         <v>1</v>
       </c>
-      <c r="J36" s="21">
+      <c r="J36" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -2224,10 +2161,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J37" s="21">
+      <c r="J37" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
@@ -2258,10 +2195,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J38" s="21">
+      <c r="J38" s="19">
         <v>0.375</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K38" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -2292,13 +2229,13 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J39" s="21">
+      <c r="J39" s="19">
         <v>0.625</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L39" s="27">
+      <c r="L39" s="25">
         <f>SUM(H32:I39)</f>
         <v>23.25</v>
       </c>
@@ -2313,8 +2250,8 @@
       <c r="G40" s="2"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="22"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
       <c r="L40" s="7"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -2344,10 +2281,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J41" s="21">
+      <c r="J41" s="19">
         <v>0.375</v>
       </c>
-      <c r="K41" s="22">
+      <c r="K41" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -2378,10 +2315,10 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="J42" s="21">
+      <c r="J42" s="19">
         <v>0.5625</v>
       </c>
-      <c r="K42" s="22">
+      <c r="K42" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -2412,10 +2349,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J43" s="21">
+      <c r="J43" s="19">
         <v>0.375</v>
       </c>
-      <c r="K43" s="22">
+      <c r="K43" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -2446,10 +2383,10 @@
         <f t="shared" si="0"/>
         <v>4.75</v>
       </c>
-      <c r="J44" s="21">
+      <c r="J44" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K44" s="22">
+      <c r="K44" s="19">
         <v>0.78125</v>
       </c>
     </row>
@@ -2480,10 +2417,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J45" s="21">
+      <c r="J45" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K45" s="22">
+      <c r="K45" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -2514,10 +2451,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J46" s="21">
+      <c r="J46" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K46" s="22">
+      <c r="K46" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -2548,10 +2485,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J47" s="21">
+      <c r="J47" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K47" s="22">
+      <c r="K47" s="19">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -2582,10 +2519,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="J48" s="21">
+      <c r="J48" s="19">
         <v>0.5</v>
       </c>
-      <c r="K48" s="22">
+      <c r="K48" s="19">
         <v>0.75</v>
       </c>
     </row>
@@ -2616,13 +2553,13 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-      <c r="J49" s="21">
+      <c r="J49" s="19">
         <v>0.79166666666666663</v>
       </c>
-      <c r="K49" s="22">
+      <c r="K49" s="19">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L49" s="31">
+      <c r="L49" s="26">
         <f>SUM(H41:I49)</f>
         <v>30</v>
       </c>
@@ -2637,8 +2574,8 @@
       <c r="G50" s="2"/>
       <c r="H50" s="15"/>
       <c r="I50" s="15"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="22"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -2664,8 +2601,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J51" s="21"/>
-      <c r="K51" s="22"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -2694,10 +2631,10 @@
         <v>4.75</v>
       </c>
       <c r="I52" s="15"/>
-      <c r="J52" s="21">
+      <c r="J52" s="19">
         <v>0.35416666666666669</v>
       </c>
-      <c r="K52" s="22">
+      <c r="K52" s="19">
         <v>0.55208333333333337</v>
       </c>
     </row>
@@ -2728,10 +2665,10 @@
         <v>4.75</v>
       </c>
       <c r="I53" s="15"/>
-      <c r="J53" s="21">
+      <c r="J53" s="19">
         <v>0.55208333333333337</v>
       </c>
-      <c r="K53" s="22">
+      <c r="K53" s="19">
         <v>0.75</v>
       </c>
     </row>
@@ -2762,10 +2699,10 @@
         <v>6</v>
       </c>
       <c r="I54" s="15"/>
-      <c r="J54" s="21">
+      <c r="J54" s="19">
         <v>0.375</v>
       </c>
-      <c r="K54" s="22">
+      <c r="K54" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -2796,10 +2733,10 @@
         <v>3</v>
       </c>
       <c r="I55" s="15"/>
-      <c r="J55" s="21">
+      <c r="J55" s="19">
         <v>0.375</v>
       </c>
-      <c r="K55" s="22">
+      <c r="K55" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -2829,10 +2766,10 @@
         <f t="shared" ref="I56:I62" si="1">ROUNDUP(((SUM(K56-J56)*24*60/60)/0.25),0)*0.25</f>
         <v>1.75</v>
       </c>
-      <c r="J56" s="21">
+      <c r="J56" s="19">
         <v>0.5</v>
       </c>
-      <c r="K56" s="22">
+      <c r="K56" s="19">
         <v>0.57291666666666663</v>
       </c>
     </row>
@@ -2862,13 +2799,13 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J57" s="21">
+      <c r="J57" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K57" s="22">
+      <c r="K57" s="19">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L57" s="31">
+      <c r="L57" s="26">
         <f>SUM(H49:I57)</f>
         <v>23</v>
       </c>
@@ -2881,8 +2818,8 @@
       <c r="D58" s="13"/>
       <c r="G58" s="2"/>
       <c r="I58" s="15"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="22"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -2910,10 +2847,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J59" s="21">
+      <c r="J59" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K59" s="22">
+      <c r="K59" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -2943,10 +2880,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J60" s="21">
+      <c r="J60" s="19">
         <v>0.625</v>
       </c>
-      <c r="K60" s="22">
+      <c r="K60" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -2977,10 +2914,10 @@
         <v>3</v>
       </c>
       <c r="I61" s="15"/>
-      <c r="J61" s="21">
+      <c r="J61" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K61" s="22">
+      <c r="K61" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -3010,10 +2947,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="J62" s="21">
+      <c r="J62" s="19">
         <v>0.625</v>
       </c>
-      <c r="K62" s="22">
+      <c r="K62" s="19">
         <v>0.83333333333333337</v>
       </c>
     </row>
@@ -3044,10 +2981,10 @@
         <v>1</v>
       </c>
       <c r="I63" s="15"/>
-      <c r="J63" s="21">
+      <c r="J63" s="19">
         <v>0.375</v>
       </c>
-      <c r="K63" s="22">
+      <c r="K63" s="19">
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -3077,10 +3014,10 @@
         <f t="shared" ref="I64:I67" si="2">ROUNDUP(((SUM(K64-J64)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J64" s="21">
+      <c r="J64" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K64" s="22">
+      <c r="K64" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -3111,10 +3048,10 @@
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="J65" s="21">
+      <c r="J65" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K65" s="22">
+      <c r="K65" s="19">
         <v>0.57291666666666663</v>
       </c>
     </row>
@@ -3145,10 +3082,10 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J66" s="21">
+      <c r="J66" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K66" s="22">
+      <c r="K66" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -3179,13 +3116,13 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="J67" s="21">
+      <c r="J67" s="19">
         <v>0.375</v>
       </c>
-      <c r="K67" s="22">
+      <c r="K67" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="L67" s="31">
+      <c r="L67" s="26">
         <f>SUM(H59:I67)</f>
         <v>22.75</v>
       </c>
@@ -3228,10 +3165,10 @@
         <v>6</v>
       </c>
       <c r="I69" s="15"/>
-      <c r="J69" s="21">
+      <c r="J69" s="19">
         <v>0.375</v>
       </c>
-      <c r="K69" s="22">
+      <c r="K69" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -3262,10 +3199,10 @@
         <f t="shared" ref="I70:I78" si="3">ROUNDUP(((SUM(K70-J70)*24*60/60)/0.25),0)*0.25</f>
         <v>1.25</v>
       </c>
-      <c r="J70" s="21">
+      <c r="J70" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K70" s="22">
+      <c r="K70" s="19">
         <v>0.71875</v>
       </c>
     </row>
@@ -3296,10 +3233,10 @@
         <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
-      <c r="J71" s="21">
+      <c r="J71" s="19">
         <v>0.71875</v>
       </c>
-      <c r="K71" s="22">
+      <c r="K71" s="19">
         <v>0.77083333333333337</v>
       </c>
     </row>
@@ -3330,13 +3267,13 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J72" s="21">
+      <c r="J72" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K72" s="22">
+      <c r="K72" s="19">
         <v>0.75</v>
       </c>
-      <c r="L72" s="31">
+      <c r="L72" s="26">
         <f>SUM(H69:I72)</f>
         <v>13.5</v>
       </c>
@@ -3379,10 +3316,10 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J74" s="21">
+      <c r="J74" s="19">
         <v>0.5</v>
       </c>
-      <c r="K74" s="22">
+      <c r="K74" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -3413,10 +3350,10 @@
         <v>1</v>
       </c>
       <c r="I75" s="15"/>
-      <c r="J75" s="21">
+      <c r="J75" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K75" s="22">
+      <c r="K75" s="19">
         <v>0.75</v>
       </c>
     </row>
@@ -3447,10 +3384,10 @@
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
-      <c r="J76" s="21">
+      <c r="J76" s="19">
         <v>0.75</v>
       </c>
-      <c r="K76" s="22">
+      <c r="K76" s="19">
         <v>0.78125</v>
       </c>
     </row>
@@ -3481,10 +3418,10 @@
         <v>3.25</v>
       </c>
       <c r="I77" s="15"/>
-      <c r="J77" s="21">
+      <c r="J77" s="19">
         <v>0.40625</v>
       </c>
-      <c r="K77" s="22">
+      <c r="K77" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
@@ -3515,10 +3452,10 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="J78" s="21">
+      <c r="J78" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K78" s="22">
+      <c r="K78" s="19">
         <v>0.75</v>
       </c>
     </row>
@@ -3549,13 +3486,13 @@
         <f t="shared" ref="I79:I81" si="4">ROUNDUP(((SUM(K79-J79)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
       </c>
-      <c r="J79" s="21">
+      <c r="J79" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K79" s="22">
+      <c r="K79" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="L79" s="31">
+      <c r="L79" s="26">
         <f>SUM(H74:I79)</f>
         <v>16</v>
       </c>
@@ -3598,10 +3535,10 @@
         <f t="shared" si="4"/>
         <v>3.25</v>
       </c>
-      <c r="J81" s="21">
+      <c r="J81" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K81" s="22">
+      <c r="K81" s="19">
         <v>0.55208333333333337</v>
       </c>
     </row>
@@ -3632,10 +3569,10 @@
         <f t="shared" ref="I82:I86" si="5">ROUNDUP(((SUM(K82-J82)*24*60/60)/0.25),0)*0.25</f>
         <v>5.25</v>
       </c>
-      <c r="J82" s="21">
+      <c r="J82" s="19">
         <v>0.55208333333333337</v>
       </c>
-      <c r="K82" s="22">
+      <c r="K82" s="19">
         <v>0.76736111111111116</v>
       </c>
     </row>
@@ -3666,10 +3603,10 @@
         <v>2.75</v>
       </c>
       <c r="I83" s="15"/>
-      <c r="J83" s="21">
+      <c r="J83" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K83" s="22">
+      <c r="K83" s="19">
         <v>0.53125</v>
       </c>
     </row>
@@ -3700,27 +3637,27 @@
         <f t="shared" si="5"/>
         <v>6.5</v>
       </c>
-      <c r="J84" s="21">
+      <c r="J84" s="19">
         <v>0.55208333333333337</v>
       </c>
-      <c r="K84" s="22">
+      <c r="K84" s="19">
         <v>0.82291666666666663</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="32">
+      <c r="A85" s="21">
         <v>22</v>
       </c>
-      <c r="B85" s="32" t="s">
+      <c r="B85" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C85" s="32" t="s">
+      <c r="C85" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D85" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E85" s="32" t="s">
+      <c r="E85" s="21" t="s">
         <v>101</v>
       </c>
       <c r="F85" s="2">
@@ -3734,27 +3671,27 @@
         <f t="shared" si="5"/>
         <v>5.75</v>
       </c>
-      <c r="J85" s="21">
+      <c r="J85" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K85" s="22">
+      <c r="K85" s="19">
         <v>0.82291666666666663</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="32">
+      <c r="A86" s="21">
         <v>22</v>
       </c>
-      <c r="B86" s="32" t="s">
+      <c r="B86" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C86" s="32" t="s">
+      <c r="C86" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D86" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E86" s="32" t="s">
+      <c r="E86" s="21" t="s">
         <v>102</v>
       </c>
       <c r="F86" s="2">
@@ -3768,13 +3705,13 @@
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="J86" s="21">
+      <c r="J86" s="19">
         <v>0.45833333333333331</v>
       </c>
-      <c r="K86" s="22">
+      <c r="K86" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="L86" s="31">
+      <c r="L86" s="26">
         <f>SUM(H81:I86)</f>
         <v>25.5</v>
       </c>
@@ -3817,27 +3754,27 @@
         <v>1.5</v>
       </c>
       <c r="I88" s="15"/>
-      <c r="J88" s="21">
+      <c r="J88" s="19">
         <v>0.375</v>
       </c>
-      <c r="K88" s="22">
+      <c r="K88" s="19">
         <v>0.4375</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A89" s="32">
+      <c r="A89" s="21">
         <v>22</v>
       </c>
-      <c r="B89" s="32" t="s">
+      <c r="B89" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C89" s="32" t="s">
+      <c r="C89" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D89" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="32" t="s">
+      <c r="E89" s="21" t="s">
         <v>109</v>
       </c>
       <c r="F89" s="2">
@@ -3851,27 +3788,27 @@
         <f t="shared" ref="I89" si="6">ROUNDUP(((SUM(K89-J89)*24*60/60)/0.25),0)*0.25</f>
         <v>2.5</v>
       </c>
-      <c r="J89" s="21">
+      <c r="J89" s="19">
         <v>0.45833333333333331</v>
       </c>
-      <c r="K89" s="22">
+      <c r="K89" s="19">
         <v>0.55208333333333337</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A90" s="32">
+      <c r="A90" s="21">
         <v>22</v>
       </c>
-      <c r="B90" s="32" t="s">
+      <c r="B90" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="32" t="s">
+      <c r="C90" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D90" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="32" t="s">
+      <c r="E90" s="21" t="s">
         <v>110</v>
       </c>
       <c r="F90" s="2">
@@ -3885,27 +3822,27 @@
         <f t="shared" ref="I90:I92" si="7">ROUNDUP(((SUM(K90-J90)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J90" s="21">
+      <c r="J90" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K90" s="22">
+      <c r="K90" s="19">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A91" s="32">
+      <c r="A91" s="21">
         <v>22</v>
       </c>
-      <c r="B91" s="32" t="s">
+      <c r="B91" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="32" t="s">
+      <c r="C91" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D91" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E91" s="32" t="s">
+      <c r="E91" s="21" t="s">
         <v>111</v>
       </c>
       <c r="F91" s="2">
@@ -3919,27 +3856,27 @@
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="J91" s="21">
+      <c r="J91" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K91" s="22">
+      <c r="K91" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A92" s="32">
+      <c r="A92" s="21">
         <v>22</v>
       </c>
-      <c r="B92" s="32" t="s">
+      <c r="B92" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="32" t="s">
+      <c r="C92" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D92" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="32" t="s">
+      <c r="E92" s="21" t="s">
         <v>112</v>
       </c>
       <c r="F92" s="2">
@@ -3953,27 +3890,27 @@
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="J92" s="21">
+      <c r="J92" s="19">
         <v>0.375</v>
       </c>
-      <c r="K92" s="22">
+      <c r="K92" s="19">
         <v>0.58333333333333337</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="32">
+      <c r="A93" s="21">
         <v>22</v>
       </c>
-      <c r="B93" s="32" t="s">
+      <c r="B93" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="32" t="s">
+      <c r="C93" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D93" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="32" t="s">
+      <c r="E93" s="21" t="s">
         <v>113</v>
       </c>
       <c r="F93" s="2">
@@ -3987,27 +3924,27 @@
         <f t="shared" ref="I93" si="8">ROUNDUP(((SUM(K93-J93)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J93" s="21">
+      <c r="J93" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K93" s="22">
+      <c r="K93" s="19">
         <v>0.75</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="32">
+      <c r="A94" s="21">
         <v>22</v>
       </c>
-      <c r="B94" s="32" t="s">
+      <c r="B94" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="32" t="s">
+      <c r="C94" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D94" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="32" t="s">
+      <c r="E94" s="21" t="s">
         <v>114</v>
       </c>
       <c r="F94" s="2">
@@ -4021,13 +3958,13 @@
         <f t="shared" ref="I94" si="9">ROUNDUP(((SUM(K94-J94)*24*60/60)/0.25),0)*0.25</f>
         <v>3</v>
       </c>
-      <c r="J94" s="21">
+      <c r="J94" s="19">
         <v>0.625</v>
       </c>
-      <c r="K94" s="22">
+      <c r="K94" s="19">
         <v>0.75</v>
       </c>
-      <c r="L94" s="31">
+      <c r="L94" s="26">
         <f>SUM(H89:I94)</f>
         <v>17.5</v>
       </c>
@@ -4044,19 +3981,19 @@
       <c r="I95" s="15"/>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A96" s="32">
+      <c r="A96" s="21">
         <v>22</v>
       </c>
-      <c r="B96" s="32" t="s">
+      <c r="B96" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="32" t="s">
+      <c r="C96" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D96" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E96" s="32" t="s">
+      <c r="E96" s="21" t="s">
         <v>114</v>
       </c>
       <c r="F96" s="2">
@@ -4070,10 +4007,10 @@
         <f t="shared" ref="I96:I99" si="10">ROUNDUP(((SUM(K96-J96)*24*60/60)/0.25),0)*0.25</f>
         <v>9</v>
       </c>
-      <c r="J96" s="21">
+      <c r="J96" s="19">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K96" s="22">
+      <c r="K96" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
@@ -4104,27 +4041,27 @@
         <v>4</v>
       </c>
       <c r="I97" s="15"/>
-      <c r="J97" s="21">
+      <c r="J97" s="19">
         <v>0.375</v>
       </c>
-      <c r="K97" s="22">
+      <c r="K97" s="19">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" s="32">
+      <c r="A98" s="21">
         <v>21</v>
       </c>
       <c r="B98" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="32" t="s">
+      <c r="C98" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D98" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="32" t="s">
+      <c r="E98" s="21" t="s">
         <v>120</v>
       </c>
       <c r="F98" s="2">
@@ -4138,27 +4075,27 @@
         <f t="shared" si="10"/>
         <v>2.5</v>
       </c>
-      <c r="J98" s="21">
+      <c r="J98" s="19">
         <v>0.625</v>
       </c>
-      <c r="K98" s="22">
+      <c r="K98" s="19">
         <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A99" s="32">
+      <c r="A99" s="21">
         <v>21</v>
       </c>
       <c r="B99" t="s">
         <v>88</v>
       </c>
-      <c r="C99" s="32" t="s">
+      <c r="C99" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D99" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E99" s="32" t="s">
+      <c r="E99" s="21" t="s">
         <v>122</v>
       </c>
       <c r="F99" s="2">
@@ -4172,27 +4109,27 @@
         <f t="shared" si="10"/>
         <v>0.5</v>
       </c>
-      <c r="J99" s="21">
+      <c r="J99" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K99" s="22">
+      <c r="K99" s="19">
         <v>0.75</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A100" s="32">
+      <c r="A100" s="21">
         <v>22</v>
       </c>
       <c r="B100" t="s">
         <v>88</v>
       </c>
-      <c r="C100" s="32" t="s">
+      <c r="C100" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D100" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E100" s="32" t="s">
+      <c r="E100" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F100" s="2">
@@ -4206,27 +4143,27 @@
         <f>ROUNDUP(((SUM(K100-J100)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J100" s="21">
+      <c r="J100" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K100" s="22">
+      <c r="K100" s="19">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A101" s="32">
+      <c r="A101" s="21">
         <v>23</v>
       </c>
       <c r="B101" t="s">
         <v>88</v>
       </c>
-      <c r="C101" s="32" t="s">
+      <c r="C101" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D101" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E101" s="32" t="s">
+      <c r="E101" s="21" t="s">
         <v>124</v>
       </c>
       <c r="F101" s="2">
@@ -4240,27 +4177,27 @@
         <f>ROUNDUP(((SUM(K101-J101)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J101" s="21">
+      <c r="J101" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K101" s="22">
+      <c r="K101" s="19">
         <v>0.75</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A102" s="32">
+      <c r="A102" s="21">
         <v>22</v>
       </c>
       <c r="B102" t="s">
         <v>88</v>
       </c>
-      <c r="C102" s="32" t="s">
+      <c r="C102" s="21" t="s">
         <v>115</v>
       </c>
       <c r="D102" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E102" s="32" t="s">
+      <c r="E102" s="21" t="s">
         <v>123</v>
       </c>
       <c r="F102" s="2">
@@ -4274,27 +4211,27 @@
         <f>ROUNDUP(((SUM(K102-J102)*24*60/60)/0.25),0)*0.25</f>
         <v>1</v>
       </c>
-      <c r="J102" s="21">
+      <c r="J102" s="19">
         <v>0.75</v>
       </c>
-      <c r="K102" s="22">
+      <c r="K102" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="32">
+      <c r="A103" s="21">
         <v>22</v>
       </c>
-      <c r="B103" s="32" t="s">
+      <c r="B103" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C103" s="32" t="s">
+      <c r="C103" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D103" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E103" s="32" t="s">
+      <c r="E103" s="21" t="s">
         <v>125</v>
       </c>
       <c r="F103" s="2">
@@ -4308,13 +4245,13 @@
         <f>ROUNDUP(((SUM(K103-J103)*24*60/60)/0.25),0)*0.25</f>
         <v>8</v>
       </c>
-      <c r="J103" s="21">
+      <c r="J103" s="19">
         <v>0.45833333333333331</v>
       </c>
-      <c r="K103" s="22">
+      <c r="K103" s="19">
         <v>0.79166666666666663</v>
       </c>
-      <c r="L103" s="31">
+      <c r="L103" s="26">
         <f>SUM(H96:I103)</f>
         <v>29</v>
       </c>
@@ -4328,19 +4265,19 @@
       <c r="G104" s="2"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A105" s="32">
+      <c r="A105" s="21">
         <v>22</v>
       </c>
-      <c r="B105" s="32" t="s">
+      <c r="B105" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C105" s="32" t="s">
+      <c r="C105" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D105" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E105" s="32" t="s">
+      <c r="E105" s="21" t="s">
         <v>128</v>
       </c>
       <c r="F105" s="2">
@@ -4353,27 +4290,27 @@
         <f t="shared" ref="I105:I110" si="11">ROUNDUP(((SUM(K105-J105)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
       </c>
-      <c r="J105" s="21">
+      <c r="J105" s="19">
         <v>0.625</v>
       </c>
-      <c r="K105" s="22">
+      <c r="K105" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A106" s="32">
+      <c r="A106" s="21">
         <v>22</v>
       </c>
-      <c r="B106" s="32" t="s">
+      <c r="B106" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="C106" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D106" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E106" s="32" t="s">
+      <c r="E106" s="21" t="s">
         <v>129</v>
       </c>
       <c r="F106" s="2">
@@ -4386,10 +4323,10 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="J106" s="21">
+      <c r="J106" s="19">
         <v>0.375</v>
       </c>
-      <c r="K106" s="22">
+      <c r="K106" s="19">
         <v>0.625</v>
       </c>
     </row>
@@ -4419,10 +4356,10 @@
         <f t="shared" si="11"/>
         <v>1.25</v>
       </c>
-      <c r="J107" s="21">
+      <c r="J107" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K107" s="22">
+      <c r="K107" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
@@ -4452,10 +4389,10 @@
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="J108" s="21">
+      <c r="J108" s="19">
         <v>0.625</v>
       </c>
-      <c r="K108" s="22">
+      <c r="K108" s="19">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -4485,27 +4422,27 @@
         <f t="shared" si="11"/>
         <v>0.25</v>
       </c>
-      <c r="J109" s="21">
+      <c r="J109" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K109" s="22">
+      <c r="K109" s="19">
         <v>0.71875</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A110" s="32">
+      <c r="A110" s="21">
         <v>22</v>
       </c>
-      <c r="B110" s="32" t="s">
+      <c r="B110" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C110" s="32" t="s">
+      <c r="C110" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D110" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E110" s="32" t="s">
+      <c r="E110" s="21" t="s">
         <v>134</v>
       </c>
       <c r="F110" s="2">
@@ -4518,27 +4455,27 @@
         <f t="shared" si="11"/>
         <v>1.75</v>
       </c>
-      <c r="J110" s="21">
+      <c r="J110" s="19">
         <v>0.71875</v>
       </c>
-      <c r="K110" s="22">
+      <c r="K110" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A111" s="32">
+      <c r="A111" s="21">
         <v>22</v>
       </c>
-      <c r="B111" s="32" t="s">
+      <c r="B111" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C111" s="32" t="s">
+      <c r="C111" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D111" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E111" s="32" t="s">
+      <c r="E111" s="21" t="s">
         <v>134</v>
       </c>
       <c r="F111" s="2">
@@ -4551,10 +4488,10 @@
         <f t="shared" ref="I111:I112" si="12">ROUNDUP(((SUM(K111-J111)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J111" s="21">
+      <c r="J111" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K111" s="22">
+      <c r="K111" s="19">
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -4584,13 +4521,13 @@
         <f t="shared" si="12"/>
         <v>1.25</v>
       </c>
-      <c r="J112" s="21">
+      <c r="J112" s="19">
         <v>0.66666666666666663</v>
       </c>
-      <c r="K112" s="22">
+      <c r="K112" s="19">
         <v>0.70833333333333337</v>
       </c>
-      <c r="L112" s="31">
+      <c r="L112" s="26">
         <f>SUM(H105:I112)</f>
         <v>17.5</v>
       </c>
@@ -4605,35 +4542,35 @@
       <c r="G113" s="2"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A114" s="32">
+      <c r="A114" s="21">
         <v>18</v>
       </c>
-      <c r="B114" s="32" t="s">
+      <c r="B114" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="C114" s="32" t="s">
+      <c r="C114" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D114" s="34" t="s">
+      <c r="D114" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E114" s="32" t="s">
+      <c r="E114" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F114" s="35">
+      <c r="F114" s="24">
         <v>44382</v>
       </c>
-      <c r="G114" s="35">
+      <c r="G114" s="24">
         <v>44359</v>
       </c>
       <c r="I114" s="15">
         <f t="shared" ref="I114" si="13">ROUNDUP(((SUM(K114-J114)*24*60/60)/0.25),0)*0.25</f>
         <v>3.5</v>
       </c>
-      <c r="J114" s="21">
+      <c r="J114" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K114" s="22">
+      <c r="K114" s="19">
         <v>0.68402777777777779</v>
       </c>
     </row>
@@ -4658,19 +4595,19 @@
       <c r="G117" s="2"/>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A118" s="32">
+      <c r="A118" s="21">
         <v>22</v>
       </c>
-      <c r="B118" s="32" t="s">
+      <c r="B118" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C118" s="32" t="s">
+      <c r="C118" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D118" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="32" t="s">
+      <c r="E118" s="21" t="s">
         <v>136</v>
       </c>
       <c r="F118" s="2">
@@ -4683,27 +4620,27 @@
         <f t="shared" ref="I118" si="14">ROUNDUP(((SUM(K118-J118)*24*60/60)/0.25),0)*0.25</f>
         <v>6</v>
       </c>
-      <c r="J118" s="21">
+      <c r="J118" s="19">
         <v>0.54166666666666663</v>
       </c>
-      <c r="K118" s="22">
+      <c r="K118" s="19">
         <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A119" s="32">
+      <c r="A119" s="21">
         <v>22</v>
       </c>
-      <c r="B119" s="32" t="s">
+      <c r="B119" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C119" s="32" t="s">
+      <c r="C119" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D119" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="32" t="s">
+      <c r="E119" s="21" t="s">
         <v>137</v>
       </c>
       <c r="F119" s="2">
@@ -4716,27 +4653,27 @@
         <f t="shared" ref="I119" si="15">ROUNDUP(((SUM(K119-J119)*24*60/60)/0.25),0)*0.25</f>
         <v>5.25</v>
       </c>
-      <c r="J119" s="21">
+      <c r="J119" s="19">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K119" s="22">
+      <c r="K119" s="19">
         <v>0.55208333333333337</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A120" s="32">
+      <c r="A120" s="21">
         <v>22</v>
       </c>
-      <c r="B120" s="32" t="s">
+      <c r="B120" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C120" s="32" t="s">
+      <c r="C120" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D120" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E120" s="32" t="s">
+      <c r="E120" s="21" t="s">
         <v>139</v>
       </c>
       <c r="F120" s="2">
@@ -4749,27 +4686,27 @@
         <f t="shared" ref="I120:I121" si="16">ROUNDUP(((SUM(K120-J120)*24*60/60)/0.25),0)*0.25</f>
         <v>1.25</v>
       </c>
-      <c r="J120" s="21">
+      <c r="J120" s="19">
         <v>0.55208333333333337</v>
       </c>
-      <c r="K120" s="22">
+      <c r="K120" s="19">
         <v>0.60416666666666663</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A121" s="32">
+      <c r="A121" s="21">
         <v>22</v>
       </c>
-      <c r="B121" s="32" t="s">
+      <c r="B121" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C121" s="32" t="s">
+      <c r="C121" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D121" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E121" s="32" t="s">
+      <c r="E121" s="21" t="s">
         <v>140</v>
       </c>
       <c r="F121" s="2">
@@ -4782,27 +4719,27 @@
         <f t="shared" si="16"/>
         <v>2.5</v>
       </c>
-      <c r="J121" s="21">
+      <c r="J121" s="19">
         <v>0.60416666666666663</v>
       </c>
-      <c r="K121" s="22">
+      <c r="K121" s="19">
         <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A122" s="32">
+      <c r="A122" s="21">
         <v>22</v>
       </c>
-      <c r="B122" s="32" t="s">
+      <c r="B122" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C122" s="32" t="s">
+      <c r="C122" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D122" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E122" s="32" t="s">
+      <c r="E122" s="21" t="s">
         <v>141</v>
       </c>
       <c r="F122" s="2">
@@ -4815,27 +4752,27 @@
         <f t="shared" ref="I122" si="17">ROUNDUP(((SUM(K122-J122)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="J122" s="21">
+      <c r="J122" s="19">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K122" s="22">
+      <c r="K122" s="19">
         <v>0.75</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A123" s="32">
+      <c r="A123" s="21">
         <v>22</v>
       </c>
-      <c r="B123" s="32" t="s">
+      <c r="B123" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C123" s="32" t="s">
+      <c r="C123" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D123" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E123" s="32" t="s">
+      <c r="E123" s="21" t="s">
         <v>142</v>
       </c>
       <c r="F123" s="2">
@@ -4848,27 +4785,27 @@
         <f t="shared" ref="I123" si="18">ROUNDUP(((SUM(K123-J123)*24*60/60)/0.25),0)*0.25</f>
         <v>1.5</v>
       </c>
-      <c r="J123" s="21">
+      <c r="J123" s="19">
         <v>0.38541666666666669</v>
       </c>
-      <c r="K123" s="22">
+      <c r="K123" s="19">
         <v>0.44791666666666669</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A124" s="32">
+      <c r="A124" s="21">
         <v>22</v>
       </c>
-      <c r="B124" s="32" t="s">
+      <c r="B124" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C124" s="32" t="s">
+      <c r="C124" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D124" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E124" s="32" t="s">
+      <c r="E124" s="21" t="s">
         <v>143</v>
       </c>
       <c r="F124" s="2">
@@ -4881,10 +4818,10 @@
         <f t="shared" ref="I124:I126" si="19">ROUNDUP(((SUM(K124-J124)*24*60/60)/0.25),0)*0.25</f>
         <v>2.75</v>
       </c>
-      <c r="J124" s="21">
+      <c r="J124" s="19">
         <v>0.44791666666666669</v>
       </c>
-      <c r="K124" s="22">
+      <c r="K124" s="19">
         <v>0.55555555555555558</v>
       </c>
     </row>
@@ -4894,19 +4831,19 @@
       <c r="G125" s="2"/>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A126" s="32">
+      <c r="A126" s="21">
         <v>22</v>
       </c>
-      <c r="B126" s="32" t="s">
+      <c r="B126" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C126" s="32" t="s">
+      <c r="C126" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D126" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E126" s="32" t="s">
+      <c r="E126" s="21" t="s">
         <v>144</v>
       </c>
       <c r="F126" s="2">
@@ -4919,27 +4856,27 @@
         <f t="shared" si="19"/>
         <v>1.5</v>
       </c>
-      <c r="J126" s="21">
+      <c r="J126" s="19">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K126" s="22">
+      <c r="K126" s="19">
         <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A127" s="32">
+      <c r="A127" s="21">
         <v>22</v>
       </c>
-      <c r="B127" s="32" t="s">
+      <c r="B127" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="C127" s="32" t="s">
+      <c r="C127" s="21" t="s">
         <v>126</v>
       </c>
       <c r="D127" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E127" s="32" t="s">
+      <c r="E127" s="21" t="s">
         <v>145</v>
       </c>
       <c r="F127" s="2">
@@ -4952,63 +4889,91 @@
         <f t="shared" ref="I127" si="20">ROUNDUP(((SUM(K127-J127)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
       </c>
-      <c r="J127" s="21">
+      <c r="J127" s="19">
         <v>0.64583333333333337</v>
       </c>
-      <c r="K127" s="22">
+      <c r="K127" s="19">
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D128" s="13"/>
-      <c r="F128" s="2"/>
-      <c r="G128" s="2"/>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="21">
+        <v>22</v>
+      </c>
+      <c r="B128" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C128" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D128" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="F128" s="2">
+        <v>44459</v>
+      </c>
+      <c r="G128" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I128" s="15">
+        <f t="shared" ref="I128" si="21">ROUNDUP(((SUM(K128-J128)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J128" s="19">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K128" s="19">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D129" s="13"/>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B130" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="24">
+      <c r="C130" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D130" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E130" s="24">
+      <c r="E130" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
       <c r="F130" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G130" s="24">
+      <c r="G130" s="18">
         <f>SUM(I:I)</f>
-        <v>237</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D131" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E131" s="33">
+      <c r="E131" s="22">
         <f>135-E130</f>
         <v>80</v>
       </c>
       <c r="F131" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G131" s="33">
+      <c r="G131" s="22">
         <f>315-G130</f>
-        <v>78</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>132</v>
       </c>
@@ -5017,13 +4982,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B133" t="s">
+    <row r="133" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="10"/>
+      <c r="B133" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="10">
         <v>15</v>
       </c>
+      <c r="D133" s="10"/>
+      <c r="E133" s="10"/>
+      <c r="F133" s="10"/>
+      <c r="G133" s="10"/>
+      <c r="H133" s="10"/>
+      <c r="I133" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">

</xml_diff>

<commit_message>
[FEATURE] Add settings screen and wip notifications and friend requests
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2F6FFF-8029-8841-97AC-9C16413D34F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA171AC5-10C8-C848-B246-0FD18F443768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="148">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>TODO refinement</t>
+  </si>
+  <si>
+    <t>Einstellungen Screen, Icons und Ideensammlung</t>
   </si>
 </sst>
 </file>
@@ -990,10 +993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P133"/>
+  <dimension ref="A1:P137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I133" sqref="I133"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E131" sqref="E131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4929,80 +4932,128 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D129" s="13"/>
-      <c r="F129" s="2"/>
-      <c r="G129" s="2"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B130" s="1" t="s">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A129" s="21">
+        <v>22</v>
+      </c>
+      <c r="B129" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C129" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D129" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E129" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F129" s="2">
+        <v>44459</v>
+      </c>
+      <c r="G129" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I129" s="15">
+        <f t="shared" ref="I129" si="22">ROUNDUP(((SUM(K129-J129)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.75</v>
+      </c>
+      <c r="J129" s="19">
+        <v>0.75</v>
+      </c>
+      <c r="K129" s="19">
+        <v>0.82291666666666663</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D130" s="13"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D131" s="13"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D132" s="13"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D133" s="13"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="18">
+      <c r="C134" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>293</v>
-      </c>
-      <c r="D130" s="14" t="s">
+        <v>294.75</v>
+      </c>
+      <c r="D134" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E130" s="18">
+      <c r="E134" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F130" s="14" t="s">
+      <c r="F134" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G130" s="18">
+      <c r="G134" s="18">
         <f>SUM(I:I)</f>
-        <v>238</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D131" s="13" t="s">
+        <v>239.75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D135" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E131" s="22">
-        <f>135-E130</f>
+      <c r="E135" s="22">
+        <f>135-E134</f>
         <v>80</v>
       </c>
-      <c r="F131" s="13" t="s">
+      <c r="F135" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G131" s="22">
-        <f>315-G130</f>
-        <v>77</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B132" t="s">
+      <c r="G135" s="22">
+        <f>315-G134</f>
+        <v>75.25</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B136" t="s">
         <v>132</v>
       </c>
-      <c r="C132">
-        <f>ROUNDUP(C130/30, 0)</f>
+      <c r="C136">
+        <f>ROUNDUP(C134/30, 0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="10"/>
-      <c r="B133" s="10" t="s">
+    <row r="137" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="10"/>
+      <c r="B137" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C133" s="10">
+      <c r="C137" s="10">
         <v>15</v>
       </c>
-      <c r="D133" s="10"/>
-      <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
-      <c r="G133" s="10"/>
-      <c r="H133" s="10"/>
-      <c r="I133" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="10"/>
+      <c r="F137" s="10"/>
+      <c r="G137" s="10"/>
+      <c r="H137" s="10"/>
+      <c r="I137" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D129" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D133" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add notification and friend request screens as well as figma frame refinement
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA171AC5-10C8-C848-B246-0FD18F443768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C82A4B-FF47-6D4F-B827-043D0AD7B15D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="149">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>Einstellungen Screen, Icons und Ideensammlung</t>
+  </si>
+  <si>
+    <t>Benachrichtigungen und Freundschaftsanfragen</t>
   </si>
 </sst>
 </file>
@@ -995,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4966,9 +4969,37 @@
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D130" s="13"/>
-      <c r="F130" s="2"/>
-      <c r="G130" s="2"/>
+      <c r="A130" s="21">
+        <v>22</v>
+      </c>
+      <c r="B130" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C130" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E130" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="F130" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G130" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I130" s="15">
+        <f t="shared" ref="I130" si="23">ROUNDUP(((SUM(K130-J130)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J130" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K130" s="19">
+        <v>0.45833333333333331</v>
+      </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D131" s="13"/>
@@ -4991,7 +5022,7 @@
       </c>
       <c r="C134" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>294.75</v>
+        <v>295.75</v>
       </c>
       <c r="D134" s="14" t="s">
         <v>45</v>
@@ -5005,7 +5036,7 @@
       </c>
       <c r="G134" s="18">
         <f>SUM(I:I)</f>
-        <v>239.75</v>
+        <v>240.75</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
@@ -5021,7 +5052,7 @@
       </c>
       <c r="G135" s="22">
         <f>315-G134</f>
-        <v>75.25</v>
+        <v>74.25</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add friendrequest send screen
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C82A4B-FF47-6D4F-B827-043D0AD7B15D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259FF018-B820-B44A-A768-8A6F155CB2EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="150">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -482,6 +482,9 @@
   </si>
   <si>
     <t>Benachrichtigungen und Freundschaftsanfragen</t>
+  </si>
+  <si>
+    <t>Freundschaftsanfrage ausstehend</t>
   </si>
 </sst>
 </file>
@@ -996,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P137"/>
+  <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I137" sqref="I137"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I141" sqref="A120:I141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4896,6 +4899,7 @@
         <v>0.5</v>
       </c>
       <c r="J127" s="19">
+        <f>K126</f>
         <v>0.64583333333333337</v>
       </c>
       <c r="K127" s="19">
@@ -4962,6 +4966,7 @@
         <v>1.75</v>
       </c>
       <c r="J129" s="19">
+        <f>K128</f>
         <v>0.75</v>
       </c>
       <c r="K129" s="19">
@@ -5002,89 +5007,148 @@
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D131" s="13"/>
-      <c r="F131" s="2"/>
-      <c r="G131" s="2"/>
+      <c r="A131" s="21">
+        <v>22</v>
+      </c>
+      <c r="B131" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C131" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D131" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E131" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="F131" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G131" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I131" s="15">
+        <f t="shared" ref="I131:I133" si="24">ROUNDUP(((SUM(K131-J131)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="J131" s="19">
+        <f>K130</f>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K131" s="19">
+        <v>0.47916666666666669</v>
+      </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A132" s="21"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="21"/>
       <c r="D132" s="13"/>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
+      <c r="I132" s="15"/>
+      <c r="J132" s="19"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A133" s="21"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="21"/>
       <c r="D133" s="13"/>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
+      <c r="I133" s="15"/>
+      <c r="J133" s="19"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B134" s="1" t="s">
+      <c r="D134" s="13"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D135" s="13"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D136" s="13"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D137" s="13"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B138" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C134" s="18">
+      <c r="C138" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>295.75</v>
-      </c>
-      <c r="D134" s="14" t="s">
+        <v>296.25</v>
+      </c>
+      <c r="D138" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E134" s="18">
+      <c r="E138" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F134" s="14" t="s">
+      <c r="F138" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G134" s="18">
+      <c r="G138" s="18">
         <f>SUM(I:I)</f>
-        <v>240.75</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D135" s="13" t="s">
+        <v>241.25</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D139" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E135" s="22">
-        <f>135-E134</f>
+      <c r="E139" s="22">
+        <f>135-E138</f>
         <v>80</v>
       </c>
-      <c r="F135" s="13" t="s">
+      <c r="F139" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G135" s="22">
-        <f>315-G134</f>
-        <v>74.25</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B136" t="s">
+      <c r="G139" s="22">
+        <f>315-G138</f>
+        <v>73.75</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B140" t="s">
         <v>132</v>
       </c>
-      <c r="C136">
-        <f>ROUNDUP(C134/30, 0)</f>
+      <c r="C140">
+        <f>ROUNDUP(C138/30, 0)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
-      <c r="B137" s="10" t="s">
+    <row r="141" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="10"/>
+      <c r="B141" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C137" s="10">
+      <c r="C141" s="10">
         <v>15</v>
       </c>
-      <c r="D137" s="10"/>
-      <c r="E137" s="10"/>
-      <c r="F137" s="10"/>
-      <c r="G137" s="10"/>
-      <c r="H137" s="10"/>
-      <c r="I137" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10"/>
+      <c r="I141" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D133" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D137" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add login and sign in screen
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259FF018-B820-B44A-A768-8A6F155CB2EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8558C2E5-EB90-7549-8021-301DE28D8DA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="151">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>Freundschaftsanfrage ausstehend</t>
+  </si>
+  <si>
+    <t>Login und SignIn Screen</t>
   </si>
 </sst>
 </file>
@@ -1001,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I141" sqref="A120:I141"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5041,14 +5044,38 @@
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A132" s="21"/>
-      <c r="B132" s="21"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="13"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
-      <c r="I132" s="15"/>
-      <c r="J132" s="19"/>
+      <c r="A132" s="21">
+        <v>22</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C132" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D132" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F132" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G132" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I132" s="15">
+        <f t="shared" ref="I132" si="25">ROUNDUP(((SUM(K132-J132)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="J132" s="19">
+        <f>K131</f>
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="K132" s="19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" s="21"/>
@@ -5086,7 +5113,7 @@
       </c>
       <c r="C138" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>296.25</v>
+        <v>296.75</v>
       </c>
       <c r="D138" s="14" t="s">
         <v>45</v>
@@ -5100,7 +5127,7 @@
       </c>
       <c r="G138" s="18">
         <f>SUM(I:I)</f>
-        <v>241.25</v>
+        <v>241.75</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -5116,7 +5143,7 @@
       </c>
       <c r="G139" s="22">
         <f>315-G138</f>
-        <v>73.75</v>
+        <v>73.25</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add predecessor and original recipe
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8558C2E5-EB90-7549-8021-301DE28D8DA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F9651-40BA-094F-BAA8-046ACAB9F455}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="152">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Login und SignIn Screen</t>
+  </si>
+  <si>
+    <t>Vorgänger und Original Rezept</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1008,7 @@
   <dimension ref="A1:P141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A123" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5078,14 +5081,38 @@
       </c>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A133" s="21"/>
-      <c r="B133" s="21"/>
-      <c r="C133" s="21"/>
-      <c r="D133" s="13"/>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
-      <c r="I133" s="15"/>
-      <c r="J133" s="19"/>
+      <c r="A133" s="21">
+        <v>22</v>
+      </c>
+      <c r="B133" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="F133" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G133" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I133" s="15">
+        <f t="shared" ref="I133" si="26">ROUNDUP(((SUM(K133-J133)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="J133" s="19">
+        <f>K132</f>
+        <v>0.5</v>
+      </c>
+      <c r="K133" s="19">
+        <v>0.5625</v>
+      </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D134" s="13"/>
@@ -5113,7 +5140,7 @@
       </c>
       <c r="C138" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>296.75</v>
+        <v>298.25</v>
       </c>
       <c r="D138" s="14" t="s">
         <v>45</v>
@@ -5127,7 +5154,7 @@
       </c>
       <c r="G138" s="18">
         <f>SUM(I:I)</f>
-        <v>241.75</v>
+        <v>243.25</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -5143,7 +5170,7 @@
       </c>
       <c r="G139" s="22">
         <f>315-G138</f>
-        <v>73.25</v>
+        <v>71.75</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[TASK] Add many changes to styleguid and frames
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F9651-40BA-094F-BAA8-046ACAB9F455}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD231487-72C4-6F4C-B69E-F4FFF0FDEA07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="21600" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="153">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -490,7 +490,10 @@
     <t>Login und SignIn Screen</t>
   </si>
   <si>
-    <t>Vorgänger und Original Rezept</t>
+    <t>Vorgaenger und Original Rezept</t>
+  </si>
+  <si>
+    <t>Figma Refinement, new Styleguide, Minor Changes</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5115,9 +5118,38 @@
       </c>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D134" s="13"/>
-      <c r="F134" s="2"/>
-      <c r="G134" s="2"/>
+      <c r="A134" s="21">
+        <v>22</v>
+      </c>
+      <c r="B134" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C134" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D134" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E134" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F134" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G134" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I134" s="15">
+        <f t="shared" ref="I134" si="27">ROUNDUP(((SUM(K134-J134)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.75</v>
+      </c>
+      <c r="J134" s="19">
+        <f>K133</f>
+        <v>0.5625</v>
+      </c>
+      <c r="K134" s="19">
+        <v>0.67708333333333337</v>
+      </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D135" s="13"/>
@@ -5140,7 +5172,7 @@
       </c>
       <c r="C138" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>298.25</v>
+        <v>301</v>
       </c>
       <c r="D138" s="14" t="s">
         <v>45</v>
@@ -5154,7 +5186,7 @@
       </c>
       <c r="G138" s="18">
         <f>SUM(I:I)</f>
-        <v>243.25</v>
+        <v>246</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -5170,7 +5202,7 @@
       </c>
       <c r="G139" s="22">
         <f>315-G138</f>
-        <v>71.75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">
@@ -5179,7 +5211,7 @@
       </c>
       <c r="C140">
         <f>ROUNDUP(C138/30, 0)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[TASK] Clean up notifications
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD231487-72C4-6F4C-B69E-F4FFF0FDEA07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566D6013-6306-1A45-8C5B-46CD8D6B287A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="153">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="K135" sqref="K135"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="K136" sqref="K136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5152,9 +5152,38 @@
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D135" s="13"/>
-      <c r="F135" s="2"/>
-      <c r="G135" s="2"/>
+      <c r="A135" s="21">
+        <v>22</v>
+      </c>
+      <c r="B135" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C135" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F135" s="2">
+        <v>44460</v>
+      </c>
+      <c r="G135" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I135" s="15">
+        <f t="shared" ref="I135" si="28">ROUNDUP(((SUM(K135-J135)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.75</v>
+      </c>
+      <c r="J135" s="19">
+        <f>K134</f>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="K135" s="19">
+        <v>0.70138888888888884</v>
+      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D136" s="13"/>
@@ -5172,7 +5201,7 @@
       </c>
       <c r="C138" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>301</v>
+        <v>301.75</v>
       </c>
       <c r="D138" s="14" t="s">
         <v>45</v>
@@ -5186,7 +5215,7 @@
       </c>
       <c r="G138" s="18">
         <f>SUM(I:I)</f>
-        <v>246</v>
+        <v>246.75</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.2">
@@ -5202,7 +5231,7 @@
       </c>
       <c r="G139" s="22">
         <f>315-G138</f>
-        <v>69</v>
+        <v>68.25</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add uploads, translations and friend recipe view
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566D6013-6306-1A45-8C5B-46CD8D6B287A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2517CF-EA30-484D-940C-32092934BE2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="154">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -494,6 +494,9 @@
   </si>
   <si>
     <t>Figma Refinement, new Styleguide, Minor Changes</t>
+  </si>
+  <si>
+    <t>Übersetzen, FreundRezeptAnsicht und Imports</t>
   </si>
 </sst>
 </file>
@@ -1008,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P141"/>
+  <dimension ref="A1:P143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="K136" sqref="K136"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="L137" sqref="L137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5038,7 +5041,7 @@
         <v>44481</v>
       </c>
       <c r="I131" s="15">
-        <f t="shared" ref="I131:I133" si="24">ROUNDUP(((SUM(K131-J131)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I131" si="24">ROUNDUP(((SUM(K131-J131)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
       </c>
       <c r="J131" s="19">
@@ -5186,84 +5189,129 @@
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D136" s="13"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
+      <c r="A136" s="21">
+        <v>22</v>
+      </c>
+      <c r="B136" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C136" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D136" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F136" s="2">
+        <v>44464</v>
+      </c>
+      <c r="G136" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I136" s="15">
+        <f t="shared" ref="I136" si="29">ROUNDUP(((SUM(K136-J136)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J136" s="19">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K136" s="19">
+        <v>0.59375</v>
+      </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D137" s="13"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
+      <c r="J137" s="19">
+        <f>K136</f>
+        <v>0.59375</v>
+      </c>
+      <c r="K137" s="19">
+        <v>0.70138888888888884</v>
+      </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B138" s="1" t="s">
+      <c r="D138" s="13"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D139" s="13"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B140" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C138" s="18">
+      <c r="C140" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>301.75</v>
-      </c>
-      <c r="D138" s="14" t="s">
+        <v>302.75</v>
+      </c>
+      <c r="D140" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E138" s="18">
+      <c r="E140" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F138" s="14" t="s">
+      <c r="F140" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G138" s="18">
+      <c r="G140" s="18">
         <f>SUM(I:I)</f>
-        <v>246.75</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D139" s="13" t="s">
+        <v>247.75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D141" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E139" s="22">
-        <f>135-E138</f>
+      <c r="E141" s="22">
+        <f>135-E140</f>
         <v>80</v>
       </c>
-      <c r="F139" s="13" t="s">
+      <c r="F141" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G139" s="22">
-        <f>315-G138</f>
-        <v>68.25</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B140" t="s">
+      <c r="G141" s="22">
+        <f>315-G140</f>
+        <v>67.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B142" t="s">
         <v>132</v>
       </c>
-      <c r="C140">
-        <f>ROUNDUP(C138/30, 0)</f>
+      <c r="C142">
+        <f>ROUNDUP(C140/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="10"/>
-      <c r="B141" s="10" t="s">
+    <row r="143" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="10"/>
+      <c r="B143" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C141" s="10">
+      <c r="C143" s="10">
         <v>15</v>
       </c>
-      <c r="D141" s="10"/>
-      <c r="E141" s="10"/>
-      <c r="F141" s="10"/>
-      <c r="G141" s="10"/>
-      <c r="H141" s="10"/>
-      <c r="I141" s="10"/>
+      <c r="D143" s="10"/>
+      <c r="E143" s="10"/>
+      <c r="F143" s="10"/>
+      <c r="G143" s="10"/>
+      <c r="H143" s="10"/>
+      <c r="I143" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D137" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D139" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tutorial screens
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2517CF-EA30-484D-940C-32092934BE2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF160B-C7B0-0140-8527-FB2DB3EC962B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="155">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -497,6 +497,9 @@
   </si>
   <si>
     <t>Übersetzen, FreundRezeptAnsicht und Imports</t>
+  </si>
+  <si>
+    <t>Einführungsscreens</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="L137" sqref="L137"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4557,12 +4560,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D113" s="13"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="21">
         <v>18</v>
       </c>
@@ -4595,12 +4598,12 @@
         <v>0.68402777777777779</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D115" s="13"/>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>135</v>
       </c>
@@ -4610,12 +4613,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D117" s="13"/>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="21">
         <v>22</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>0.79166666666666663</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="21">
         <v>22</v>
       </c>
@@ -4681,7 +4684,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="21">
         <v>22</v>
       </c>
@@ -4714,7 +4717,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" s="21">
         <v>22</v>
       </c>
@@ -4747,7 +4750,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" s="21">
         <v>22</v>
       </c>
@@ -4780,7 +4783,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" s="21">
         <v>22</v>
       </c>
@@ -4813,7 +4816,7 @@
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A124" s="21">
         <v>22</v>
       </c>
@@ -4845,13 +4848,21 @@
       <c r="K124" s="19">
         <v>0.55555555555555558</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L124" s="26">
+        <f>SUM(H114:I124)</f>
+        <v>23.25</v>
+      </c>
+      <c r="M124" s="15">
+        <f>SUM(L124+19.5)</f>
+        <v>42.75</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D125" s="13"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" s="21">
         <v>22</v>
       </c>
@@ -4884,7 +4895,7 @@
         <v>0.64583333333333337</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" s="21">
         <v>22</v>
       </c>
@@ -4918,7 +4929,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="21">
         <v>22</v>
       </c>
@@ -4951,7 +4962,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="21">
         <v>22</v>
       </c>
@@ -4985,7 +4996,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="21">
         <v>22</v>
       </c>
@@ -5018,7 +5029,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" s="21">
         <v>22</v>
       </c>
@@ -5052,7 +5063,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" s="21">
         <v>22</v>
       </c>
@@ -5086,7 +5097,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" s="21">
         <v>22</v>
       </c>
@@ -5120,7 +5131,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" s="21">
         <v>22</v>
       </c>
@@ -5154,7 +5165,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="21">
         <v>22</v>
       </c>
@@ -5188,7 +5199,7 @@
         <v>0.70138888888888884</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="21">
         <v>22</v>
       </c>
@@ -5220,36 +5231,67 @@
       <c r="K136" s="19">
         <v>0.59375</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L136" s="26">
+        <f>SUM(H126:I136)</f>
+        <v>12.75</v>
+      </c>
+      <c r="M136" s="15">
+        <f>SUM(L136+19.5)</f>
+        <v>32.25</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D137" s="13"/>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="J137" s="19">
-        <f>K136</f>
-        <v>0.59375</v>
-      </c>
-      <c r="K137" s="19">
-        <v>0.70138888888888884</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D138" s="13"/>
-      <c r="F138" s="2"/>
-      <c r="G138" s="2"/>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J137" s="19"/>
+      <c r="K137" s="19"/>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A138" s="21">
+        <v>22</v>
+      </c>
+      <c r="B138" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C138" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D138" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E138" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="F138" s="2">
+        <v>44464</v>
+      </c>
+      <c r="G138" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I138" s="15">
+        <f t="shared" ref="I138" si="30">ROUNDUP(((SUM(K138-J138)*24*60/60)/0.25),0)*0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="J138" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K138" s="19">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D139" s="13"/>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C140" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>302.75</v>
+        <v>304</v>
       </c>
       <c r="D140" s="14" t="s">
         <v>45</v>
@@ -5263,10 +5305,10 @@
       </c>
       <c r="G140" s="18">
         <f>SUM(I:I)</f>
-        <v>247.75</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D141" s="13" t="s">
         <v>131</v>
       </c>
@@ -5279,10 +5321,10 @@
       </c>
       <c r="G141" s="22">
         <f>315-G140</f>
-        <v>67.25</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>132</v>
       </c>
@@ -5291,7 +5333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A143" s="10"/>
       <c r="B143" s="10" t="s">
         <v>133</v>
@@ -5307,7 +5349,7 @@
       <c r="I143" s="10"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
[FEATURE] Add icons for the settings
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DF160B-C7B0-0140-8527-FB2DB3EC962B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDC68B5-B74E-B24C-8947-5299A013AD80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="156">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>Einführungsscreens</t>
+  </si>
+  <si>
+    <t>Einstellungsicons</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -548,6 +551,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -652,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -698,6 +707,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1014,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P143"/>
+  <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="L124" sqref="L124"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H138" sqref="H138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5270,7 +5282,7 @@
         <v>44481</v>
       </c>
       <c r="I138" s="15">
-        <f t="shared" ref="I138" si="30">ROUNDUP(((SUM(K138-J138)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I138:I139" si="30">ROUNDUP(((SUM(K138-J138)*24*60/60)/0.25),0)*0.25</f>
         <v>1.25</v>
       </c>
       <c r="J138" s="19">
@@ -5281,79 +5293,124 @@
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D139" s="13"/>
-      <c r="F139" s="2"/>
-      <c r="G139" s="2"/>
+      <c r="A139" s="21">
+        <v>22</v>
+      </c>
+      <c r="B139" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C139" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D139" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E139" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F139" s="24">
+        <v>44464</v>
+      </c>
+      <c r="G139" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H139" s="21"/>
+      <c r="I139" s="15">
+        <f t="shared" si="30"/>
+        <v>0.5</v>
+      </c>
+      <c r="J139" s="19">
+        <f>K138</f>
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="K139" s="29">
+        <v>0.53125</v>
+      </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B140" s="1" t="s">
+      <c r="D140" s="13"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D141" s="13"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D142" s="13"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B143" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C140" s="18">
+      <c r="C143" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>304</v>
-      </c>
-      <c r="D140" s="14" t="s">
+        <v>304.5</v>
+      </c>
+      <c r="D143" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E140" s="18">
+      <c r="E143" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F140" s="14" t="s">
+      <c r="F143" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G140" s="18">
+      <c r="G143" s="18">
         <f>SUM(I:I)</f>
-        <v>249</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D141" s="13" t="s">
+        <v>249.5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D144" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E141" s="22">
-        <f>135-E140</f>
+      <c r="E144" s="22">
+        <f>135-E143</f>
         <v>80</v>
       </c>
-      <c r="F141" s="13" t="s">
+      <c r="F144" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G141" s="22">
-        <f>315-G140</f>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B142" t="s">
+      <c r="G144" s="22">
+        <f>315-G143</f>
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B145" t="s">
         <v>132</v>
       </c>
-      <c r="C142">
-        <f>ROUNDUP(C140/30, 0)</f>
+      <c r="C145">
+        <f>ROUNDUP(C143/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="10"/>
-      <c r="B143" s="10" t="s">
+    <row r="146" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="10"/>
+      <c r="B146" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C143" s="10">
+      <c r="C146" s="10">
         <v>15</v>
       </c>
-      <c r="D143" s="10"/>
-      <c r="E143" s="10"/>
-      <c r="F143" s="10"/>
-      <c r="G143" s="10"/>
-      <c r="H143" s="10"/>
-      <c r="I143" s="10"/>
+      <c r="D146" s="10"/>
+      <c r="E146" s="10"/>
+      <c r="F146" s="10"/>
+      <c r="G146" s="10"/>
+      <c r="H146" s="10"/>
+      <c r="I146" s="10"/>
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D139" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D138 D140:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tutorial text tips
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDC68B5-B74E-B24C-8947-5299A013AD80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09926321-A4B1-FB4D-97B6-227CC168598A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="157">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -503,6 +503,9 @@
   </si>
   <si>
     <t>Einstellungsicons</t>
+  </si>
+  <si>
+    <t>Einführungskommentare</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H138" sqref="H138"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5328,9 +5331,39 @@
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D140" s="13"/>
-      <c r="F140" s="2"/>
-      <c r="G140" s="2"/>
+      <c r="A140" s="21">
+        <v>22</v>
+      </c>
+      <c r="B140" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C140" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D140" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="F140" s="24">
+        <v>44464</v>
+      </c>
+      <c r="G140" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H140" s="21"/>
+      <c r="I140" s="15">
+        <f t="shared" ref="I140" si="31">ROUNDUP(((SUM(K140-J140)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.5</v>
+      </c>
+      <c r="J140" s="19">
+        <f>K139</f>
+        <v>0.53125</v>
+      </c>
+      <c r="K140" s="29">
+        <v>0.55208333333333337</v>
+      </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D141" s="13"/>
@@ -5348,7 +5381,7 @@
       </c>
       <c r="C143" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>304.5</v>
+        <v>305</v>
       </c>
       <c r="D143" s="14" t="s">
         <v>45</v>
@@ -5362,7 +5395,7 @@
       </c>
       <c r="G143" s="18">
         <f>SUM(I:I)</f>
-        <v>249.5</v>
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
@@ -5378,7 +5411,7 @@
       </c>
       <c r="G144" s="22">
         <f>315-G143</f>
-        <v>65.5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -5410,7 +5443,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D138 D140:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D138 D141:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Change out profile images to stock image
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09926321-A4B1-FB4D-97B6-227CC168598A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192A212-F61D-C743-9541-D84E8821DED7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="158">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -506,6 +506,9 @@
   </si>
   <si>
     <t>Einführungskommentare</t>
+  </si>
+  <si>
+    <t>Bilder austauschen</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
   <dimension ref="A1:P146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="E141" sqref="E141"/>
+      <selection activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5305,7 +5308,7 @@
       <c r="C139" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D139" s="23" t="s">
+      <c r="D139" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E139" s="21" t="s">
@@ -5340,7 +5343,7 @@
       <c r="C140" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="D140" s="23" t="s">
+      <c r="D140" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E140" s="21" t="s">
@@ -5366,9 +5369,39 @@
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D141" s="13"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="2"/>
+      <c r="A141" s="21">
+        <v>22</v>
+      </c>
+      <c r="B141" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C141" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D141" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E141" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="F141" s="24">
+        <v>44464</v>
+      </c>
+      <c r="G141" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H141" s="21"/>
+      <c r="I141" s="15">
+        <f t="shared" ref="I141" si="32">ROUNDUP(((SUM(K141-J141)*24*60/60)/0.25),0)*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="J141" s="19">
+        <f>K140</f>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K141" s="29">
+        <v>0.5625</v>
+      </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D142" s="13"/>
@@ -5381,7 +5414,7 @@
       </c>
       <c r="C143" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>305</v>
+        <v>305.25</v>
       </c>
       <c r="D143" s="14" t="s">
         <v>45</v>
@@ -5395,7 +5428,7 @@
       </c>
       <c r="G143" s="18">
         <f>SUM(I:I)</f>
-        <v>250</v>
+        <v>250.25</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
@@ -5411,7 +5444,7 @@
       </c>
       <c r="G144" s="22">
         <f>315-G143</f>
-        <v>65</v>
+        <v>64.75</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.2">
@@ -5439,11 +5472,11 @@
       <c r="I146" s="10"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D138 D141:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Update folder structure and add tablet main screens
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192A212-F61D-C743-9541-D84E8821DED7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8349EE43-3E07-1D46-8487-814C78CEF2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="159">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -509,6 +509,9 @@
   </si>
   <si>
     <t>Bilder austauschen</t>
+  </si>
+  <si>
+    <t>Umbau von Ordner Struktur und anlegen von Tablets</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P146"/>
+  <dimension ref="A1:P147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
       <selection activeCell="I144" sqref="I144"/>
@@ -5392,7 +5395,7 @@
       </c>
       <c r="H141" s="21"/>
       <c r="I141" s="15">
-        <f t="shared" ref="I141" si="32">ROUNDUP(((SUM(K141-J141)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I141:I142" si="32">ROUNDUP(((SUM(K141-J141)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
       </c>
       <c r="J141" s="19">
@@ -5404,79 +5407,113 @@
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D142" s="13"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
+      <c r="A142" s="21">
+        <v>22</v>
+      </c>
+      <c r="B142" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C142" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D142" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="F142" s="24">
+        <v>44464</v>
+      </c>
+      <c r="G142" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H142" s="21"/>
+      <c r="I142" s="15">
+        <f t="shared" si="32"/>
+        <v>1.5</v>
+      </c>
+      <c r="J142" s="29">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="K142" s="29">
+        <v>0.61458333333333337</v>
+      </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B143" s="1" t="s">
+      <c r="D143" s="13"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B144" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C143" s="18">
+      <c r="C144" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>305.25</v>
-      </c>
-      <c r="D143" s="14" t="s">
+        <v>306.75</v>
+      </c>
+      <c r="D144" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E143" s="18">
+      <c r="E144" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F143" s="14" t="s">
+      <c r="F144" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G143" s="18">
+      <c r="G144" s="18">
         <f>SUM(I:I)</f>
-        <v>250.25</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D144" s="13" t="s">
+        <v>251.75</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D145" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E144" s="22">
-        <f>135-E143</f>
+      <c r="E145" s="22">
+        <f>135-E144</f>
         <v>80</v>
       </c>
-      <c r="F144" s="13" t="s">
+      <c r="F145" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G144" s="22">
-        <f>315-G143</f>
-        <v>64.75</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B145" t="s">
+      <c r="G145" s="22">
+        <f>315-G144</f>
+        <v>63.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B146" t="s">
         <v>132</v>
       </c>
-      <c r="C145">
-        <f>ROUNDUP(C143/30, 0)</f>
+      <c r="C146">
+        <f>ROUNDUP(C144/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="146" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="10"/>
-      <c r="B146" s="10" t="s">
+    <row r="147" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="10"/>
+      <c r="B147" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C146" s="10">
+      <c r="C147" s="10">
         <v>15</v>
       </c>
-      <c r="D146" s="10"/>
-      <c r="E146" s="10"/>
-      <c r="F146" s="10"/>
-      <c r="G146" s="10"/>
-      <c r="H146" s="10"/>
-      <c r="I146" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="10"/>
+      <c r="F147" s="10"/>
+      <c r="G147" s="10"/>
+      <c r="H147" s="10"/>
+      <c r="I147" s="10"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D142" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[TASK] Refine mock ups and styleguide
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8349EE43-3E07-1D46-8487-814C78CEF2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904241B6-72CA-C54A-95EE-3437B96D8C20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
     <sheet name="Projektplan rechnung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="161">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -512,6 +512,12 @@
   </si>
   <si>
     <t>Umbau von Ordner Struktur und anlegen von Tablets</t>
+  </si>
+  <si>
+    <t>Refinement und neue Todos</t>
+  </si>
+  <si>
+    <t>Tablet Card design</t>
   </si>
 </sst>
 </file>
@@ -1035,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P147"/>
+  <dimension ref="A1:P152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I144" sqref="I144"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="H147" sqref="H147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5406,7 +5412,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A142" s="21">
         <v>22</v>
       </c>
@@ -5439,81 +5445,170 @@
       <c r="K142" s="29">
         <v>0.61458333333333337</v>
       </c>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L142" s="26">
+        <f>SUM(H138:I142)</f>
+        <v>4</v>
+      </c>
+      <c r="M142" s="15">
+        <f>SUM(L142+19.5)</f>
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D143" s="13"/>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B144" s="1" t="s">
+      <c r="A144" s="21">
+        <v>22</v>
+      </c>
+      <c r="B144" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C144" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D144" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="F144" s="2">
+        <v>44481</v>
+      </c>
+      <c r="G144" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I144" s="15">
+        <f t="shared" ref="I144" si="33">ROUNDUP(((SUM(K144-J144)*24*60/60)/0.25),0)*0.25</f>
+        <v>3.5</v>
+      </c>
+      <c r="J144" s="19">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="K144" s="19">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" s="21">
+        <v>22</v>
+      </c>
+      <c r="B145" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C145" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D145" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F145" s="2">
+        <v>44481</v>
+      </c>
+      <c r="G145" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I145" s="15">
+        <f t="shared" ref="I145" si="34">ROUNDUP(((SUM(K145-J145)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.75</v>
+      </c>
+      <c r="J145" s="19">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K145" s="19">
+        <v>0.69791666666666663</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D146" s="13"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D147" s="13"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D148" s="13"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B149" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C144" s="18">
+      <c r="C149" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>306.75</v>
-      </c>
-      <c r="D144" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="D149" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E144" s="18">
+      <c r="E149" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F144" s="14" t="s">
+      <c r="F149" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G144" s="18">
+      <c r="G149" s="18">
         <f>SUM(I:I)</f>
-        <v>251.75</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D145" s="13" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D150" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E145" s="22">
-        <f>135-E144</f>
+      <c r="E150" s="22">
+        <f>135-E149</f>
         <v>80</v>
       </c>
-      <c r="F145" s="13" t="s">
+      <c r="F150" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G145" s="22">
-        <f>315-G144</f>
-        <v>63.25</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B146" t="s">
+      <c r="G150" s="22">
+        <f>315-G149</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B151" t="s">
         <v>132</v>
       </c>
-      <c r="C146">
-        <f>ROUNDUP(C144/30, 0)</f>
+      <c r="C151">
+        <f>ROUNDUP(C149/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="147" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="10"/>
-      <c r="B147" s="10" t="s">
+    <row r="152" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="10"/>
+      <c r="B152" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C147" s="10">
+      <c r="C152" s="10">
         <v>15</v>
       </c>
-      <c r="D147" s="10"/>
-      <c r="E147" s="10"/>
-      <c r="F147" s="10"/>
-      <c r="G147" s="10"/>
-      <c r="H147" s="10"/>
-      <c r="I147" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="10"/>
+      <c r="F152" s="10"/>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D148" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet card design and refine mobile cards
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904241B6-72CA-C54A-95EE-3437B96D8C20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D583AE4B-7049-6D41-8A97-071F912453E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
     <sheet name="Projektplan rechnung" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="162">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>Tablet Card design</t>
+  </si>
+  <si>
+    <t>Mobile and Tablet Card design</t>
   </si>
 </sst>
 </file>
@@ -1044,7 +1047,7 @@
   <dimension ref="A1:P152"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="H147" sqref="H147"/>
+      <selection activeCell="J152" sqref="J152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5531,9 +5534,37 @@
       <c r="G146" s="2"/>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D147" s="13"/>
-      <c r="F147" s="2"/>
-      <c r="G147" s="2"/>
+      <c r="A147" s="21">
+        <v>22</v>
+      </c>
+      <c r="B147" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C147" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D147" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F147" s="2">
+        <v>44489</v>
+      </c>
+      <c r="G147" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I147" s="15">
+        <f t="shared" ref="I147" si="35">ROUNDUP(((SUM(K147-J147)*24*60/60)/0.25),0)*0.25</f>
+        <v>5.75</v>
+      </c>
+      <c r="J147" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K147" s="19">
+        <v>0.69791666666666663</v>
+      </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D148" s="13"/>
@@ -5546,7 +5577,7 @@
       </c>
       <c r="C149" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>313</v>
+        <v>318.75</v>
       </c>
       <c r="D149" s="14" t="s">
         <v>45</v>
@@ -5560,7 +5591,7 @@
       </c>
       <c r="G149" s="18">
         <f>SUM(I:I)</f>
-        <v>258</v>
+        <v>263.75</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
@@ -5576,7 +5607,7 @@
       </c>
       <c r="G150" s="22">
         <f>315-G149</f>
-        <v>57</v>
+        <v>51.25</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[FEATURE] Add tablet homescreen and own profile
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D583AE4B-7049-6D41-8A97-071F912453E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAE3A39-B960-974E-86C4-8F223C305B96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="164">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>Mobile and Tablet Card design</t>
+  </si>
+  <si>
+    <t>Mobile refinement</t>
+  </si>
+  <si>
+    <t>Tablet Startseite und Profilübersicht</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P152"/>
+  <dimension ref="A1:P155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="J152" sqref="J152"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I155" sqref="I155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5567,79 +5573,150 @@
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D148" s="13"/>
-      <c r="F148" s="2"/>
-      <c r="G148" s="2"/>
+      <c r="A148" s="21">
+        <v>22</v>
+      </c>
+      <c r="B148" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C148" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D148" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="F148" s="2">
+        <v>44491</v>
+      </c>
+      <c r="G148" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I148" s="15">
+        <f t="shared" ref="I148" si="36">ROUNDUP(((SUM(K148-J148)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J148" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K148" s="19">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B149" s="1" t="s">
+      <c r="A149" s="21">
+        <v>22</v>
+      </c>
+      <c r="B149" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C149" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D149" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E149" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F149" s="2">
+        <v>44491</v>
+      </c>
+      <c r="G149" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I149" s="15">
+        <f t="shared" ref="I149" si="37">ROUNDUP(((SUM(K149-J149)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="J149" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="K149" s="19">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D150" s="13"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D151" s="13"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B152" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C149" s="18">
+      <c r="C152" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>318.75</v>
-      </c>
-      <c r="D149" s="14" t="s">
+        <v>323.75</v>
+      </c>
+      <c r="D152" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E149" s="18">
+      <c r="E152" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F149" s="14" t="s">
+      <c r="F152" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G149" s="18">
+      <c r="G152" s="18">
         <f>SUM(I:I)</f>
-        <v>263.75</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D150" s="13" t="s">
+        <v>268.75</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D153" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E150" s="22">
-        <f>135-E149</f>
+      <c r="E153" s="22">
+        <f>135-E152</f>
         <v>80</v>
       </c>
-      <c r="F150" s="13" t="s">
+      <c r="F153" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G150" s="22">
-        <f>315-G149</f>
-        <v>51.25</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B151" t="s">
+      <c r="G153" s="22">
+        <f>315-G152</f>
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B154" t="s">
         <v>132</v>
       </c>
-      <c r="C151">
-        <f>ROUNDUP(C149/30, 0)</f>
+      <c r="C154">
+        <f>ROUNDUP(C152/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="10"/>
-      <c r="B152" s="10" t="s">
+    <row r="155" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="10"/>
+      <c r="B155" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C152" s="10">
+      <c r="C155" s="10">
         <v>15</v>
       </c>
-      <c r="D152" s="10"/>
-      <c r="E152" s="10"/>
-      <c r="F152" s="10"/>
-      <c r="G152" s="10"/>
-      <c r="H152" s="10"/>
-      <c r="I152" s="10"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+      <c r="F155" s="10"/>
+      <c r="G155" s="10"/>
+      <c r="H155" s="10"/>
+      <c r="I155" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D148" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D151" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet cookbook overview
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAE3A39-B960-974E-86C4-8F223C305B96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AA3273-971F-7144-B4B5-42EF8C04B8BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="165">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t>Tablet Startseite und Profilübersicht</t>
+  </si>
+  <si>
+    <t>Tablet Mein Kochbuch</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P155"/>
+  <dimension ref="A1:P156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I155" sqref="I155"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I156" sqref="I156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5639,9 +5642,37 @@
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D150" s="13"/>
-      <c r="F150" s="2"/>
-      <c r="G150" s="2"/>
+      <c r="A150" s="21">
+        <v>22</v>
+      </c>
+      <c r="B150" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C150" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D150" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E150" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="F150" s="2">
+        <v>44492</v>
+      </c>
+      <c r="G150" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I150" s="15">
+        <f t="shared" ref="I150" si="38">ROUNDUP(((SUM(K150-J150)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.5</v>
+      </c>
+      <c r="J150" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="K150" s="19">
+        <v>0.60416666666666663</v>
+      </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D151" s="13"/>
@@ -5649,74 +5680,79 @@
       <c r="G151" s="2"/>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B152" s="1" t="s">
+      <c r="D152" s="13"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B153" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C152" s="18">
+      <c r="C153" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>323.75</v>
-      </c>
-      <c r="D152" s="14" t="s">
+        <v>326.25</v>
+      </c>
+      <c r="D153" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E152" s="18">
+      <c r="E153" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F152" s="14" t="s">
+      <c r="F153" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G152" s="18">
+      <c r="G153" s="18">
         <f>SUM(I:I)</f>
-        <v>268.75</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D153" s="13" t="s">
+        <v>271.25</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D154" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E153" s="22">
-        <f>135-E152</f>
+      <c r="E154" s="22">
+        <f>135-E153</f>
         <v>80</v>
       </c>
-      <c r="F153" s="13" t="s">
+      <c r="F154" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G153" s="22">
-        <f>315-G152</f>
-        <v>46.25</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B154" t="s">
+      <c r="G154" s="22">
+        <f>315-G153</f>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B155" t="s">
         <v>132</v>
       </c>
-      <c r="C154">
-        <f>ROUNDUP(C152/30, 0)</f>
+      <c r="C155">
+        <f>ROUNDUP(C153/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="155" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="10"/>
-      <c r="B155" s="10" t="s">
+    <row r="156" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="10"/>
+      <c r="B156" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C155" s="10">
+      <c r="C156" s="10">
         <v>15</v>
       </c>
-      <c r="D155" s="10"/>
-      <c r="E155" s="10"/>
-      <c r="F155" s="10"/>
-      <c r="G155" s="10"/>
-      <c r="H155" s="10"/>
-      <c r="I155" s="10"/>
+      <c r="D156" s="10"/>
+      <c r="E156" s="10"/>
+      <c r="F156" s="10"/>
+      <c r="G156" s="10"/>
+      <c r="H156" s="10"/>
+      <c r="I156" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D151" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D152" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet settings screens
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03AA3273-971F-7144-B4B5-42EF8C04B8BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D642FAF-6B51-4B46-A30C-3FB4B1B98645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="166">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -530,6 +530,9 @@
   </si>
   <si>
     <t>Tablet Mein Kochbuch</t>
+  </si>
+  <si>
+    <t>Tablet Album und Kochbuch Einstellungen</t>
   </si>
 </sst>
 </file>
@@ -1053,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P156"/>
+  <dimension ref="A1:P159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I156" sqref="I156"/>
+      <selection activeCell="I159" sqref="A1:I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5680,79 +5683,122 @@
       <c r="G151" s="2"/>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D152" s="13"/>
-      <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
+      <c r="A152" s="21">
+        <v>22</v>
+      </c>
+      <c r="B152" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C152" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D152" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E152" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="F152" s="2">
+        <v>44494</v>
+      </c>
+      <c r="G152" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I152" s="15">
+        <f t="shared" ref="I152" si="39">ROUNDUP(((SUM(K152-J152)*24*60/60)/0.25),0)*0.25</f>
+        <v>2.5</v>
+      </c>
+      <c r="J152" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="K152" s="19">
+        <v>0.60416666666666663</v>
+      </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B153" s="1" t="s">
+      <c r="D153" s="13"/>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D154" s="13"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D155" s="13"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="2"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B156" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C153" s="18">
+      <c r="C156" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>326.25</v>
-      </c>
-      <c r="D153" s="14" t="s">
+        <v>328.75</v>
+      </c>
+      <c r="D156" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E153" s="18">
+      <c r="E156" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F153" s="14" t="s">
+      <c r="F156" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G153" s="18">
+      <c r="G156" s="18">
         <f>SUM(I:I)</f>
-        <v>271.25</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D154" s="13" t="s">
+        <v>273.75</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D157" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E154" s="22">
-        <f>135-E153</f>
+      <c r="E157" s="22">
+        <f>135-E156</f>
         <v>80</v>
       </c>
-      <c r="F154" s="13" t="s">
+      <c r="F157" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G154" s="22">
-        <f>315-G153</f>
-        <v>43.75</v>
-      </c>
-    </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B155" t="s">
+      <c r="G157" s="22">
+        <f>315-G156</f>
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B158" t="s">
         <v>132</v>
       </c>
-      <c r="C155">
-        <f>ROUNDUP(C153/30, 0)</f>
+      <c r="C158">
+        <f>ROUNDUP(C156/30, 0)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="156" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="10"/>
-      <c r="B156" s="10" t="s">
+    <row r="159" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="10"/>
+      <c r="B159" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C156" s="10">
+      <c r="C159" s="10">
         <v>15</v>
       </c>
-      <c r="D156" s="10"/>
-      <c r="E156" s="10"/>
-      <c r="F156" s="10"/>
-      <c r="G156" s="10"/>
-      <c r="H156" s="10"/>
-      <c r="I156" s="10"/>
+      <c r="D159" s="10"/>
+      <c r="E159" s="10"/>
+      <c r="F159" s="10"/>
+      <c r="G159" s="10"/>
+      <c r="H159" s="10"/>
+      <c r="I159" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D152" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D155" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet edit recipe and modify mobile versions
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D642FAF-6B51-4B46-A30C-3FB4B1B98645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988EB7B5-8511-AE4A-8D26-F300A22DADB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="167">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>Tablet Album und Kochbuch Einstellungen</t>
+  </si>
+  <si>
+    <t>Tablet und Mobile Rezept bearbeiten</t>
   </si>
 </sst>
 </file>
@@ -1058,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
   <dimension ref="A1:P159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="I159" sqref="A1:I159"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5716,9 +5719,37 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D153" s="13"/>
-      <c r="F153" s="2"/>
-      <c r="G153" s="2"/>
+      <c r="A153" s="21">
+        <v>22</v>
+      </c>
+      <c r="B153" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C153" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D153" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="F153" s="2">
+        <v>44499</v>
+      </c>
+      <c r="G153" s="2">
+        <v>44481</v>
+      </c>
+      <c r="I153" s="15">
+        <f t="shared" ref="I153" si="40">ROUNDUP(((SUM(K153-J153)*24*60/60)/0.25),0)*0.25</f>
+        <v>4.5</v>
+      </c>
+      <c r="J153" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K153" s="19">
+        <v>0.64583333333333337</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D154" s="13"/>
@@ -5736,7 +5767,7 @@
       </c>
       <c r="C156" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>328.75</v>
+        <v>333.25</v>
       </c>
       <c r="D156" s="14" t="s">
         <v>45</v>
@@ -5750,7 +5781,7 @@
       </c>
       <c r="G156" s="18">
         <f>SUM(I:I)</f>
-        <v>273.75</v>
+        <v>278.25</v>
       </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
@@ -5766,7 +5797,7 @@
       </c>
       <c r="G157" s="22">
         <f>315-G156</f>
-        <v>41.25</v>
+        <v>36.75</v>
       </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
@@ -5775,7 +5806,7 @@
       </c>
       <c r="C158">
         <f>ROUNDUP(C156/30, 0)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[FEATURE] Add tablet recipe views and modify mobile versions
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988EB7B5-8511-AE4A-8D26-F300A22DADB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C115581-C359-0D4D-B78F-BD719EE254F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
   <sheets>
     <sheet name="Arbeitsmatrix" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="169">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -536,6 +536,12 @@
   </si>
   <si>
     <t>Tablet und Mobile Rezept bearbeiten</t>
+  </si>
+  <si>
+    <t>Tablet und Mobile Rezept ansicht</t>
+  </si>
+  <si>
+    <t>Tablet und Mobile Profile</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P159"/>
+  <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="G155" sqref="G155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5741,7 +5747,7 @@
         <v>44481</v>
       </c>
       <c r="I153" s="15">
-        <f t="shared" ref="I153" si="40">ROUNDUP(((SUM(K153-J153)*24*60/60)/0.25),0)*0.25</f>
+        <f t="shared" ref="I153:I156" si="40">ROUNDUP(((SUM(K153-J153)*24*60/60)/0.25),0)*0.25</f>
         <v>4.5</v>
       </c>
       <c r="J153" s="19">
@@ -5757,79 +5763,153 @@
       <c r="G154" s="2"/>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D155" s="13"/>
-      <c r="F155" s="2"/>
-      <c r="G155" s="2"/>
+      <c r="A155" s="21">
+        <v>22</v>
+      </c>
+      <c r="B155" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C155" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D155" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E155" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="F155" s="24">
+        <v>44501</v>
+      </c>
+      <c r="G155" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H155" s="21"/>
+      <c r="I155" s="15">
+        <f t="shared" si="40"/>
+        <v>3.5</v>
+      </c>
+      <c r="J155" s="29">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K155" s="29">
+        <v>0.60416666666666663</v>
+      </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B156" s="1" t="s">
+      <c r="A156" s="21">
+        <v>22</v>
+      </c>
+      <c r="B156" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C156" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D156" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E156" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="F156" s="24">
+        <v>44501</v>
+      </c>
+      <c r="G156" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H156" s="21"/>
+      <c r="I156" s="15">
+        <f t="shared" si="40"/>
+        <v>2.25</v>
+      </c>
+      <c r="J156" s="19">
+        <f>K155</f>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="K156" s="29">
+        <v>0.69791666666666663</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D157" s="13"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D158" s="13"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B159" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C156" s="18">
+      <c r="C159" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>333.25</v>
-      </c>
-      <c r="D156" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="D159" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E156" s="18">
+      <c r="E159" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F156" s="14" t="s">
+      <c r="F159" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G156" s="18">
+      <c r="G159" s="18">
         <f>SUM(I:I)</f>
-        <v>278.25</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D157" s="13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D160" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E157" s="22">
-        <f>135-E156</f>
+      <c r="E160" s="22">
+        <f>135-E159</f>
         <v>80</v>
       </c>
-      <c r="F157" s="13" t="s">
+      <c r="F160" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G157" s="22">
-        <f>315-G156</f>
-        <v>36.75</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B158" t="s">
+      <c r="G160" s="22">
+        <f>315-G159</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B161" t="s">
         <v>132</v>
       </c>
-      <c r="C158">
-        <f>ROUNDUP(C156/30, 0)</f>
+      <c r="C161">
+        <f>ROUNDUP(C159/30, 0)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="10"/>
-      <c r="B159" s="10" t="s">
+    <row r="162" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="10"/>
+      <c r="B162" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C159" s="10">
+      <c r="C162" s="10">
         <v>15</v>
       </c>
-      <c r="D159" s="10"/>
-      <c r="E159" s="10"/>
-      <c r="F159" s="10"/>
-      <c r="G159" s="10"/>
-      <c r="H159" s="10"/>
-      <c r="I159" s="10"/>
+      <c r="D162" s="10"/>
+      <c r="E162" s="10"/>
+      <c r="F162" s="10"/>
+      <c r="G162" s="10"/>
+      <c r="H162" s="10"/>
+      <c r="I162" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D155" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D157:D158" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet cookbook views and modify mobile versions
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrrobot/Documents/GitHub/PPSS21Mai/Artefakte/Zeiterfassung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C115581-C359-0D4D-B78F-BD719EE254F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455DAB9D-E55F-E241-ACD7-28FB570A705E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{1643B313-5BB8-5844-9818-3B05D1C17679}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="171">
   <si>
     <t>Issue Nr</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>Tablet und Mobile Profile</t>
+  </si>
+  <si>
+    <t>Tablet und Mobile Freundschaftsanfragen und Einstellungen</t>
+  </si>
+  <si>
+    <t>Tablet und Mobile Mein Kochbuch und Untermenues</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17511CF7-E337-9E45-A616-16F66912E25D}">
-  <dimension ref="A1:P162"/>
+  <dimension ref="A1:P166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="G155" sqref="G155"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="138" workbookViewId="0">
+      <selection activeCell="I166" sqref="I166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5473,9 +5479,9 @@
         <f>SUM(H138:I142)</f>
         <v>4</v>
       </c>
-      <c r="M142" s="15">
-        <f>SUM(L142+19.5)</f>
-        <v>23.5</v>
+      <c r="M142">
+        <f>SUM(L142+16)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -5516,7 +5522,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A145" s="21">
         <v>22</v>
       </c>
@@ -5548,13 +5554,21 @@
       <c r="K145" s="19">
         <v>0.69791666666666663</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L145" s="26">
+        <f>SUM(H144:I145)</f>
+        <v>6.25</v>
+      </c>
+      <c r="M145">
+        <f>SUM(L145+16)</f>
+        <v>22.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D146" s="13"/>
       <c r="F146" s="2"/>
       <c r="G146" s="2"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" s="21">
         <v>22</v>
       </c>
@@ -5587,7 +5601,7 @@
         <v>0.69791666666666663</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" s="21">
         <v>22</v>
       </c>
@@ -5620,7 +5634,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" s="21">
         <v>22</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A150" s="21">
         <v>22</v>
       </c>
@@ -5685,13 +5699,21 @@
       <c r="K150" s="19">
         <v>0.60416666666666663</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L150" s="26">
+        <f>SUM(H147:I150)</f>
+        <v>13.25</v>
+      </c>
+      <c r="M150">
+        <f>SUM(L150+16)</f>
+        <v>29.25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D151" s="13"/>
       <c r="F151" s="2"/>
       <c r="G151" s="2"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" s="21">
         <v>22</v>
       </c>
@@ -5724,7 +5746,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A153" s="21">
         <v>22</v>
       </c>
@@ -5756,13 +5778,21 @@
       <c r="K153" s="19">
         <v>0.64583333333333337</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L153" s="26">
+        <f>SUM(H152:I153)</f>
+        <v>7</v>
+      </c>
+      <c r="M153">
+        <f>SUM(L153+16)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="D154" s="13"/>
       <c r="F154" s="2"/>
       <c r="G154" s="2"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" s="21">
         <v>22</v>
       </c>
@@ -5796,7 +5826,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A156" s="21">
         <v>22</v>
       </c>
@@ -5830,86 +5860,188 @@
       <c r="K156" s="29">
         <v>0.69791666666666663</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D157" s="13"/>
-      <c r="F157" s="2"/>
-      <c r="G157" s="2"/>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D158" s="13"/>
-      <c r="F158" s="2"/>
-      <c r="G158" s="2"/>
-    </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B159" s="1" t="s">
+      <c r="L156" s="26">
+        <f>SUM(H155:I156)</f>
+        <v>5.75</v>
+      </c>
+      <c r="M156">
+        <f>SUM(L156+16)</f>
+        <v>21.75</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="21"/>
+      <c r="B157" s="21"/>
+      <c r="C157" s="21"/>
+      <c r="D157" s="23"/>
+      <c r="E157" s="21"/>
+      <c r="F157" s="24"/>
+      <c r="G157" s="24"/>
+      <c r="H157" s="21"/>
+      <c r="I157" s="15"/>
+      <c r="J157" s="19"/>
+      <c r="K157" s="29"/>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A158" s="21">
+        <v>22</v>
+      </c>
+      <c r="B158" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C158" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D158" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E158" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="F158" s="24">
+        <v>44508</v>
+      </c>
+      <c r="G158" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H158" s="21"/>
+      <c r="I158" s="15">
+        <f t="shared" ref="I158" si="41">ROUNDUP(((SUM(K158-J158)*24*60/60)/0.25),0)*0.25</f>
+        <v>3</v>
+      </c>
+      <c r="J158" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K158" s="29">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="21">
+        <v>22</v>
+      </c>
+      <c r="B159" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C159" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D159" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E159" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="F159" s="24">
+        <v>44509</v>
+      </c>
+      <c r="G159" s="24">
+        <v>44481</v>
+      </c>
+      <c r="H159" s="21"/>
+      <c r="I159" s="15">
+        <f t="shared" ref="I159" si="42">ROUNDUP(((SUM(K159-J159)*24*60/60)/0.25),0)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="J159" s="19">
+        <v>0.5</v>
+      </c>
+      <c r="K159" s="29">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L159" s="26">
+        <f>SUM(H158:I159)</f>
+        <v>7</v>
+      </c>
+      <c r="M159">
+        <f>SUM(L159+16)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D160" s="13"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D161" s="13"/>
+      <c r="F161" s="2"/>
+      <c r="G161" s="2"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D162" s="13"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="2"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B163" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C159" s="18">
+      <c r="C163" s="18">
         <f>SUM(I:I)+SUM(H:H)</f>
-        <v>339</v>
-      </c>
-      <c r="D159" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="D163" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E159" s="18">
+      <c r="E163" s="18">
         <f>SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F159" s="14" t="s">
+      <c r="F163" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="G159" s="18">
+      <c r="G163" s="18">
         <f>SUM(I:I)</f>
-        <v>284</v>
-      </c>
-    </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D160" s="13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D164" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E160" s="22">
-        <f>135-E159</f>
+      <c r="E164" s="22">
+        <f>135-E163</f>
         <v>80</v>
       </c>
-      <c r="F160" s="13" t="s">
+      <c r="F164" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="G160" s="22">
-        <f>315-G159</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B161" t="s">
+      <c r="G164" s="22">
+        <f>315-G163</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B165" t="s">
         <v>132</v>
       </c>
-      <c r="C161">
-        <f>ROUNDUP(C159/30, 0)</f>
+      <c r="C165">
+        <f>ROUNDUP(C163/30, 0)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="10"/>
-      <c r="B162" s="10" t="s">
+    <row r="166" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="10"/>
+      <c r="B166" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C162" s="10">
+      <c r="C166" s="10">
         <v>15</v>
       </c>
-      <c r="D162" s="10"/>
-      <c r="E162" s="10"/>
-      <c r="F162" s="10"/>
-      <c r="G162" s="10"/>
-      <c r="H162" s="10"/>
-      <c r="I162" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="10"/>
+      <c r="F166" s="10"/>
+      <c r="G166" s="10"/>
+      <c r="H166" s="10"/>
+      <c r="I166" s="10"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D4:D12 D18:D21 D28:D34 D37:D40" xr:uid="{D855B4B3-52DF-7445-9249-7A409F05BF2B}">
       <formula1>$N$3:$N$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D157:D158" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Prefix nicht unterstützt" error="Es konnte kein korrekter Prefix ausgegeben werden_x000a_" promptTitle="Prefix" prompt="Wählen Sie einen Prefix aus" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160:D162" xr:uid="{6F8E02CB-534C-AB4D-A4E7-36DF02FD6C81}">
       <formula1>$N$3:$N$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[FEATURE] Add tablet new recipe screens
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="173">
   <si>
     <t xml:space="preserve">Issue Nr</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tablet neues Rezept anlegen screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tablet neues Rezept anlegen screens</t>
   </si>
   <si>
     <t xml:space="preserve">Stunden insgesamt</t>
@@ -701,7 +704,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,10 +759,6 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -899,13 +898,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P167"/>
+  <dimension ref="A1:P168"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E164" activeCellId="0" sqref="E164"/>
+      <selection pane="topLeft" activeCell="G164" activeCellId="0" sqref="G164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.84"/>
@@ -1251,7 +1250,6 @@
       <c r="K11" s="13" t="n">
         <v>0.722222222222222</v>
       </c>
-      <c r="L11" s="14"/>
       <c r="M11" s="12"/>
       <c r="P11" s="12"/>
     </row>
@@ -1288,7 +1286,6 @@
       <c r="K12" s="13" t="n">
         <v>0.739583333333333</v>
       </c>
-      <c r="L12" s="14"/>
       <c r="M12" s="12"/>
       <c r="P12" s="12"/>
     </row>
@@ -2468,7 +2465,7 @@
       <c r="K49" s="13" t="n">
         <v>0.822916666666667</v>
       </c>
-      <c r="L49" s="15" t="n">
+      <c r="L49" s="14" t="n">
         <f aca="false">SUM(H41:I49)</f>
         <v>30</v>
       </c>
@@ -2714,7 +2711,7 @@
       <c r="K57" s="13" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="L57" s="15" t="n">
+      <c r="L57" s="14" t="n">
         <f aca="false">SUM(H49:I57)</f>
         <v>23</v>
       </c>
@@ -3031,7 +3028,7 @@
       <c r="K67" s="13" t="n">
         <v>0.583333333333333</v>
       </c>
-      <c r="L67" s="15" t="n">
+      <c r="L67" s="14" t="n">
         <f aca="false">SUM(H59:I67)</f>
         <v>22.75</v>
       </c>
@@ -3182,7 +3179,7 @@
       <c r="K72" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="L72" s="15" t="n">
+      <c r="L72" s="14" t="n">
         <f aca="false">SUM(H69:I72)</f>
         <v>13.5</v>
       </c>
@@ -3401,7 +3398,7 @@
       <c r="K79" s="13" t="n">
         <v>0.583333333333333</v>
       </c>
-      <c r="L79" s="15" t="n">
+      <c r="L79" s="14" t="n">
         <f aca="false">SUM(H74:I79)</f>
         <v>16</v>
       </c>
@@ -3554,19 +3551,19 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="16" t="n">
+      <c r="A85" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B85" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C85" s="16" t="s">
+      <c r="B85" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="15" t="s">
         <v>100</v>
       </c>
       <c r="F85" s="7" t="n">
@@ -3588,19 +3585,19 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="16" t="n">
+      <c r="A86" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B86" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C86" s="16" t="s">
+      <c r="B86" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="15" t="s">
         <v>101</v>
       </c>
       <c r="F86" s="7" t="n">
@@ -3620,7 +3617,7 @@
       <c r="K86" s="13" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="L86" s="15" t="n">
+      <c r="L86" s="14" t="n">
         <f aca="false">SUM(H81:I86)</f>
         <v>25.5</v>
       </c>
@@ -3671,19 +3668,19 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="16" t="n">
+      <c r="A89" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B89" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C89" s="16" t="s">
+      <c r="B89" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="E89" s="15" t="s">
         <v>103</v>
       </c>
       <c r="F89" s="7" t="n">
@@ -3705,19 +3702,19 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="16" t="n">
+      <c r="A90" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C90" s="16" t="s">
+      <c r="B90" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D90" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="15" t="s">
         <v>104</v>
       </c>
       <c r="F90" s="7" t="n">
@@ -3739,19 +3736,19 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="16" t="n">
+      <c r="A91" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B91" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C91" s="16" t="s">
+      <c r="B91" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C91" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="E91" s="15" t="s">
         <v>105</v>
       </c>
       <c r="F91" s="7" t="n">
@@ -3773,19 +3770,19 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="16" t="n">
+      <c r="A92" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B92" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C92" s="16" t="s">
+      <c r="B92" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C92" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D92" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="15" t="s">
         <v>106</v>
       </c>
       <c r="F92" s="7" t="n">
@@ -3807,19 +3804,19 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="16" t="n">
+      <c r="A93" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B93" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C93" s="16" t="s">
+      <c r="B93" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F93" s="7" t="n">
@@ -3841,19 +3838,19 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="16" t="n">
+      <c r="A94" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B94" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C94" s="16" t="s">
+      <c r="B94" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C94" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F94" s="7" t="n">
@@ -3873,7 +3870,7 @@
       <c r="K94" s="13" t="n">
         <v>0.75</v>
       </c>
-      <c r="L94" s="15" t="n">
+      <c r="L94" s="14" t="n">
         <f aca="false">SUM(H89:I94)</f>
         <v>17.5</v>
       </c>
@@ -3890,19 +3887,19 @@
       <c r="I95" s="12"/>
     </row>
     <row r="96" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="16" t="n">
+      <c r="A96" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B96" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C96" s="16" t="s">
+      <c r="B96" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C96" s="15" t="s">
         <v>96</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="15" t="s">
         <v>108</v>
       </c>
       <c r="F96" s="7" t="n">
@@ -3958,19 +3955,19 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="16" t="n">
+      <c r="A98" s="15" t="n">
         <v>21</v>
       </c>
       <c r="B98" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C98" s="16" t="s">
+      <c r="C98" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="15" t="s">
         <v>110</v>
       </c>
       <c r="F98" s="7" t="n">
@@ -3992,19 +3989,19 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="16" t="n">
+      <c r="A99" s="15" t="n">
         <v>21</v>
       </c>
       <c r="B99" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C99" s="16" t="s">
+      <c r="C99" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E99" s="15" t="s">
         <v>111</v>
       </c>
       <c r="F99" s="7" t="n">
@@ -4026,19 +4023,19 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="16" t="n">
+      <c r="A100" s="15" t="n">
         <v>22</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C100" s="16" t="s">
+      <c r="C100" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F100" s="7" t="n">
@@ -4060,19 +4057,19 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="16" t="n">
+      <c r="A101" s="15" t="n">
         <v>23</v>
       </c>
       <c r="B101" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C101" s="16" t="s">
+      <c r="C101" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="15" t="s">
         <v>113</v>
       </c>
       <c r="F101" s="7" t="n">
@@ -4094,19 +4091,19 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="16" t="n">
+      <c r="A102" s="15" t="n">
         <v>22</v>
       </c>
       <c r="B102" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C102" s="16" t="s">
+      <c r="C102" s="15" t="s">
         <v>109</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E102" s="15" t="s">
         <v>112</v>
       </c>
       <c r="F102" s="7" t="n">
@@ -4128,19 +4125,19 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="16" t="n">
+      <c r="A103" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B103" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C103" s="16" t="s">
+      <c r="B103" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C103" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="E103" s="15" t="s">
         <v>115</v>
       </c>
       <c r="F103" s="7" t="n">
@@ -4160,7 +4157,7 @@
       <c r="K103" s="13" t="n">
         <v>0.791666666666667</v>
       </c>
-      <c r="L103" s="15" t="n">
+      <c r="L103" s="14" t="n">
         <f aca="false">SUM(H96:I103)</f>
         <v>29</v>
       </c>
@@ -4174,19 +4171,19 @@
       <c r="G104" s="7"/>
     </row>
     <row r="105" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="16" t="n">
+      <c r="A105" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B105" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C105" s="16" t="s">
+      <c r="B105" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C105" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="E105" s="15" t="s">
         <v>116</v>
       </c>
       <c r="F105" s="7" t="n">
@@ -4207,19 +4204,19 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="16" t="n">
+      <c r="A106" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B106" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C106" s="16" t="s">
+      <c r="B106" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C106" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="E106" s="15" t="s">
         <v>117</v>
       </c>
       <c r="F106" s="7" t="n">
@@ -4339,19 +4336,19 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="16" t="n">
+      <c r="A110" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B110" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C110" s="16" t="s">
+      <c r="B110" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="E110" s="15" t="s">
         <v>120</v>
       </c>
       <c r="F110" s="7" t="n">
@@ -4372,19 +4369,19 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="16" t="n">
+      <c r="A111" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B111" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C111" s="16" t="s">
+      <c r="B111" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C111" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E111" s="16" t="s">
+      <c r="E111" s="15" t="s">
         <v>120</v>
       </c>
       <c r="F111" s="7" t="n">
@@ -4436,7 +4433,7 @@
       <c r="K112" s="13" t="n">
         <v>0.708333333333333</v>
       </c>
-      <c r="L112" s="15" t="n">
+      <c r="L112" s="14" t="n">
         <f aca="false">SUM(H105:I112)</f>
         <v>17.5</v>
       </c>
@@ -4451,25 +4448,25 @@
       <c r="G113" s="7"/>
     </row>
     <row r="114" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="16" t="n">
+      <c r="A114" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C114" s="16" t="s">
+      <c r="C114" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E114" s="16" t="s">
+      <c r="E114" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="F114" s="17" t="n">
+      <c r="F114" s="16" t="n">
         <v>44382</v>
       </c>
-      <c r="G114" s="17" t="n">
+      <c r="G114" s="16" t="n">
         <v>44359</v>
       </c>
       <c r="I114" s="12" t="n">
@@ -4504,19 +4501,19 @@
       <c r="G117" s="7"/>
     </row>
     <row r="118" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="16" t="n">
+      <c r="A118" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B118" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C118" s="16" t="s">
+      <c r="B118" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C118" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E118" s="16" t="s">
+      <c r="E118" s="15" t="s">
         <v>123</v>
       </c>
       <c r="F118" s="7" t="n">
@@ -4537,19 +4534,19 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="16" t="n">
+      <c r="A119" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B119" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C119" s="16" t="s">
+      <c r="B119" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C119" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E119" s="16" t="s">
+      <c r="E119" s="15" t="s">
         <v>124</v>
       </c>
       <c r="F119" s="7" t="n">
@@ -4570,19 +4567,19 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="16" t="n">
+      <c r="A120" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B120" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C120" s="16" t="s">
+      <c r="B120" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C120" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E120" s="16" t="s">
+      <c r="E120" s="15" t="s">
         <v>125</v>
       </c>
       <c r="F120" s="7" t="n">
@@ -4603,19 +4600,19 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="16" t="n">
+      <c r="A121" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B121" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C121" s="16" t="s">
+      <c r="B121" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C121" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D121" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E121" s="16" t="s">
+      <c r="E121" s="15" t="s">
         <v>126</v>
       </c>
       <c r="F121" s="7" t="n">
@@ -4636,19 +4633,19 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="16" t="n">
+      <c r="A122" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B122" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C122" s="16" t="s">
+      <c r="B122" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E122" s="16" t="s">
+      <c r="E122" s="15" t="s">
         <v>127</v>
       </c>
       <c r="F122" s="7" t="n">
@@ -4669,19 +4666,19 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="16" t="n">
+      <c r="A123" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B123" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C123" s="16" t="s">
+      <c r="B123" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C123" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E123" s="16" t="s">
+      <c r="E123" s="15" t="s">
         <v>128</v>
       </c>
       <c r="F123" s="7" t="n">
@@ -4702,19 +4699,19 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="16" t="n">
+      <c r="A124" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B124" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C124" s="16" t="s">
+      <c r="B124" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C124" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E124" s="16" t="s">
+      <c r="E124" s="15" t="s">
         <v>129</v>
       </c>
       <c r="F124" s="7" t="n">
@@ -4733,7 +4730,7 @@
       <c r="K124" s="13" t="n">
         <v>0.555555555555556</v>
       </c>
-      <c r="L124" s="15" t="n">
+      <c r="L124" s="14" t="n">
         <f aca="false">SUM(H114:I124)</f>
         <v>23.25</v>
       </c>
@@ -4748,19 +4745,19 @@
       <c r="G125" s="7"/>
     </row>
     <row r="126" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="16" t="n">
+      <c r="A126" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B126" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C126" s="16" t="s">
+      <c r="B126" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C126" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D126" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E126" s="16" t="s">
+      <c r="E126" s="15" t="s">
         <v>130</v>
       </c>
       <c r="F126" s="7" t="n">
@@ -4781,19 +4778,19 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="16" t="n">
+      <c r="A127" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B127" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C127" s="16" t="s">
+      <c r="B127" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C127" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E127" s="16" t="s">
+      <c r="E127" s="15" t="s">
         <v>131</v>
       </c>
       <c r="F127" s="7" t="n">
@@ -4815,19 +4812,19 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="16" t="n">
+      <c r="A128" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B128" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C128" s="16" t="s">
+      <c r="B128" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D128" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E128" s="16" t="s">
+      <c r="E128" s="15" t="s">
         <v>132</v>
       </c>
       <c r="F128" s="7" t="n">
@@ -4848,19 +4845,19 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="16" t="n">
+      <c r="A129" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B129" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C129" s="16" t="s">
+      <c r="B129" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C129" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E129" s="16" t="s">
+      <c r="E129" s="15" t="s">
         <v>133</v>
       </c>
       <c r="F129" s="7" t="n">
@@ -4882,19 +4879,19 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="16" t="n">
+      <c r="A130" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B130" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C130" s="16" t="s">
+      <c r="B130" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D130" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E130" s="16" t="s">
+      <c r="E130" s="15" t="s">
         <v>134</v>
       </c>
       <c r="F130" s="7" t="n">
@@ -4915,19 +4912,19 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="16" t="n">
+      <c r="A131" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B131" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C131" s="16" t="s">
+      <c r="B131" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C131" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E131" s="16" t="s">
+      <c r="E131" s="15" t="s">
         <v>135</v>
       </c>
       <c r="F131" s="7" t="n">
@@ -4949,19 +4946,19 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="16" t="n">
+      <c r="A132" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B132" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C132" s="16" t="s">
+      <c r="B132" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C132" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D132" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E132" s="16" t="s">
+      <c r="E132" s="15" t="s">
         <v>136</v>
       </c>
       <c r="F132" s="7" t="n">
@@ -4983,19 +4980,19 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="16" t="n">
+      <c r="A133" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B133" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C133" s="16" t="s">
+      <c r="B133" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E133" s="16" t="s">
+      <c r="E133" s="15" t="s">
         <v>137</v>
       </c>
       <c r="F133" s="7" t="n">
@@ -5017,19 +5014,19 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="16" t="n">
+      <c r="A134" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B134" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C134" s="16" t="s">
+      <c r="B134" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C134" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D134" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E134" s="16" t="s">
+      <c r="E134" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F134" s="7" t="n">
@@ -5051,19 +5048,19 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="16" t="n">
+      <c r="A135" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B135" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C135" s="16" t="s">
+      <c r="B135" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C135" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D135" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E135" s="16" t="s">
+      <c r="E135" s="15" t="s">
         <v>138</v>
       </c>
       <c r="F135" s="7" t="n">
@@ -5085,19 +5082,19 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="16" t="n">
+      <c r="A136" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B136" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C136" s="16" t="s">
+      <c r="B136" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C136" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D136" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E136" s="16" t="s">
+      <c r="E136" s="15" t="s">
         <v>139</v>
       </c>
       <c r="F136" s="7" t="n">
@@ -5116,7 +5113,7 @@
       <c r="K136" s="13" t="n">
         <v>0.59375</v>
       </c>
-      <c r="L136" s="15" t="n">
+      <c r="L136" s="14" t="n">
         <f aca="false">SUM(H126:I136)</f>
         <v>12.75</v>
       </c>
@@ -5133,19 +5130,19 @@
       <c r="K137" s="13"/>
     </row>
     <row r="138" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="16" t="n">
+      <c r="A138" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B138" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C138" s="16" t="s">
+      <c r="B138" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C138" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D138" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E138" s="16" t="s">
+      <c r="E138" s="15" t="s">
         <v>140</v>
       </c>
       <c r="F138" s="7" t="n">
@@ -5166,28 +5163,28 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="16" t="n">
+      <c r="A139" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B139" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C139" s="16" t="s">
+      <c r="B139" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C139" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E139" s="16" t="s">
+      <c r="E139" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="F139" s="17" t="n">
+      <c r="F139" s="16" t="n">
         <v>44464</v>
       </c>
-      <c r="G139" s="17" t="n">
+      <c r="G139" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H139" s="16"/>
+      <c r="H139" s="15"/>
       <c r="I139" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K139-J139)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
@@ -5196,33 +5193,33 @@
         <f aca="false">K138</f>
         <v>0.510416666666667</v>
       </c>
-      <c r="K139" s="18" t="n">
+      <c r="K139" s="17" t="n">
         <v>0.53125</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="16" t="n">
+      <c r="A140" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B140" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C140" s="16" t="s">
+      <c r="B140" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D140" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E140" s="16" t="s">
+      <c r="E140" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="F140" s="17" t="n">
+      <c r="F140" s="16" t="n">
         <v>44464</v>
       </c>
-      <c r="G140" s="17" t="n">
+      <c r="G140" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H140" s="16"/>
+      <c r="H140" s="15"/>
       <c r="I140" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K140-J140)*24*60/60)/0.25),0)*0.25</f>
         <v>0.5</v>
@@ -5231,33 +5228,33 @@
         <f aca="false">K139</f>
         <v>0.53125</v>
       </c>
-      <c r="K140" s="18" t="n">
+      <c r="K140" s="17" t="n">
         <v>0.552083333333333</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="16" t="n">
+      <c r="A141" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B141" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C141" s="16" t="s">
+      <c r="B141" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C141" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D141" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E141" s="16" t="s">
+      <c r="E141" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="F141" s="17" t="n">
+      <c r="F141" s="16" t="n">
         <v>44464</v>
       </c>
-      <c r="G141" s="17" t="n">
+      <c r="G141" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H141" s="16"/>
+      <c r="H141" s="15"/>
       <c r="I141" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K141-J141)*24*60/60)/0.25),0)*0.25</f>
         <v>0.25</v>
@@ -5266,44 +5263,44 @@
         <f aca="false">K140</f>
         <v>0.552083333333333</v>
       </c>
-      <c r="K141" s="18" t="n">
+      <c r="K141" s="17" t="n">
         <v>0.5625</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="16" t="n">
+      <c r="A142" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B142" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C142" s="16" t="s">
+      <c r="B142" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C142" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D142" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E142" s="16" t="s">
+      <c r="E142" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="F142" s="17" t="n">
+      <c r="F142" s="16" t="n">
         <v>44464</v>
       </c>
-      <c r="G142" s="17" t="n">
+      <c r="G142" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H142" s="16"/>
+      <c r="H142" s="15"/>
       <c r="I142" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K142-J142)*24*60/60)/0.25),0)*0.25</f>
         <v>1.5</v>
       </c>
-      <c r="J142" s="18" t="n">
+      <c r="J142" s="17" t="n">
         <v>0.552083333333333</v>
       </c>
-      <c r="K142" s="18" t="n">
+      <c r="K142" s="17" t="n">
         <v>0.614583333333333</v>
       </c>
-      <c r="L142" s="15" t="n">
+      <c r="L142" s="14" t="n">
         <f aca="false">SUM(H138:I142)</f>
         <v>4</v>
       </c>
@@ -5318,19 +5315,19 @@
       <c r="G143" s="7"/>
     </row>
     <row r="144" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="16" t="n">
+      <c r="A144" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B144" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C144" s="16" t="s">
+      <c r="B144" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C144" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D144" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E144" s="16" t="s">
+      <c r="E144" s="15" t="s">
         <v>145</v>
       </c>
       <c r="F144" s="7" t="n">
@@ -5351,19 +5348,19 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="16" t="n">
+      <c r="A145" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B145" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C145" s="16" t="s">
+      <c r="B145" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C145" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D145" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E145" s="16" t="s">
+      <c r="E145" s="15" t="s">
         <v>146</v>
       </c>
       <c r="F145" s="7" t="n">
@@ -5382,7 +5379,7 @@
       <c r="K145" s="13" t="n">
         <v>0.697916666666667</v>
       </c>
-      <c r="L145" s="15" t="n">
+      <c r="L145" s="14" t="n">
         <f aca="false">SUM(H144:I145)</f>
         <v>6.25</v>
       </c>
@@ -5397,19 +5394,19 @@
       <c r="G146" s="7"/>
     </row>
     <row r="147" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="16" t="n">
+      <c r="A147" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B147" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C147" s="16" t="s">
+      <c r="B147" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C147" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D147" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E147" s="16" t="s">
+      <c r="E147" s="15" t="s">
         <v>147</v>
       </c>
       <c r="F147" s="7" t="n">
@@ -5430,19 +5427,19 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="16" t="n">
+      <c r="A148" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B148" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C148" s="16" t="s">
+      <c r="B148" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C148" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D148" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E148" s="16" t="s">
+      <c r="E148" s="15" t="s">
         <v>148</v>
       </c>
       <c r="F148" s="7" t="n">
@@ -5463,19 +5460,19 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="16" t="n">
+      <c r="A149" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B149" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C149" s="16" t="s">
+      <c r="B149" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C149" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E149" s="16" t="s">
+      <c r="E149" s="15" t="s">
         <v>149</v>
       </c>
       <c r="F149" s="7" t="n">
@@ -5496,19 +5493,19 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="16" t="n">
+      <c r="A150" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B150" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C150" s="16" t="s">
+      <c r="B150" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C150" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D150" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E150" s="16" t="s">
+      <c r="E150" s="15" t="s">
         <v>150</v>
       </c>
       <c r="F150" s="7" t="n">
@@ -5527,7 +5524,7 @@
       <c r="K150" s="13" t="n">
         <v>0.604166666666667</v>
       </c>
-      <c r="L150" s="15" t="n">
+      <c r="L150" s="14" t="n">
         <f aca="false">SUM(H147:I150)</f>
         <v>13.25</v>
       </c>
@@ -5542,19 +5539,19 @@
       <c r="G151" s="7"/>
     </row>
     <row r="152" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="16" t="n">
+      <c r="A152" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B152" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C152" s="16" t="s">
+      <c r="B152" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C152" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D152" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E152" s="16" t="s">
+      <c r="E152" s="15" t="s">
         <v>151</v>
       </c>
       <c r="F152" s="7" t="n">
@@ -5575,19 +5572,19 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="16" t="n">
+      <c r="A153" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B153" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C153" s="16" t="s">
+      <c r="B153" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C153" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E153" s="16" t="s">
+      <c r="E153" s="15" t="s">
         <v>152</v>
       </c>
       <c r="F153" s="7" t="n">
@@ -5606,7 +5603,7 @@
       <c r="K153" s="13" t="n">
         <v>0.645833333333333</v>
       </c>
-      <c r="L153" s="15" t="n">
+      <c r="L153" s="14" t="n">
         <f aca="false">SUM(H152:I153)</f>
         <v>7</v>
       </c>
@@ -5621,62 +5618,62 @@
       <c r="G154" s="7"/>
     </row>
     <row r="155" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="16" t="n">
+      <c r="A155" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B155" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C155" s="16" t="s">
+      <c r="B155" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C155" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E155" s="16" t="s">
+      <c r="E155" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="F155" s="17" t="n">
+      <c r="F155" s="16" t="n">
         <v>44501</v>
       </c>
-      <c r="G155" s="17" t="n">
+      <c r="G155" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H155" s="16"/>
+      <c r="H155" s="15"/>
       <c r="I155" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K155-J155)*24*60/60)/0.25),0)*0.25</f>
         <v>3.5</v>
       </c>
-      <c r="J155" s="18" t="n">
+      <c r="J155" s="17" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="K155" s="18" t="n">
+      <c r="K155" s="17" t="n">
         <v>0.604166666666667</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="16" t="n">
+      <c r="A156" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B156" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C156" s="16" t="s">
+      <c r="B156" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C156" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D156" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E156" s="16" t="s">
+      <c r="E156" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="F156" s="17" t="n">
+      <c r="F156" s="16" t="n">
         <v>44501</v>
       </c>
-      <c r="G156" s="17" t="n">
+      <c r="G156" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H156" s="16"/>
+      <c r="H156" s="15"/>
       <c r="I156" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K156-J156)*24*60/60)/0.25),0)*0.25</f>
         <v>2.25</v>
@@ -5685,10 +5682,10 @@
         <f aca="false">K155</f>
         <v>0.604166666666667</v>
       </c>
-      <c r="K156" s="18" t="n">
+      <c r="K156" s="17" t="n">
         <v>0.697916666666667</v>
       </c>
-      <c r="L156" s="15" t="n">
+      <c r="L156" s="14" t="n">
         <f aca="false">SUM(H155:I156)</f>
         <v>5.75</v>
       </c>
@@ -5698,41 +5695,41 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="16"/>
-      <c r="B157" s="16"/>
-      <c r="C157" s="16"/>
+      <c r="A157" s="15"/>
+      <c r="B157" s="15"/>
+      <c r="C157" s="15"/>
       <c r="D157" s="6"/>
-      <c r="E157" s="16"/>
-      <c r="F157" s="17"/>
-      <c r="G157" s="17"/>
-      <c r="H157" s="16"/>
+      <c r="E157" s="15"/>
+      <c r="F157" s="16"/>
+      <c r="G157" s="16"/>
+      <c r="H157" s="15"/>
       <c r="I157" s="12"/>
       <c r="J157" s="13"/>
-      <c r="K157" s="18"/>
+      <c r="K157" s="17"/>
     </row>
     <row r="158" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="16" t="n">
+      <c r="A158" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B158" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C158" s="16" t="s">
+      <c r="B158" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C158" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D158" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E158" s="16" t="s">
+      <c r="E158" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="F158" s="17" t="n">
+      <c r="F158" s="16" t="n">
         <v>44508</v>
       </c>
-      <c r="G158" s="17" t="n">
+      <c r="G158" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H158" s="16"/>
+      <c r="H158" s="15"/>
       <c r="I158" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K158-J158)*24*60/60)/0.25),0)*0.25</f>
         <v>3</v>
@@ -5740,33 +5737,33 @@
       <c r="J158" s="13" t="n">
         <v>0.458333333333333</v>
       </c>
-      <c r="K158" s="18" t="n">
+      <c r="K158" s="17" t="n">
         <v>0.583333333333333</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="16" t="n">
+      <c r="A159" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B159" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C159" s="16" t="s">
+      <c r="B159" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C159" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E159" s="16" t="s">
+      <c r="E159" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="F159" s="17" t="n">
+      <c r="F159" s="16" t="n">
         <v>44509</v>
       </c>
-      <c r="G159" s="17" t="n">
+      <c r="G159" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H159" s="16"/>
+      <c r="H159" s="15"/>
       <c r="I159" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K159-J159)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
@@ -5774,10 +5771,10 @@
       <c r="J159" s="13" t="n">
         <v>0.5</v>
       </c>
-      <c r="K159" s="18" t="n">
+      <c r="K159" s="17" t="n">
         <v>0.666666666666667</v>
       </c>
-      <c r="L159" s="15" t="n">
+      <c r="L159" s="14" t="n">
         <f aca="false">SUM(H158:I159)</f>
         <v>7</v>
       </c>
@@ -5792,28 +5789,28 @@
       <c r="G160" s="7"/>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="16" t="n">
+      <c r="A161" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B161" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="C161" s="16" t="s">
+      <c r="B161" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C161" s="15" t="s">
         <v>114</v>
       </c>
       <c r="D161" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E161" s="16" t="s">
+      <c r="E161" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="F161" s="17" t="n">
+      <c r="F161" s="16" t="n">
         <v>44513</v>
       </c>
-      <c r="G161" s="17" t="n">
+      <c r="G161" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H161" s="16"/>
+      <c r="H161" s="15"/>
       <c r="I161" s="12" t="n">
         <f aca="false">ROUNDUP(((SUM(K161-J161)*24*60/60)/0.25),0)*0.25</f>
         <v>4</v>
@@ -5821,82 +5818,145 @@
       <c r="J161" s="13" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="K161" s="18" t="n">
+      <c r="K161" s="17" t="n">
         <v>0.708333333333333</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D162" s="6"/>
-      <c r="F162" s="7"/>
-      <c r="G162" s="7"/>
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B162" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C162" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D162" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E162" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F162" s="16" t="n">
+        <v>44514</v>
+      </c>
+      <c r="G162" s="16" t="n">
+        <v>44481</v>
+      </c>
+      <c r="H162" s="15"/>
+      <c r="I162" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K162-J162)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J162" s="13" t="n">
+        <v>0.708333333333333</v>
+      </c>
+      <c r="K162" s="17" t="n">
+        <v>0.791666666666667</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="6"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="7"/>
-    </row>
-    <row r="164" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="2" t="s">
+      <c r="A163" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B163" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C163" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D163" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E163" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C164" s="19" t="n">
+      <c r="F163" s="16" t="n">
+        <v>44515</v>
+      </c>
+      <c r="G163" s="16" t="n">
+        <v>44481</v>
+      </c>
+      <c r="H163" s="15"/>
+      <c r="I163" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K163-J163)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J163" s="13" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="K163" s="17" t="n">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D164" s="6"/>
+      <c r="F164" s="7"/>
+      <c r="G164" s="7"/>
+    </row>
+    <row r="165" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B165" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C165" s="18" t="n">
         <f aca="false">SUM(I:I)+SUM(H:H)</f>
-        <v>349</v>
-      </c>
-      <c r="D164" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D165" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E164" s="19" t="n">
+      <c r="E165" s="18" t="n">
         <f aca="false">SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F164" s="3" t="s">
+      <c r="F165" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G164" s="19" t="n">
+      <c r="G165" s="18" t="n">
         <f aca="false">SUM(I:I)</f>
-        <v>294</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D165" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="E165" s="20" t="n">
-        <f aca="false">135-E164</f>
+        <v>298</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D166" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E166" s="19" t="n">
+        <f aca="false">135-E165</f>
         <v>80</v>
       </c>
-      <c r="F165" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="G165" s="20" t="n">
-        <f aca="false">315-G164</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="0" t="s">
+      <c r="F166" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="C166" s="0" t="n">
-        <f aca="false">ROUNDUP(C164/30, 0)</f>
+      <c r="G166" s="19" t="n">
+        <f aca="false">315-G165</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <f aca="false">ROUNDUP(C165/30, 0)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="21"/>
-      <c r="B167" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C167" s="21" t="n">
+    <row r="168" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="20"/>
+      <c r="B168" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C168" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="D167" s="21"/>
-      <c r="E167" s="21"/>
-      <c r="F167" s="21"/>
-      <c r="G167" s="21"/>
-      <c r="H167" s="21"/>
-      <c r="I167" s="21"/>
+      <c r="D168" s="20"/>
+      <c r="E168" s="20"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="20"/>
+      <c r="H168" s="20"/>
+      <c r="I168" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5904,7 +5964,7 @@
       <formula1>$N$3:$N$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D162:D163" type="list">
+    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D164" type="list">
       <formula1>$N$3:$N$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5930,55 +5990,55 @@
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+      <c r="A5" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="B5" s="23" t="n">
+      <c r="B5" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C5" s="23" t="n">
+      <c r="C5" s="22" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="23" t="n">
+      <c r="D5" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E5" s="24" t="n">
+      <c r="E5" s="23" t="n">
         <f aca="false">(B5*3)+C5+D5</f>
         <v>36</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">SUM(E5:E7)</f>
         <v>107</v>
       </c>
-      <c r="H5" s="25" t="n">
+      <c r="H5" s="24" t="n">
         <v>44298</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="n">
+      <c r="A6" s="25" t="n">
         <v>16</v>
       </c>
       <c r="B6" s="10" t="n">
@@ -5990,57 +6050,57 @@
       <c r="D6" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="26" t="n">
         <f aca="false">(B6*3)+C6+D6</f>
         <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="n">
+      <c r="A7" s="27" t="n">
         <v>17</v>
       </c>
-      <c r="B7" s="21" t="n">
+      <c r="B7" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="C7" s="21" t="n">
+      <c r="C7" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="E7" s="29" t="n">
+      <c r="E7" s="28" t="n">
         <f aca="false">(B7*3)+C7+D7</f>
         <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
+      <c r="A8" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="B8" s="23" t="n">
+      <c r="B8" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23" t="n">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="24" t="n">
+      <c r="E8" s="23" t="n">
         <f aca="false">(B8*3)+C8+D8</f>
         <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">SUM(E8:E10)</f>
         <v>102</v>
       </c>
-      <c r="H8" s="25" t="n">
+      <c r="H8" s="24" t="n">
         <v>44319</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26" t="n">
+      <c r="A9" s="25" t="n">
         <v>19</v>
       </c>
       <c r="B9" s="10" t="n">
@@ -6052,57 +6112,57 @@
       <c r="D9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="26" t="n">
         <f aca="false">(B9*3)+C9+D9</f>
         <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="n">
+      <c r="A10" s="27" t="n">
         <v>20</v>
       </c>
-      <c r="B10" s="21" t="n">
+      <c r="B10" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="21" t="n">
+      <c r="C10" s="20" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="21" t="n">
+      <c r="D10" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="29" t="n">
+      <c r="E10" s="28" t="n">
         <f aca="false">(B10*3)+C10+D10</f>
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
+      <c r="A11" s="21" t="n">
         <v>21</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23" t="n">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E11" s="24" t="n">
+      <c r="E11" s="23" t="n">
         <f aca="false">(B11*3)+C11+D11</f>
         <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">SUM(E11:E13)</f>
         <v>101</v>
       </c>
-      <c r="H11" s="25" t="n">
+      <c r="H11" s="24" t="n">
         <v>44340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="n">
+      <c r="A12" s="25" t="n">
         <v>22</v>
       </c>
       <c r="B12" s="10" t="n">
@@ -6112,13 +6172,13 @@
       <c r="D12" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="27" t="n">
+      <c r="E12" s="26" t="n">
         <f aca="false">(B12*3)+C12+D12</f>
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="n">
+      <c r="A13" s="25" t="n">
         <v>23</v>
       </c>
       <c r="B13" s="10" t="n">
@@ -6130,95 +6190,95 @@
       <c r="D13" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E13" s="27" t="n">
+      <c r="E13" s="26" t="n">
         <f aca="false">(B13*3)+C13+D13</f>
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="n">
+      <c r="A14" s="21" t="n">
         <v>24</v>
       </c>
-      <c r="B14" s="23" t="n">
+      <c r="B14" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="23" t="n">
+      <c r="C14" s="22" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="23" t="n">
+      <c r="D14" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="24" t="n">
+      <c r="E14" s="23" t="n">
         <f aca="false">(B14*3)+C14+D14</f>
         <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">SUM(E14:E15)</f>
         <v>74</v>
       </c>
-      <c r="H14" s="25" t="n">
+      <c r="H14" s="24" t="n">
         <v>44361</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28" t="n">
+      <c r="A15" s="27" t="n">
         <v>25</v>
       </c>
-      <c r="B15" s="21" t="n">
+      <c r="B15" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="21" t="n">
+      <c r="C15" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="21" t="n">
+      <c r="D15" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="29" t="n">
+      <c r="E15" s="28" t="n">
         <f aca="false">(B15*3)+C15+D15</f>
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="n">
+      <c r="A16" s="21" t="n">
         <v>26</v>
       </c>
-      <c r="B16" s="23" t="n">
+      <c r="B16" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23" t="n">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="24" t="n">
+      <c r="E16" s="23" t="n">
         <f aca="false">(B16*3)+C16+D16</f>
         <v>32</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">SUM(E16:E17)</f>
         <v>64</v>
       </c>
-      <c r="H16" s="25" t="n">
+      <c r="H16" s="24" t="n">
         <v>44375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="n">
+      <c r="A17" s="27" t="n">
         <v>27</v>
       </c>
-      <c r="B17" s="21" t="n">
+      <c r="B17" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21" t="n">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20" t="n">
         <v>8</v>
       </c>
-      <c r="E17" s="29" t="n">
+      <c r="E17" s="28" t="n">
         <f aca="false">(B17*3)+C17+D17</f>
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
[FEATURE] Add tutorial screens for tablet
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="174">
   <si>
     <t xml:space="preserve">Issue Nr</t>
   </si>
@@ -498,6 +498,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tablet neues Rezept anlegen screens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tablet Einfuehrung in die App</t>
   </si>
   <si>
     <t xml:space="preserve">Stunden insgesamt</t>
@@ -898,13 +901,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P168"/>
+  <dimension ref="A1:P170"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G164" activeCellId="0" sqref="G164"/>
+      <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.84"/>
@@ -5855,108 +5858,163 @@
       <c r="K162" s="17" t="n">
         <v>0.791666666666667</v>
       </c>
+      <c r="L162" s="14" t="n">
+        <f aca="false">SUM(H161:I162)</f>
+        <v>6</v>
+      </c>
+      <c r="M162" s="0" t="n">
+        <f aca="false">SUM(L162+16)</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="15" t="n">
+      <c r="A163" s="15"/>
+      <c r="B163" s="15"/>
+      <c r="C163" s="15"/>
+      <c r="D163" s="6"/>
+      <c r="E163" s="15"/>
+      <c r="F163" s="16"/>
+      <c r="G163" s="16"/>
+      <c r="H163" s="15"/>
+      <c r="I163" s="12"/>
+      <c r="J163" s="13"/>
+      <c r="K163" s="17"/>
+    </row>
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B163" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C163" s="15" t="s">
+      <c r="B164" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C164" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D163" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E163" s="15" t="s">
+      <c r="D164" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E164" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F163" s="16" t="n">
+      <c r="F164" s="16" t="n">
         <v>44515</v>
       </c>
-      <c r="G163" s="16" t="n">
+      <c r="G164" s="16" t="n">
         <v>44481</v>
       </c>
-      <c r="H163" s="15"/>
-      <c r="I163" s="12" t="n">
-        <f aca="false">ROUNDUP(((SUM(K163-J163)*24*60/60)/0.25),0)*0.25</f>
+      <c r="H164" s="15"/>
+      <c r="I164" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K164-J164)*24*60/60)/0.25),0)*0.25</f>
         <v>2</v>
       </c>
-      <c r="J163" s="13" t="n">
+      <c r="J164" s="13" t="n">
         <v>0.541666666666667</v>
       </c>
-      <c r="K163" s="17" t="n">
+      <c r="K164" s="17" t="n">
         <v>0.625</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D164" s="6"/>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-    </row>
-    <row r="165" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="2" t="s">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B165" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C165" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D165" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E165" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C165" s="18" t="n">
+      <c r="F165" s="16" t="n">
+        <v>44515</v>
+      </c>
+      <c r="G165" s="16" t="n">
+        <v>44481</v>
+      </c>
+      <c r="H165" s="15"/>
+      <c r="I165" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K165-J165)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J165" s="13" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="K165" s="17" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D166" s="6"/>
+      <c r="F166" s="7"/>
+      <c r="G166" s="7"/>
+    </row>
+    <row r="167" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B167" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C167" s="18" t="n">
         <f aca="false">SUM(I:I)+SUM(H:H)</f>
-        <v>353</v>
-      </c>
-      <c r="D165" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D167" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E165" s="18" t="n">
+      <c r="E167" s="18" t="n">
         <f aca="false">SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F165" s="3" t="s">
+      <c r="F167" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G165" s="18" t="n">
+      <c r="G167" s="18" t="n">
         <f aca="false">SUM(I:I)</f>
-        <v>298</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D166" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="E166" s="19" t="n">
-        <f aca="false">135-E165</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D168" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E168" s="19" t="n">
+        <f aca="false">135-E167</f>
         <v>80</v>
       </c>
-      <c r="F166" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="G166" s="19" t="n">
-        <f aca="false">315-G165</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="0" t="s">
+      <c r="F168" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C167" s="0" t="n">
-        <f aca="false">ROUNDUP(C165/30, 0)</f>
+      <c r="G168" s="19" t="n">
+        <f aca="false">315-G167</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <f aca="false">ROUNDUP(C167/30, 0)</f>
         <v>12</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="20"/>
-      <c r="B168" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C168" s="20" t="n">
+    <row r="170" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="20"/>
+      <c r="B170" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C170" s="20" t="n">
         <v>15</v>
       </c>
-      <c r="D168" s="20"/>
-      <c r="E168" s="20"/>
-      <c r="F168" s="20"/>
-      <c r="G168" s="20"/>
-      <c r="H168" s="20"/>
-      <c r="I168" s="20"/>
+      <c r="D170" s="20"/>
+      <c r="E170" s="20"/>
+      <c r="F170" s="20"/>
+      <c r="G170" s="20"/>
+      <c r="H170" s="20"/>
+      <c r="I170" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5964,7 +6022,7 @@
       <formula1>$N$3:$N$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D164" type="list">
+    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D166" type="list">
       <formula1>$N$3:$N$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5990,23 +6048,23 @@
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6027,7 +6085,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">SUM(E5:E7)</f>
@@ -6089,7 +6147,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">SUM(E8:E10)</f>
@@ -6151,7 +6209,7 @@
         <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">SUM(E11:E13)</f>
@@ -6213,7 +6271,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">SUM(E14:E15)</f>
@@ -6257,7 +6315,7 @@
         <v>32</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">SUM(E16:E17)</f>

</xml_diff>

<commit_message>
[FEATURE] Add desktop screens and fix tablet new recipe
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="175">
   <si>
     <t xml:space="preserve">Issue Nr</t>
   </si>
@@ -501,6 +501,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tablet Einfuehrung in die App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desktop von Tablet geerbt und abgeändert</t>
   </si>
   <si>
     <t xml:space="preserve">Stunden insgesamt</t>
@@ -901,13 +904,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P170"/>
+  <dimension ref="A1:P172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A142" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I170" activeCellId="0" sqref="I170"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.84"/>
@@ -5953,68 +5956,107 @@
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
     </row>
-    <row r="167" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="2" t="s">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B167" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C167" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E167" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C167" s="18" t="n">
+      <c r="F167" s="16" t="n">
+        <v>44526</v>
+      </c>
+      <c r="G167" s="16" t="n">
+        <v>44481</v>
+      </c>
+      <c r="H167" s="15"/>
+      <c r="I167" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K167-J167)*24*60/60)/0.25),0)*0.25</f>
+        <v>5</v>
+      </c>
+      <c r="J167" s="13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K167" s="17" t="n">
+        <v>0.708333333333333</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D168" s="6"/>
+      <c r="F168" s="7"/>
+      <c r="G168" s="7"/>
+    </row>
+    <row r="169" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B169" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C169" s="18" t="n">
         <f aca="false">SUM(I:I)+SUM(H:H)</f>
-        <v>355</v>
-      </c>
-      <c r="D167" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="D169" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E167" s="18" t="n">
+      <c r="E169" s="18" t="n">
         <f aca="false">SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F167" s="3" t="s">
+      <c r="F169" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G167" s="18" t="n">
+      <c r="G169" s="18" t="n">
         <f aca="false">SUM(I:I)</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="E168" s="19" t="n">
-        <f aca="false">135-E167</f>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D170" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E170" s="19" t="n">
+        <f aca="false">135-E169</f>
         <v>80</v>
       </c>
-      <c r="F168" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G168" s="19" t="n">
-        <f aca="false">315-G167</f>
+      <c r="F170" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="G170" s="19" t="n">
+        <f aca="false">315-G169</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B171" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <f aca="false">ROUNDUP(C169/30, 0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="20"/>
+      <c r="B172" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C172" s="20" t="n">
         <v>15</v>
       </c>
-    </row>
-    <row r="169" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="C169" s="0" t="n">
-        <f aca="false">ROUNDUP(C167/30, 0)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="20"/>
-      <c r="B170" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C170" s="20" t="n">
-        <v>15</v>
-      </c>
-      <c r="D170" s="20"/>
-      <c r="E170" s="20"/>
-      <c r="F170" s="20"/>
-      <c r="G170" s="20"/>
-      <c r="H170" s="20"/>
-      <c r="I170" s="20"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="20"/>
+      <c r="F172" s="20"/>
+      <c r="G172" s="20"/>
+      <c r="H172" s="20"/>
+      <c r="I172" s="20"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6022,7 +6064,7 @@
       <formula1>$N$3:$N$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D166" type="list">
+    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D166 D168" type="list">
       <formula1>$N$3:$N$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6048,23 +6090,23 @@
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6085,7 +6127,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">SUM(E5:E7)</f>
@@ -6147,7 +6189,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">SUM(E8:E10)</f>
@@ -6209,7 +6251,7 @@
         <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">SUM(E11:E13)</f>
@@ -6271,7 +6313,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">SUM(E14:E15)</f>
@@ -6315,7 +6357,7 @@
         <v>32</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">SUM(E16:E17)</f>

</xml_diff>

<commit_message>
[FEATURE] Enhance figma prototype by refining design and clickable actions
</commit_message>
<xml_diff>
--- a/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
+++ b/Artefakte/Zeiterfassung/Arbeitsmatrix.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="179">
   <si>
     <t xml:space="preserve">Issue Nr</t>
   </si>
@@ -504,6 +504,18 @@
   </si>
   <si>
     <t xml:space="preserve">Desktop von Tablet geerbt und abgeändert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokumentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facharbeit verfassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inhaltsverzeichnis und LatexVorlage erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Designs refinen und Prototypen erweitern</t>
   </si>
   <si>
     <t xml:space="preserve">Stunden insgesamt</t>
@@ -552,13 +564,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="General"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="hh:mm"/>
-    <numFmt numFmtId="169" formatCode="dd/\ mmm"/>
+    <numFmt numFmtId="169" formatCode="hh:mm:ss"/>
+    <numFmt numFmtId="170" formatCode="dd/\ mmm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -710,7 +723,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -783,6 +796,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -807,7 +824,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -904,13 +921,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P172"/>
+  <dimension ref="A1:P175"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G148" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J161" activeCellId="0" sqref="J161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.84"/>
@@ -5991,72 +6008,144 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="6"/>
-      <c r="F168" s="7"/>
-      <c r="G168" s="7"/>
-    </row>
-    <row r="169" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="2" t="s">
+      <c r="A168" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B168" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="C169" s="18" t="n">
+      <c r="C168" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F168" s="7" t="n">
+        <v>44528</v>
+      </c>
+      <c r="G168" s="7" t="n">
+        <v>44554</v>
+      </c>
+      <c r="I168" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K168-J168)*24*60/60)/0.25),0)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="J168" s="18" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="K168" s="18" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D169" s="6"/>
+      <c r="F169" s="7"/>
+      <c r="G169" s="7"/>
+    </row>
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="15" t="n">
+        <v>22</v>
+      </c>
+      <c r="B170" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C170" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E170" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F170" s="16" t="n">
+        <v>44529</v>
+      </c>
+      <c r="G170" s="16" t="n">
+        <v>44481</v>
+      </c>
+      <c r="H170" s="15"/>
+      <c r="I170" s="12" t="n">
+        <f aca="false">ROUNDUP(((SUM(K170-J170)*24*60/60)/0.25),0)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="J170" s="13" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="K170" s="17" t="n">
+        <v>0.583333333333333</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D171" s="6"/>
+      <c r="F171" s="7"/>
+      <c r="G171" s="7"/>
+    </row>
+    <row r="172" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B172" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C172" s="19" t="n">
         <f aca="false">SUM(I:I)+SUM(H:H)</f>
-        <v>360</v>
-      </c>
-      <c r="D169" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D172" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E169" s="18" t="n">
+      <c r="E172" s="19" t="n">
         <f aca="false">SUM(H:H)</f>
         <v>55</v>
       </c>
-      <c r="F169" s="3" t="s">
+      <c r="F172" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G169" s="18" t="n">
+      <c r="G172" s="19" t="n">
         <f aca="false">SUM(I:I)</f>
-        <v>305</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D170" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="E170" s="19" t="n">
-        <f aca="false">135-E169</f>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D173" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E173" s="20" t="n">
+        <f aca="false">135-E172</f>
         <v>80</v>
       </c>
-      <c r="F170" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="G170" s="19" t="n">
-        <f aca="false">315-G169</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="C171" s="0" t="n">
-        <f aca="false">ROUNDUP(C169/30, 0)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="20"/>
-      <c r="B172" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C172" s="20" t="n">
+      <c r="F173" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G173" s="20" t="n">
+        <f aca="false">315-G172</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B174" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <f aca="false">ROUNDUP(C172/30, 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="21"/>
+      <c r="B175" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C175" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="D172" s="20"/>
-      <c r="E172" s="20"/>
-      <c r="F172" s="20"/>
-      <c r="G172" s="20"/>
-      <c r="H172" s="20"/>
-      <c r="I172" s="20"/>
+      <c r="D175" s="21"/>
+      <c r="E175" s="21"/>
+      <c r="F175" s="21"/>
+      <c r="G175" s="21"/>
+      <c r="H175" s="21"/>
+      <c r="I175" s="21"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -6064,7 +6153,7 @@
       <formula1>$N$3:$N$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D166 D168" type="list">
+    <dataValidation allowBlank="true" error="Es konnte kein korrekter Prefix ausgegeben werden&#10;" errorStyle="stop" errorTitle="Prefix nicht unterstützt" operator="between" prompt="Wählen Sie einen Prefix aus" promptTitle="Prefix" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D3 D13:D17 D22:D27 D35:D36 D41:D113 D115:D141 D143:D154 D160 D166 D168:D169 D171" type="list">
       <formula1>$N$3:$N$6</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -6090,55 +6179,55 @@
       <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="n">
+      <c r="A5" s="22" t="n">
         <v>15</v>
       </c>
-      <c r="B5" s="22" t="n">
+      <c r="B5" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="C5" s="22" t="n">
+      <c r="C5" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="22" t="n">
+      <c r="D5" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E5" s="23" t="n">
+      <c r="E5" s="24" t="n">
         <f aca="false">(B5*3)+C5+D5</f>
         <v>36</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">SUM(E5:E7)</f>
         <v>107</v>
       </c>
-      <c r="H5" s="24" t="n">
+      <c r="H5" s="25" t="n">
         <v>44298</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="n">
+      <c r="A6" s="26" t="n">
         <v>16</v>
       </c>
       <c r="B6" s="10" t="n">
@@ -6150,57 +6239,57 @@
       <c r="D6" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E6" s="26" t="n">
+      <c r="E6" s="27" t="n">
         <f aca="false">(B6*3)+C6+D6</f>
         <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="n">
+      <c r="A7" s="28" t="n">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="n">
+      <c r="B7" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C7" s="20" t="n">
+      <c r="C7" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="20" t="n">
+      <c r="D7" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="E7" s="28" t="n">
+      <c r="E7" s="29" t="n">
         <f aca="false">(B7*3)+C7+D7</f>
         <v>35</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="n">
+      <c r="A8" s="22" t="n">
         <v>18</v>
       </c>
-      <c r="B8" s="22" t="n">
+      <c r="B8" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22" t="n">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E8" s="23" t="n">
+      <c r="E8" s="24" t="n">
         <f aca="false">(B8*3)+C8+D8</f>
         <v>32</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">SUM(E8:E10)</f>
         <v>102</v>
       </c>
-      <c r="H8" s="24" t="n">
+      <c r="H8" s="25" t="n">
         <v>44319</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="n">
+      <c r="A9" s="26" t="n">
         <v>19</v>
       </c>
       <c r="B9" s="10" t="n">
@@ -6212,57 +6301,57 @@
       <c r="D9" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="26" t="n">
+      <c r="E9" s="27" t="n">
         <f aca="false">(B9*3)+C9+D9</f>
         <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="n">
+      <c r="A10" s="28" t="n">
         <v>20</v>
       </c>
-      <c r="B10" s="20" t="n">
+      <c r="B10" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="20" t="n">
+      <c r="C10" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="D10" s="20" t="n">
+      <c r="D10" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="E10" s="28" t="n">
+      <c r="E10" s="29" t="n">
         <f aca="false">(B10*3)+C10+D10</f>
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="21" t="n">
+      <c r="A11" s="22" t="n">
         <v>21</v>
       </c>
-      <c r="B11" s="22" t="n">
+      <c r="B11" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22" t="n">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E11" s="23" t="n">
+      <c r="E11" s="24" t="n">
         <f aca="false">(B11*3)+C11+D11</f>
         <v>32</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">SUM(E11:E13)</f>
         <v>101</v>
       </c>
-      <c r="H11" s="24" t="n">
+      <c r="H11" s="25" t="n">
         <v>44340</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="25" t="n">
+      <c r="A12" s="26" t="n">
         <v>22</v>
       </c>
       <c r="B12" s="10" t="n">
@@ -6272,13 +6361,13 @@
       <c r="D12" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="26" t="n">
+      <c r="E12" s="27" t="n">
         <f aca="false">(B12*3)+C12+D12</f>
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="25" t="n">
+      <c r="A13" s="26" t="n">
         <v>23</v>
       </c>
       <c r="B13" s="10" t="n">
@@ -6290,95 +6379,95 @@
       <c r="D13" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E13" s="26" t="n">
+      <c r="E13" s="27" t="n">
         <f aca="false">(B13*3)+C13+D13</f>
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="21" t="n">
+      <c r="A14" s="22" t="n">
         <v>24</v>
       </c>
-      <c r="B14" s="22" t="n">
+      <c r="B14" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="C14" s="22" t="n">
+      <c r="C14" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="22" t="n">
+      <c r="D14" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="23" t="n">
+      <c r="E14" s="24" t="n">
         <f aca="false">(B14*3)+C14+D14</f>
         <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">SUM(E14:E15)</f>
         <v>74</v>
       </c>
-      <c r="H14" s="24" t="n">
+      <c r="H14" s="25" t="n">
         <v>44361</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="n">
+      <c r="A15" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="B15" s="20" t="n">
+      <c r="B15" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C15" s="20" t="n">
+      <c r="C15" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="D15" s="20" t="n">
+      <c r="D15" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="28" t="n">
+      <c r="E15" s="29" t="n">
         <f aca="false">(B15*3)+C15+D15</f>
         <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="n">
+      <c r="A16" s="22" t="n">
         <v>26</v>
       </c>
-      <c r="B16" s="22" t="n">
+      <c r="B16" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22" t="n">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="23" t="n">
+      <c r="E16" s="24" t="n">
         <f aca="false">(B16*3)+C16+D16</f>
         <v>32</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">SUM(E16:E17)</f>
         <v>64</v>
       </c>
-      <c r="H16" s="24" t="n">
+      <c r="H16" s="25" t="n">
         <v>44375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="n">
+      <c r="A17" s="28" t="n">
         <v>27</v>
       </c>
-      <c r="B17" s="20" t="n">
+      <c r="B17" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20" t="n">
+      <c r="C17" s="21"/>
+      <c r="D17" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="E17" s="28" t="n">
+      <c r="E17" s="29" t="n">
         <f aca="false">(B17*3)+C17+D17</f>
         <v>32</v>
       </c>

</xml_diff>